<commit_message>
pareto exponent for extrapolation was incorrectly arounded.
</commit_message>
<xml_diff>
--- a/data_analyzed/moment.xlsx
+++ b/data_analyzed/moment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M815"/>
+  <dimension ref="A1:M910"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20156,10 +20156,18 @@
       <c r="I456" t="n">
         <v>6.340092180308363</v>
       </c>
-      <c r="J456" t="inlineStr"/>
-      <c r="K456" t="inlineStr"/>
-      <c r="L456" t="inlineStr"/>
-      <c r="M456" t="inlineStr"/>
+      <c r="J456" t="n">
+        <v>-0.4171720644817287</v>
+      </c>
+      <c r="K456" t="n">
+        <v>0.3357195371335476</v>
+      </c>
+      <c r="L456" t="n">
+        <v>0.2372264367509181</v>
+      </c>
+      <c r="M456" t="n">
+        <v>2.175867269640444</v>
+      </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
@@ -20969,10 +20977,18 @@
       <c r="I475" t="n">
         <v>7.538921199370701</v>
       </c>
-      <c r="J475" t="inlineStr"/>
-      <c r="K475" t="inlineStr"/>
-      <c r="L475" t="inlineStr"/>
-      <c r="M475" t="inlineStr"/>
+      <c r="J475" t="n">
+        <v>-0.475090227869142</v>
+      </c>
+      <c r="K475" t="n">
+        <v>0.3390417815583261</v>
+      </c>
+      <c r="L475" t="n">
+        <v>0.2941700511571806</v>
+      </c>
+      <c r="M475" t="n">
+        <v>2.206662329477553</v>
+      </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
@@ -21776,10 +21792,18 @@
       <c r="I494" t="n">
         <v>6.858465299510215</v>
       </c>
-      <c r="J494" t="inlineStr"/>
-      <c r="K494" t="inlineStr"/>
-      <c r="L494" t="inlineStr"/>
-      <c r="M494" t="inlineStr"/>
+      <c r="J494" t="n">
+        <v>-1.090592475347884</v>
+      </c>
+      <c r="K494" t="n">
+        <v>0.305552710783839</v>
+      </c>
+      <c r="L494" t="n">
+        <v>0.459843913720376</v>
+      </c>
+      <c r="M494" t="n">
+        <v>2.595473261476525</v>
+      </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
@@ -22583,10 +22607,18 @@
       <c r="I513" t="n">
         <v>8.056092228949829</v>
       </c>
-      <c r="J513" t="inlineStr"/>
-      <c r="K513" t="inlineStr"/>
-      <c r="L513" t="inlineStr"/>
-      <c r="M513" t="inlineStr"/>
+      <c r="J513" t="n">
+        <v>-0.9712759750021939</v>
+      </c>
+      <c r="K513" t="n">
+        <v>0.2859287179783679</v>
+      </c>
+      <c r="L513" t="n">
+        <v>0.5190875794184199</v>
+      </c>
+      <c r="M513" t="n">
+        <v>2.848823562284922</v>
+      </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
@@ -23390,10 +23422,18 @@
       <c r="I532" t="n">
         <v>6.28830101052083</v>
       </c>
-      <c r="J532" t="inlineStr"/>
-      <c r="K532" t="inlineStr"/>
-      <c r="L532" t="inlineStr"/>
-      <c r="M532" t="inlineStr"/>
+      <c r="J532" t="n">
+        <v>-1.417434297872755</v>
+      </c>
+      <c r="K532" t="n">
+        <v>0.2306493530254091</v>
+      </c>
+      <c r="L532" t="n">
+        <v>0.2501630079354575</v>
+      </c>
+      <c r="M532" t="n">
+        <v>2.346422858371362</v>
+      </c>
     </row>
     <row r="533">
       <c r="A533" t="inlineStr">
@@ -24150,10 +24190,18 @@
       <c r="I550" t="n">
         <v>6.236857686632747</v>
       </c>
-      <c r="J550" t="inlineStr"/>
-      <c r="K550" t="inlineStr"/>
-      <c r="L550" t="inlineStr"/>
-      <c r="M550" t="inlineStr"/>
+      <c r="J550" t="n">
+        <v>-0.9853713629864949</v>
+      </c>
+      <c r="K550" t="n">
+        <v>0.2062375548920074</v>
+      </c>
+      <c r="L550" t="n">
+        <v>0.2052426328312739</v>
+      </c>
+      <c r="M550" t="n">
+        <v>2.39656107586889</v>
+      </c>
     </row>
     <row r="551">
       <c r="A551" t="inlineStr">
@@ -24955,10 +25003,18 @@
       <c r="I569" t="n">
         <v>6.93498853200975</v>
       </c>
-      <c r="J569" t="inlineStr"/>
-      <c r="K569" t="inlineStr"/>
-      <c r="L569" t="inlineStr"/>
-      <c r="M569" t="inlineStr"/>
+      <c r="J569" t="n">
+        <v>-0.8738619947286198</v>
+      </c>
+      <c r="K569" t="n">
+        <v>0.1872709478582608</v>
+      </c>
+      <c r="L569" t="n">
+        <v>0.1902102483788586</v>
+      </c>
+      <c r="M569" t="n">
+        <v>2.518181527300346</v>
+      </c>
     </row>
     <row r="570">
       <c r="A570" t="inlineStr">
@@ -25754,10 +25810,18 @@
       <c r="I588" t="n">
         <v>7.893800570573736</v>
       </c>
-      <c r="J588" t="inlineStr"/>
-      <c r="K588" t="inlineStr"/>
-      <c r="L588" t="inlineStr"/>
-      <c r="M588" t="inlineStr"/>
+      <c r="J588" t="n">
+        <v>-0.5348266449214059</v>
+      </c>
+      <c r="K588" t="n">
+        <v>0.1282018702557457</v>
+      </c>
+      <c r="L588" t="n">
+        <v>-0.2262958989451835</v>
+      </c>
+      <c r="M588" t="n">
+        <v>2.013425631032702</v>
+      </c>
     </row>
     <row r="589">
       <c r="A589" t="inlineStr">
@@ -26553,10 +26617,18 @@
       <c r="I607" t="n">
         <v>7.814295974217599</v>
       </c>
-      <c r="J607" t="inlineStr"/>
-      <c r="K607" t="inlineStr"/>
-      <c r="L607" t="inlineStr"/>
-      <c r="M607" t="inlineStr"/>
+      <c r="J607" t="n">
+        <v>-0.4136749362997461</v>
+      </c>
+      <c r="K607" t="n">
+        <v>0.1266985367328312</v>
+      </c>
+      <c r="L607" t="n">
+        <v>-0.1582366148292134</v>
+      </c>
+      <c r="M607" t="n">
+        <v>2.04042933805079</v>
+      </c>
     </row>
     <row r="608">
       <c r="A608" t="inlineStr">
@@ -27352,10 +27424,18 @@
       <c r="I626" t="n">
         <v>8.243353072496781</v>
       </c>
-      <c r="J626" t="inlineStr"/>
-      <c r="K626" t="inlineStr"/>
-      <c r="L626" t="inlineStr"/>
-      <c r="M626" t="inlineStr"/>
+      <c r="J626" t="n">
+        <v>-0.2080064881564166</v>
+      </c>
+      <c r="K626" t="n">
+        <v>0.1304043896348948</v>
+      </c>
+      <c r="L626" t="n">
+        <v>-0.09342636787466206</v>
+      </c>
+      <c r="M626" t="n">
+        <v>1.993387849628447</v>
+      </c>
     </row>
     <row r="627">
       <c r="A627" t="inlineStr">
@@ -28104,10 +28184,18 @@
       <c r="I644" t="n">
         <v>14.55164498862496</v>
       </c>
-      <c r="J644" t="inlineStr"/>
-      <c r="K644" t="inlineStr"/>
-      <c r="L644" t="inlineStr"/>
-      <c r="M644" t="inlineStr"/>
+      <c r="J644" t="n">
+        <v>-0.2809526231947743</v>
+      </c>
+      <c r="K644" t="n">
+        <v>0.1328999324788512</v>
+      </c>
+      <c r="L644" t="n">
+        <v>-0.01258305283788508</v>
+      </c>
+      <c r="M644" t="n">
+        <v>1.984619266005203</v>
+      </c>
     </row>
     <row r="645">
       <c r="A645" t="inlineStr">
@@ -28901,10 +28989,18 @@
       <c r="I663" t="n">
         <v>22.22244899502702</v>
       </c>
-      <c r="J663" t="inlineStr"/>
-      <c r="K663" t="inlineStr"/>
-      <c r="L663" t="inlineStr"/>
-      <c r="M663" t="inlineStr"/>
+      <c r="J663" t="n">
+        <v>-0.6067089621107076</v>
+      </c>
+      <c r="K663" t="n">
+        <v>0.1224968750237004</v>
+      </c>
+      <c r="L663" t="n">
+        <v>0.006238849779163275</v>
+      </c>
+      <c r="M663" t="n">
+        <v>2.054960549259019</v>
+      </c>
     </row>
     <row r="664">
       <c r="A664" t="inlineStr">
@@ -29692,10 +29788,18 @@
       <c r="I682" t="n">
         <v>8.659380502592677</v>
       </c>
-      <c r="J682" t="inlineStr"/>
-      <c r="K682" t="inlineStr"/>
-      <c r="L682" t="inlineStr"/>
-      <c r="M682" t="inlineStr"/>
+      <c r="J682" t="n">
+        <v>-0.1107587875764343</v>
+      </c>
+      <c r="K682" t="n">
+        <v>0.1116453926146825</v>
+      </c>
+      <c r="L682" t="n">
+        <v>0.1635099888121481</v>
+      </c>
+      <c r="M682" t="n">
+        <v>2.252950313514092</v>
+      </c>
     </row>
     <row r="683">
       <c r="A683" t="inlineStr">
@@ -30483,10 +30587,18 @@
       <c r="I701" t="n">
         <v>7.471548015969184</v>
       </c>
-      <c r="J701" t="inlineStr"/>
-      <c r="K701" t="inlineStr"/>
-      <c r="L701" t="inlineStr"/>
-      <c r="M701" t="inlineStr"/>
+      <c r="J701" t="n">
+        <v>0.2019572604821628</v>
+      </c>
+      <c r="K701" t="n">
+        <v>0.1159468389252036</v>
+      </c>
+      <c r="L701" t="n">
+        <v>0.07503651310250715</v>
+      </c>
+      <c r="M701" t="n">
+        <v>2.189568379381487</v>
+      </c>
     </row>
     <row r="702">
       <c r="A702" t="inlineStr">
@@ -31274,10 +31386,18 @@
       <c r="I720" t="n">
         <v>10.12607725425915</v>
       </c>
-      <c r="J720" t="inlineStr"/>
-      <c r="K720" t="inlineStr"/>
-      <c r="L720" t="inlineStr"/>
-      <c r="M720" t="inlineStr"/>
+      <c r="J720" t="n">
+        <v>-0.09976713721595667</v>
+      </c>
+      <c r="K720" t="n">
+        <v>0.1226080174363657</v>
+      </c>
+      <c r="L720" t="n">
+        <v>0.1223982275083728</v>
+      </c>
+      <c r="M720" t="n">
+        <v>2.086696089546653</v>
+      </c>
     </row>
     <row r="721">
       <c r="A721" t="inlineStr">
@@ -32018,10 +32138,18 @@
       <c r="I738" t="n">
         <v>6.7565544071346</v>
       </c>
-      <c r="J738" t="inlineStr"/>
-      <c r="K738" t="inlineStr"/>
-      <c r="L738" t="inlineStr"/>
-      <c r="M738" t="inlineStr"/>
+      <c r="J738" t="n">
+        <v>-0.2889366546078636</v>
+      </c>
+      <c r="K738" t="n">
+        <v>0.1255641108669581</v>
+      </c>
+      <c r="L738" t="n">
+        <v>0.2492139062772706</v>
+      </c>
+      <c r="M738" t="n">
+        <v>2.134687693561835</v>
+      </c>
     </row>
     <row r="739">
       <c r="A739" t="inlineStr">
@@ -32533,10 +32661,18 @@
       <c r="I751" t="n">
         <v>11.69664547001226</v>
       </c>
-      <c r="J751" t="inlineStr"/>
-      <c r="K751" t="inlineStr"/>
-      <c r="L751" t="inlineStr"/>
-      <c r="M751" t="inlineStr"/>
+      <c r="J751" t="n">
+        <v>0.3222525556017057</v>
+      </c>
+      <c r="K751" t="n">
+        <v>0.05337495275340508</v>
+      </c>
+      <c r="L751" t="n">
+        <v>-0.4103541666894833</v>
+      </c>
+      <c r="M751" t="n">
+        <v>1.728572074161355</v>
+      </c>
     </row>
     <row r="752">
       <c r="A752" t="inlineStr">
@@ -32760,10 +32896,18 @@
       <c r="I756" t="n">
         <v>24.32112420090724</v>
       </c>
-      <c r="J756" t="inlineStr"/>
-      <c r="K756" t="inlineStr"/>
-      <c r="L756" t="inlineStr"/>
-      <c r="M756" t="inlineStr"/>
+      <c r="J756" t="n">
+        <v>0.4887390112796265</v>
+      </c>
+      <c r="K756" t="n">
+        <v>0.1186085878524447</v>
+      </c>
+      <c r="L756" t="n">
+        <v>0.1721465981455686</v>
+      </c>
+      <c r="M756" t="n">
+        <v>2.224517934906989</v>
+      </c>
     </row>
     <row r="757">
       <c r="A757" t="inlineStr">
@@ -33267,10 +33411,18 @@
       <c r="I769" t="n">
         <v>6.521624677964191</v>
       </c>
-      <c r="J769" t="inlineStr"/>
-      <c r="K769" t="inlineStr"/>
-      <c r="L769" t="inlineStr"/>
-      <c r="M769" t="inlineStr"/>
+      <c r="J769" t="n">
+        <v>-0.009480606601132577</v>
+      </c>
+      <c r="K769" t="n">
+        <v>0.01578916715912978</v>
+      </c>
+      <c r="L769" t="n">
+        <v>-0.2836171216747701</v>
+      </c>
+      <c r="M769" t="n">
+        <v>2.311125364129039</v>
+      </c>
     </row>
     <row r="770">
       <c r="A770" t="inlineStr">
@@ -33306,10 +33458,18 @@
       <c r="I770" t="n">
         <v>9.981517865116112</v>
       </c>
-      <c r="J770" t="inlineStr"/>
-      <c r="K770" t="inlineStr"/>
-      <c r="L770" t="inlineStr"/>
-      <c r="M770" t="inlineStr"/>
+      <c r="J770" t="n">
+        <v>0.008713973304380595</v>
+      </c>
+      <c r="K770" t="n">
+        <v>0.01551982827831129</v>
+      </c>
+      <c r="L770" t="n">
+        <v>-0.5380701125052759</v>
+      </c>
+      <c r="M770" t="n">
+        <v>2.392278948236461</v>
+      </c>
     </row>
     <row r="771">
       <c r="A771" t="inlineStr">
@@ -33386,10 +33546,18 @@
       <c r="I772" t="n">
         <v>6.437865236174289</v>
       </c>
-      <c r="J772" t="inlineStr"/>
-      <c r="K772" t="inlineStr"/>
-      <c r="L772" t="inlineStr"/>
-      <c r="M772" t="inlineStr"/>
+      <c r="J772" t="n">
+        <v>0.06622089617124935</v>
+      </c>
+      <c r="K772" t="n">
+        <v>0.03672917298683431</v>
+      </c>
+      <c r="L772" t="n">
+        <v>0.6725847961907231</v>
+      </c>
+      <c r="M772" t="n">
+        <v>3.168892690376738</v>
+      </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
@@ -33519,10 +33687,18 @@
       <c r="I775" t="n">
         <v>6.701751478932397</v>
       </c>
-      <c r="J775" t="inlineStr"/>
-      <c r="K775" t="inlineStr"/>
-      <c r="L775" t="inlineStr"/>
-      <c r="M775" t="inlineStr"/>
+      <c r="J775" t="n">
+        <v>0.1697846028918021</v>
+      </c>
+      <c r="K775" t="n">
+        <v>0.07334250380262709</v>
+      </c>
+      <c r="L775" t="n">
+        <v>0.4683031253288178</v>
+      </c>
+      <c r="M775" t="n">
+        <v>2.011110609254798</v>
+      </c>
     </row>
     <row r="776">
       <c r="A776" t="inlineStr">
@@ -34026,10 +34202,18 @@
       <c r="I788" t="n">
         <v>5.725677283246958</v>
       </c>
-      <c r="J788" t="inlineStr"/>
-      <c r="K788" t="inlineStr"/>
-      <c r="L788" t="inlineStr"/>
-      <c r="M788" t="inlineStr"/>
+      <c r="J788" t="n">
+        <v>-0.1138270110700734</v>
+      </c>
+      <c r="K788" t="n">
+        <v>0.01678756918276458</v>
+      </c>
+      <c r="L788" t="n">
+        <v>0.053487084533311</v>
+      </c>
+      <c r="M788" t="n">
+        <v>2.298063698297935</v>
+      </c>
     </row>
     <row r="789">
       <c r="A789" t="inlineStr">
@@ -34065,10 +34249,18 @@
       <c r="I789" t="n">
         <v>9.952175328699088</v>
       </c>
-      <c r="J789" t="inlineStr"/>
-      <c r="K789" t="inlineStr"/>
-      <c r="L789" t="inlineStr"/>
-      <c r="M789" t="inlineStr"/>
+      <c r="J789" t="n">
+        <v>-0.08943813976169483</v>
+      </c>
+      <c r="K789" t="n">
+        <v>0.01696372620412041</v>
+      </c>
+      <c r="L789" t="n">
+        <v>-0.2880759216279744</v>
+      </c>
+      <c r="M789" t="n">
+        <v>2.14521553204206</v>
+      </c>
     </row>
     <row r="790">
       <c r="A790" t="inlineStr">
@@ -34104,10 +34296,18 @@
       <c r="I790" t="n">
         <v>5.887377683849195</v>
       </c>
-      <c r="J790" t="inlineStr"/>
-      <c r="K790" t="inlineStr"/>
-      <c r="L790" t="inlineStr"/>
-      <c r="M790" t="inlineStr"/>
+      <c r="J790" t="n">
+        <v>-0.02189067404115775</v>
+      </c>
+      <c r="K790" t="n">
+        <v>0.04191629749799171</v>
+      </c>
+      <c r="L790" t="n">
+        <v>0.6704757719610467</v>
+      </c>
+      <c r="M790" t="n">
+        <v>2.815473210689341</v>
+      </c>
     </row>
     <row r="791">
       <c r="A791" t="inlineStr">
@@ -34184,10 +34384,18 @@
       <c r="I792" t="n">
         <v>15.13411246037325</v>
       </c>
-      <c r="J792" t="inlineStr"/>
-      <c r="K792" t="inlineStr"/>
-      <c r="L792" t="inlineStr"/>
-      <c r="M792" t="inlineStr"/>
+      <c r="J792" t="n">
+        <v>0.03408971441573483</v>
+      </c>
+      <c r="K792" t="n">
+        <v>0.05861338755323488</v>
+      </c>
+      <c r="L792" t="n">
+        <v>0.4399583757458075</v>
+      </c>
+      <c r="M792" t="n">
+        <v>1.992906231796149</v>
+      </c>
     </row>
     <row r="793">
       <c r="A793" t="inlineStr">
@@ -34270,10 +34478,18 @@
       <c r="I794" t="n">
         <v>6.835166303708448</v>
       </c>
-      <c r="J794" t="inlineStr"/>
-      <c r="K794" t="inlineStr"/>
-      <c r="L794" t="inlineStr"/>
-      <c r="M794" t="inlineStr"/>
+      <c r="J794" t="n">
+        <v>0.09378818548282215</v>
+      </c>
+      <c r="K794" t="n">
+        <v>0.08061204851819169</v>
+      </c>
+      <c r="L794" t="n">
+        <v>0.3553474179588729</v>
+      </c>
+      <c r="M794" t="n">
+        <v>1.795346708229094</v>
+      </c>
     </row>
     <row r="795">
       <c r="A795" t="inlineStr">
@@ -34777,10 +34993,18 @@
       <c r="I807" t="n">
         <v>5.963606545374893</v>
       </c>
-      <c r="J807" t="inlineStr"/>
-      <c r="K807" t="inlineStr"/>
-      <c r="L807" t="inlineStr"/>
-      <c r="M807" t="inlineStr"/>
+      <c r="J807" t="n">
+        <v>0.2473204566274169</v>
+      </c>
+      <c r="K807" t="n">
+        <v>0.008750979825177335</v>
+      </c>
+      <c r="L807" t="n">
+        <v>0.8089196720461374</v>
+      </c>
+      <c r="M807" t="n">
+        <v>2.101860250809634</v>
+      </c>
     </row>
     <row r="808">
       <c r="A808" t="inlineStr">
@@ -34816,10 +35040,18 @@
       <c r="I808" t="n">
         <v>16.54907703958716</v>
       </c>
-      <c r="J808" t="inlineStr"/>
-      <c r="K808" t="inlineStr"/>
-      <c r="L808" t="inlineStr"/>
-      <c r="M808" t="inlineStr"/>
+      <c r="J808" t="n">
+        <v>0.2666942839323744</v>
+      </c>
+      <c r="K808" t="n">
+        <v>0.008502164597911139</v>
+      </c>
+      <c r="L808" t="n">
+        <v>0.2680339375067249</v>
+      </c>
+      <c r="M808" t="n">
+        <v>1.532865872683723</v>
+      </c>
     </row>
     <row r="809">
       <c r="A809" t="inlineStr">
@@ -34855,10 +35087,18 @@
       <c r="I809" t="n">
         <v>6.484052199504728</v>
       </c>
-      <c r="J809" t="inlineStr"/>
-      <c r="K809" t="inlineStr"/>
-      <c r="L809" t="inlineStr"/>
-      <c r="M809" t="inlineStr"/>
+      <c r="J809" t="n">
+        <v>0.3380914860526574</v>
+      </c>
+      <c r="K809" t="n">
+        <v>0.03257293951794873</v>
+      </c>
+      <c r="L809" t="n">
+        <v>1.009832860521988</v>
+      </c>
+      <c r="M809" t="n">
+        <v>2.815720396193842</v>
+      </c>
     </row>
     <row r="810">
       <c r="A810" t="inlineStr">
@@ -34894,10 +35134,18 @@
       <c r="I810" t="n">
         <v>6.861491321269101</v>
       </c>
-      <c r="J810" t="inlineStr"/>
-      <c r="K810" t="inlineStr"/>
-      <c r="L810" t="inlineStr"/>
-      <c r="M810" t="inlineStr"/>
+      <c r="J810" t="n">
+        <v>0.3951692466145622</v>
+      </c>
+      <c r="K810" t="n">
+        <v>0.04746688694852878</v>
+      </c>
+      <c r="L810" t="n">
+        <v>0.569185250568909</v>
+      </c>
+      <c r="M810" t="n">
+        <v>1.739304231923645</v>
+      </c>
     </row>
     <row r="811">
       <c r="A811" t="inlineStr">
@@ -34974,10 +35222,18 @@
       <c r="I812" t="n">
         <v>7.131555547897904</v>
       </c>
-      <c r="J812" t="inlineStr"/>
-      <c r="K812" t="inlineStr"/>
-      <c r="L812" t="inlineStr"/>
-      <c r="M812" t="inlineStr"/>
+      <c r="J812" t="n">
+        <v>0.4561555070866828</v>
+      </c>
+      <c r="K812" t="n">
+        <v>0.06756879384457612</v>
+      </c>
+      <c r="L812" t="n">
+        <v>0.4030054558325659</v>
+      </c>
+      <c r="M812" t="n">
+        <v>1.590884813525737</v>
+      </c>
     </row>
     <row r="813">
       <c r="A813" t="inlineStr">
@@ -35096,6 +35352,3807 @@
       <c r="L815" t="inlineStr"/>
       <c r="M815" t="inlineStr"/>
     </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D816" t="n">
+        <v>0.05753424657534247</v>
+      </c>
+      <c r="E816" t="n">
+        <v>111950.099610962</v>
+      </c>
+      <c r="F816" t="n">
+        <v>0.002293563032286254</v>
+      </c>
+      <c r="G816" t="n">
+        <v>0.1576424449324726</v>
+      </c>
+      <c r="H816" t="n">
+        <v>-0.8055530864960956</v>
+      </c>
+      <c r="I816" t="n">
+        <v>6.814174400985319</v>
+      </c>
+      <c r="J816" t="inlineStr"/>
+      <c r="K816" t="inlineStr"/>
+      <c r="L816" t="inlineStr"/>
+      <c r="M816" t="inlineStr"/>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D817" t="n">
+        <v>0.1534246575342466</v>
+      </c>
+      <c r="E817" t="n">
+        <v>112803.1891561327</v>
+      </c>
+      <c r="F817" t="n">
+        <v>9.701185263500406e-05</v>
+      </c>
+      <c r="G817" t="n">
+        <v>0.1722957261695063</v>
+      </c>
+      <c r="H817" t="n">
+        <v>-1.22248897823845</v>
+      </c>
+      <c r="I817" t="n">
+        <v>10.43423696254672</v>
+      </c>
+      <c r="J817" t="inlineStr"/>
+      <c r="K817" t="inlineStr"/>
+      <c r="L817" t="inlineStr"/>
+      <c r="M817" t="inlineStr"/>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D818" t="n">
+        <v>0.2301369863013699</v>
+      </c>
+      <c r="E818" t="n">
+        <v>113606.554906055</v>
+      </c>
+      <c r="F818" t="n">
+        <v>-0.002890898904414514</v>
+      </c>
+      <c r="G818" t="n">
+        <v>0.1923176121256891</v>
+      </c>
+      <c r="H818" t="n">
+        <v>-1.132220241259939</v>
+      </c>
+      <c r="I818" t="n">
+        <v>9.957529844255356</v>
+      </c>
+      <c r="J818" t="inlineStr"/>
+      <c r="K818" t="inlineStr"/>
+      <c r="L818" t="inlineStr"/>
+      <c r="M818" t="inlineStr"/>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D819" t="n">
+        <v>0.3068493150684932</v>
+      </c>
+      <c r="E819" t="n">
+        <v>114194.4678753093</v>
+      </c>
+      <c r="F819" t="n">
+        <v>-0.012021211363259</v>
+      </c>
+      <c r="G819" t="n">
+        <v>0.2232821526960972</v>
+      </c>
+      <c r="H819" t="n">
+        <v>-1.308430985346893</v>
+      </c>
+      <c r="I819" t="n">
+        <v>9.890040629932885</v>
+      </c>
+      <c r="J819" t="inlineStr"/>
+      <c r="K819" t="inlineStr"/>
+      <c r="L819" t="inlineStr"/>
+      <c r="M819" t="inlineStr"/>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D820" t="n">
+        <v>0.4027397260273973</v>
+      </c>
+      <c r="E820" t="n">
+        <v>115094.6184930315</v>
+      </c>
+      <c r="F820" t="n">
+        <v>-0.01131461168908758</v>
+      </c>
+      <c r="G820" t="n">
+        <v>0.2045939589546089</v>
+      </c>
+      <c r="H820" t="n">
+        <v>-0.5604727309264568</v>
+      </c>
+      <c r="I820" t="n">
+        <v>5.218431885528368</v>
+      </c>
+      <c r="J820" t="inlineStr"/>
+      <c r="K820" t="inlineStr"/>
+      <c r="L820" t="inlineStr"/>
+      <c r="M820" t="inlineStr"/>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D821" t="n">
+        <v>0.4794520547945205</v>
+      </c>
+      <c r="E821" t="n">
+        <v>115744.2328964068</v>
+      </c>
+      <c r="F821" t="n">
+        <v>-0.01428943651869636</v>
+      </c>
+      <c r="G821" t="n">
+        <v>0.2051886454571602</v>
+      </c>
+      <c r="H821" t="n">
+        <v>-0.4031830220238187</v>
+      </c>
+      <c r="I821" t="n">
+        <v>4.761088007090696</v>
+      </c>
+      <c r="J821" t="inlineStr"/>
+      <c r="K821" t="inlineStr"/>
+      <c r="L821" t="inlineStr"/>
+      <c r="M821" t="inlineStr"/>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D822" t="n">
+        <v>0.7287671232876712</v>
+      </c>
+      <c r="E822" t="n">
+        <v>115896.2040295099</v>
+      </c>
+      <c r="F822" t="n">
+        <v>-0.032632487527276</v>
+      </c>
+      <c r="G822" t="n">
+        <v>0.2093133162937546</v>
+      </c>
+      <c r="H822" t="n">
+        <v>-1.367002483580489</v>
+      </c>
+      <c r="I822" t="n">
+        <v>9.01776789703051</v>
+      </c>
+      <c r="J822" t="inlineStr"/>
+      <c r="K822" t="inlineStr"/>
+      <c r="L822" t="inlineStr"/>
+      <c r="M822" t="inlineStr"/>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D823" t="n">
+        <v>0.8054794520547945</v>
+      </c>
+      <c r="E823" t="n">
+        <v>117591.1708460943</v>
+      </c>
+      <c r="F823" t="n">
+        <v>-0.05756627903728836</v>
+      </c>
+      <c r="G823" t="n">
+        <v>0.3136165992303823</v>
+      </c>
+      <c r="H823" t="n">
+        <v>-1.583661129879171</v>
+      </c>
+      <c r="I823" t="n">
+        <v>9.505436324235388</v>
+      </c>
+      <c r="J823" t="inlineStr"/>
+      <c r="K823" t="inlineStr"/>
+      <c r="L823" t="inlineStr"/>
+      <c r="M823" t="inlineStr"/>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D824" t="n">
+        <v>1.054794520547945</v>
+      </c>
+      <c r="E824" t="n">
+        <v>118988.9405505411</v>
+      </c>
+      <c r="F824" t="n">
+        <v>-0.09833901090262025</v>
+      </c>
+      <c r="G824" t="n">
+        <v>0.4186621339055681</v>
+      </c>
+      <c r="H824" t="n">
+        <v>-1.930336354359066</v>
+      </c>
+      <c r="I824" t="n">
+        <v>10.06319598730032</v>
+      </c>
+      <c r="J824" t="inlineStr"/>
+      <c r="K824" t="inlineStr"/>
+      <c r="L824" t="inlineStr"/>
+      <c r="M824" t="inlineStr"/>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D825" t="n">
+        <v>1.301369863013699</v>
+      </c>
+      <c r="E825" t="n">
+        <v>120893.2601175081</v>
+      </c>
+      <c r="F825" t="n">
+        <v>-0.1603343416758367</v>
+      </c>
+      <c r="G825" t="n">
+        <v>0.6466744142559917</v>
+      </c>
+      <c r="H825" t="n">
+        <v>-2.221641284329906</v>
+      </c>
+      <c r="I825" t="n">
+        <v>9.531777449110113</v>
+      </c>
+      <c r="J825" t="inlineStr"/>
+      <c r="K825" t="inlineStr"/>
+      <c r="L825" t="inlineStr"/>
+      <c r="M825" t="inlineStr"/>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D826" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E826" t="n">
+        <v>111922.4848009286</v>
+      </c>
+      <c r="F826" t="n">
+        <v>0.04762781495851497</v>
+      </c>
+      <c r="G826" t="n">
+        <v>0.08711891077207809</v>
+      </c>
+      <c r="H826" t="n">
+        <v>-0.6451696411852456</v>
+      </c>
+      <c r="I826" t="n">
+        <v>5.799865174877321</v>
+      </c>
+      <c r="J826" t="n">
+        <v>0.01517991677278606</v>
+      </c>
+      <c r="K826" t="n">
+        <v>0.011610365631929</v>
+      </c>
+      <c r="L826" t="n">
+        <v>0.6004555249989233</v>
+      </c>
+      <c r="M826" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D827" t="n">
+        <v>0.0273972602739726</v>
+      </c>
+      <c r="E827" t="n">
+        <v>111913.636236021</v>
+      </c>
+      <c r="F827" t="n">
+        <v>0.0150794376495774</v>
+      </c>
+      <c r="G827" t="n">
+        <v>0.153530327157326</v>
+      </c>
+      <c r="H827" t="n">
+        <v>-0.8414873904767076</v>
+      </c>
+      <c r="I827" t="n">
+        <v>7.011937907066979</v>
+      </c>
+      <c r="J827" t="inlineStr"/>
+      <c r="K827" t="inlineStr"/>
+      <c r="L827" t="inlineStr"/>
+      <c r="M827" t="inlineStr"/>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D828" t="n">
+        <v>0.01095890410958904</v>
+      </c>
+      <c r="E828" t="n">
+        <v>111992.6742273136</v>
+      </c>
+      <c r="F828" t="n">
+        <v>0.04413863204402541</v>
+      </c>
+      <c r="G828" t="n">
+        <v>0.1239319196069358</v>
+      </c>
+      <c r="H828" t="n">
+        <v>-0.3799280037148337</v>
+      </c>
+      <c r="I828" t="n">
+        <v>4.67882136465155</v>
+      </c>
+      <c r="J828" t="n">
+        <v>0.03844845610568442</v>
+      </c>
+      <c r="K828" t="n">
+        <v>0.01033204899200667</v>
+      </c>
+      <c r="L828" t="n">
+        <v>0.02964126085934176</v>
+      </c>
+      <c r="M828" t="n">
+        <v>1.252041615773261</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D829" t="n">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="E829" t="n">
+        <v>111922.4151948104</v>
+      </c>
+      <c r="F829" t="n">
+        <v>0.03155389514894694</v>
+      </c>
+      <c r="G829" t="n">
+        <v>0.1428362445838861</v>
+      </c>
+      <c r="H829" t="n">
+        <v>-0.7838226599377212</v>
+      </c>
+      <c r="I829" t="n">
+        <v>6.07017067294946</v>
+      </c>
+      <c r="J829" t="n">
+        <v>0.1225871604057971</v>
+      </c>
+      <c r="K829" t="n">
+        <v>0.03658292543881253</v>
+      </c>
+      <c r="L829" t="n">
+        <v>0.7269108226853095</v>
+      </c>
+      <c r="M829" t="n">
+        <v>2.283258046995905</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D830" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E830" t="n">
+        <v>111949.0290608311</v>
+      </c>
+      <c r="F830" t="n">
+        <v>0.02820439540375154</v>
+      </c>
+      <c r="G830" t="n">
+        <v>0.1567903892481256</v>
+      </c>
+      <c r="H830" t="n">
+        <v>-0.6609413669389544</v>
+      </c>
+      <c r="I830" t="n">
+        <v>5.829481920231169</v>
+      </c>
+      <c r="J830" t="n">
+        <v>0.1857726821611913</v>
+      </c>
+      <c r="K830" t="n">
+        <v>0.05044782199651743</v>
+      </c>
+      <c r="L830" t="n">
+        <v>0.3093338362019623</v>
+      </c>
+      <c r="M830" t="n">
+        <v>1.524200376593016</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D831" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E831" t="n">
+        <v>111872.231584931</v>
+      </c>
+      <c r="F831" t="n">
+        <v>0.01892712527436574</v>
+      </c>
+      <c r="G831" t="n">
+        <v>0.1702764310070614</v>
+      </c>
+      <c r="H831" t="n">
+        <v>-1.604158327874284</v>
+      </c>
+      <c r="I831" t="n">
+        <v>15.01642476338653</v>
+      </c>
+      <c r="J831" t="n">
+        <v>0.2516799863301211</v>
+      </c>
+      <c r="K831" t="n">
+        <v>0.0693036267396242</v>
+      </c>
+      <c r="L831" t="n">
+        <v>0.166800521123699</v>
+      </c>
+      <c r="M831" t="n">
+        <v>1.492689794117197</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D832" t="n">
+        <v>0.03835616438356165</v>
+      </c>
+      <c r="E832" t="n">
+        <v>111980.2028822354</v>
+      </c>
+      <c r="F832" t="n">
+        <v>0.01053782083727607</v>
+      </c>
+      <c r="G832" t="n">
+        <v>0.1625916714896777</v>
+      </c>
+      <c r="H832" t="n">
+        <v>-0.79344328612077</v>
+      </c>
+      <c r="I832" t="n">
+        <v>7.251224732472367</v>
+      </c>
+      <c r="J832" t="inlineStr"/>
+      <c r="K832" t="inlineStr"/>
+      <c r="L832" t="inlineStr"/>
+      <c r="M832" t="inlineStr"/>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D833" t="n">
+        <v>0.07671232876712329</v>
+      </c>
+      <c r="E833" t="n">
+        <v>112967.1226771672</v>
+      </c>
+      <c r="F833" t="n">
+        <v>0.02772516384122036</v>
+      </c>
+      <c r="G833" t="n">
+        <v>0.1595180809597363</v>
+      </c>
+      <c r="H833" t="n">
+        <v>-0.5854302720873038</v>
+      </c>
+      <c r="I833" t="n">
+        <v>5.571798574880623</v>
+      </c>
+      <c r="J833" t="inlineStr"/>
+      <c r="K833" t="inlineStr"/>
+      <c r="L833" t="inlineStr"/>
+      <c r="M833" t="inlineStr"/>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D834" t="n">
+        <v>0.0958904109589041</v>
+      </c>
+      <c r="E834" t="n">
+        <v>112806.9498575561</v>
+      </c>
+      <c r="F834" t="n">
+        <v>0.01433507702473926</v>
+      </c>
+      <c r="G834" t="n">
+        <v>0.168378615873762</v>
+      </c>
+      <c r="H834" t="n">
+        <v>-0.6562902607940158</v>
+      </c>
+      <c r="I834" t="n">
+        <v>5.371320605976026</v>
+      </c>
+      <c r="J834" t="inlineStr"/>
+      <c r="K834" t="inlineStr"/>
+      <c r="L834" t="inlineStr"/>
+      <c r="M834" t="inlineStr"/>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D835" t="n">
+        <v>0.04931506849315068</v>
+      </c>
+      <c r="E835" t="n">
+        <v>112475.662957574</v>
+      </c>
+      <c r="F835" t="n">
+        <v>-0.01140724445524908</v>
+      </c>
+      <c r="G835" t="n">
+        <v>0.1479596428958266</v>
+      </c>
+      <c r="H835" t="n">
+        <v>-0.8570923606517562</v>
+      </c>
+      <c r="I835" t="n">
+        <v>7.170469853157511</v>
+      </c>
+      <c r="J835" t="inlineStr"/>
+      <c r="K835" t="inlineStr"/>
+      <c r="L835" t="inlineStr"/>
+      <c r="M835" t="inlineStr"/>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D836" t="n">
+        <v>0.1452054794520548</v>
+      </c>
+      <c r="E836" t="n">
+        <v>113312.1531741012</v>
+      </c>
+      <c r="F836" t="n">
+        <v>-0.008099423416980949</v>
+      </c>
+      <c r="G836" t="n">
+        <v>0.1674370927440353</v>
+      </c>
+      <c r="H836" t="n">
+        <v>-1.303595366108981</v>
+      </c>
+      <c r="I836" t="n">
+        <v>11.75268514010502</v>
+      </c>
+      <c r="J836" t="inlineStr"/>
+      <c r="K836" t="inlineStr"/>
+      <c r="L836" t="inlineStr"/>
+      <c r="M836" t="inlineStr"/>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D837" t="n">
+        <v>0.2219178082191781</v>
+      </c>
+      <c r="E837" t="n">
+        <v>114012.9960156796</v>
+      </c>
+      <c r="F837" t="n">
+        <v>-0.012793570798794</v>
+      </c>
+      <c r="G837" t="n">
+        <v>0.2077691993767707</v>
+      </c>
+      <c r="H837" t="n">
+        <v>-2.505932944546365</v>
+      </c>
+      <c r="I837" t="n">
+        <v>28.71420195217609</v>
+      </c>
+      <c r="J837" t="inlineStr"/>
+      <c r="K837" t="inlineStr"/>
+      <c r="L837" t="inlineStr"/>
+      <c r="M837" t="inlineStr"/>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D838" t="n">
+        <v>0.2986301369863014</v>
+      </c>
+      <c r="E838" t="n">
+        <v>114772.4762990291</v>
+      </c>
+      <c r="F838" t="n">
+        <v>-0.01270215520375952</v>
+      </c>
+      <c r="G838" t="n">
+        <v>0.2013345021341199</v>
+      </c>
+      <c r="H838" t="n">
+        <v>-1.073502543772299</v>
+      </c>
+      <c r="I838" t="n">
+        <v>8.792760753136537</v>
+      </c>
+      <c r="J838" t="inlineStr"/>
+      <c r="K838" t="inlineStr"/>
+      <c r="L838" t="inlineStr"/>
+      <c r="M838" t="inlineStr"/>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D839" t="n">
+        <v>0.3945205479452055</v>
+      </c>
+      <c r="E839" t="n">
+        <v>115925.7710213943</v>
+      </c>
+      <c r="F839" t="n">
+        <v>-0.01070196667881092</v>
+      </c>
+      <c r="G839" t="n">
+        <v>0.1998130525869451</v>
+      </c>
+      <c r="H839" t="n">
+        <v>-0.8023875817831331</v>
+      </c>
+      <c r="I839" t="n">
+        <v>7.399622717820547</v>
+      </c>
+      <c r="J839" t="inlineStr"/>
+      <c r="K839" t="inlineStr"/>
+      <c r="L839" t="inlineStr"/>
+      <c r="M839" t="inlineStr"/>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D840" t="n">
+        <v>0.4712328767123288</v>
+      </c>
+      <c r="E840" t="n">
+        <v>116306.7190943286</v>
+      </c>
+      <c r="F840" t="n">
+        <v>-0.02223758087095558</v>
+      </c>
+      <c r="G840" t="n">
+        <v>0.227079742128506</v>
+      </c>
+      <c r="H840" t="n">
+        <v>-1.179416438324198</v>
+      </c>
+      <c r="I840" t="n">
+        <v>8.389009548028856</v>
+      </c>
+      <c r="J840" t="inlineStr"/>
+      <c r="K840" t="inlineStr"/>
+      <c r="L840" t="inlineStr"/>
+      <c r="M840" t="inlineStr"/>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D841" t="n">
+        <v>0.7205479452054795</v>
+      </c>
+      <c r="E841" t="n">
+        <v>116442.3861980024</v>
+      </c>
+      <c r="F841" t="n">
+        <v>-0.03448748950367278</v>
+      </c>
+      <c r="G841" t="n">
+        <v>0.2029215864781988</v>
+      </c>
+      <c r="H841" t="n">
+        <v>-1.368716605644995</v>
+      </c>
+      <c r="I841" t="n">
+        <v>9.458329263714418</v>
+      </c>
+      <c r="J841" t="inlineStr"/>
+      <c r="K841" t="inlineStr"/>
+      <c r="L841" t="inlineStr"/>
+      <c r="M841" t="inlineStr"/>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D842" t="n">
+        <v>0.7972602739726027</v>
+      </c>
+      <c r="E842" t="n">
+        <v>117951.8372220107</v>
+      </c>
+      <c r="F842" t="n">
+        <v>-0.0613640345435921</v>
+      </c>
+      <c r="G842" t="n">
+        <v>0.3077364299375565</v>
+      </c>
+      <c r="H842" t="n">
+        <v>-1.520785764836273</v>
+      </c>
+      <c r="I842" t="n">
+        <v>8.9093404038132</v>
+      </c>
+      <c r="J842" t="inlineStr"/>
+      <c r="K842" t="inlineStr"/>
+      <c r="L842" t="inlineStr"/>
+      <c r="M842" t="inlineStr"/>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D843" t="n">
+        <v>1.046575342465753</v>
+      </c>
+      <c r="E843" t="n">
+        <v>119528.7813635168</v>
+      </c>
+      <c r="F843" t="n">
+        <v>-0.09413004086265164</v>
+      </c>
+      <c r="G843" t="n">
+        <v>0.3762842735929738</v>
+      </c>
+      <c r="H843" t="n">
+        <v>-1.524244133288902</v>
+      </c>
+      <c r="I843" t="n">
+        <v>7.404424575030574</v>
+      </c>
+      <c r="J843" t="inlineStr"/>
+      <c r="K843" t="inlineStr"/>
+      <c r="L843" t="inlineStr"/>
+      <c r="M843" t="inlineStr"/>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D844" t="n">
+        <v>1.293150684931507</v>
+      </c>
+      <c r="E844" t="n">
+        <v>124114.848909564</v>
+      </c>
+      <c r="F844" t="n">
+        <v>-0.09117028907325496</v>
+      </c>
+      <c r="G844" t="n">
+        <v>0.4233968085335629</v>
+      </c>
+      <c r="H844" t="n">
+        <v>-1.776333503404707</v>
+      </c>
+      <c r="I844" t="n">
+        <v>7.648188420902539</v>
+      </c>
+      <c r="J844" t="inlineStr"/>
+      <c r="K844" t="inlineStr"/>
+      <c r="L844" t="inlineStr"/>
+      <c r="M844" t="inlineStr"/>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D845" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E845" t="n">
+        <v>112482.3875728318</v>
+      </c>
+      <c r="F845" t="n">
+        <v>-0.002507994126054419</v>
+      </c>
+      <c r="G845" t="n">
+        <v>0.1443621796361534</v>
+      </c>
+      <c r="H845" t="n">
+        <v>-0.7780749770495108</v>
+      </c>
+      <c r="I845" t="n">
+        <v>6.288697433255122</v>
+      </c>
+      <c r="J845" t="inlineStr"/>
+      <c r="K845" t="inlineStr"/>
+      <c r="L845" t="inlineStr"/>
+      <c r="M845" t="inlineStr"/>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D846" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E846" t="n">
+        <v>112480.9607316328</v>
+      </c>
+      <c r="F846" t="n">
+        <v>0.0150908187715532</v>
+      </c>
+      <c r="G846" t="n">
+        <v>0.1706598524907748</v>
+      </c>
+      <c r="H846" t="n">
+        <v>-0.08230811079841927</v>
+      </c>
+      <c r="I846" t="n">
+        <v>2.854703979207449</v>
+      </c>
+      <c r="J846" t="n">
+        <v>-0.0566961977795883</v>
+      </c>
+      <c r="K846" t="inlineStr"/>
+      <c r="L846" t="inlineStr"/>
+      <c r="M846" t="inlineStr"/>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D847" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E847" t="n">
+        <v>112458.2279090198</v>
+      </c>
+      <c r="F847" t="n">
+        <v>-0.005862230499384257</v>
+      </c>
+      <c r="G847" t="n">
+        <v>0.1559461381421021</v>
+      </c>
+      <c r="H847" t="n">
+        <v>-1.301167218025355</v>
+      </c>
+      <c r="I847" t="n">
+        <v>12.53748302699012</v>
+      </c>
+      <c r="J847" t="inlineStr"/>
+      <c r="K847" t="inlineStr"/>
+      <c r="L847" t="inlineStr"/>
+      <c r="M847" t="inlineStr"/>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D848" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E848" t="n">
+        <v>112515.9762390781</v>
+      </c>
+      <c r="F848" t="n">
+        <v>0.01323934363543634</v>
+      </c>
+      <c r="G848" t="n">
+        <v>0.1292365718580022</v>
+      </c>
+      <c r="H848" t="n">
+        <v>-0.2941812139323229</v>
+      </c>
+      <c r="I848" t="n">
+        <v>3.649714375147955</v>
+      </c>
+      <c r="J848" t="n">
+        <v>0.1187477539713453</v>
+      </c>
+      <c r="K848" t="n">
+        <v>0.03078058020598393</v>
+      </c>
+      <c r="L848" t="n">
+        <v>0</v>
+      </c>
+      <c r="M848" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D849" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E849" t="n">
+        <v>112453.5870632726</v>
+      </c>
+      <c r="F849" t="n">
+        <v>0.001925339802519785</v>
+      </c>
+      <c r="G849" t="n">
+        <v>0.1471464165632581</v>
+      </c>
+      <c r="H849" t="n">
+        <v>-0.6512128457295741</v>
+      </c>
+      <c r="I849" t="n">
+        <v>4.665193692170698</v>
+      </c>
+      <c r="J849" t="n">
+        <v>0.1914151756656277</v>
+      </c>
+      <c r="K849" t="n">
+        <v>0.03108149515537862</v>
+      </c>
+      <c r="L849" t="n">
+        <v>-0.6763282335868304</v>
+      </c>
+      <c r="M849" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D850" t="n">
+        <v>0.01095890410958904</v>
+      </c>
+      <c r="E850" t="n">
+        <v>112457.6135103974</v>
+      </c>
+      <c r="F850" t="n">
+        <v>-0.0002936800205633542</v>
+      </c>
+      <c r="G850" t="n">
+        <v>0.1543298320016014</v>
+      </c>
+      <c r="H850" t="n">
+        <v>-0.6487565508246312</v>
+      </c>
+      <c r="I850" t="n">
+        <v>4.764132664041259</v>
+      </c>
+      <c r="J850" t="n">
+        <v>0.2641047666141533</v>
+      </c>
+      <c r="K850" t="n">
+        <v>0.03916245126332588</v>
+      </c>
+      <c r="L850" t="n">
+        <v>-0.7172214601094596</v>
+      </c>
+      <c r="M850" t="n">
+        <v>2.09969529306094</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D851" t="n">
+        <v>0.03013698630136986</v>
+      </c>
+      <c r="E851" t="n">
+        <v>112456.2436100248</v>
+      </c>
+      <c r="F851" t="n">
+        <v>-0.008741226341814163</v>
+      </c>
+      <c r="G851" t="n">
+        <v>0.1516867128355948</v>
+      </c>
+      <c r="H851" t="n">
+        <v>-0.892777600240229</v>
+      </c>
+      <c r="I851" t="n">
+        <v>7.989412686763538</v>
+      </c>
+      <c r="J851" t="inlineStr"/>
+      <c r="K851" t="inlineStr"/>
+      <c r="L851" t="inlineStr"/>
+      <c r="M851" t="inlineStr"/>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D852" t="n">
+        <v>0.0684931506849315</v>
+      </c>
+      <c r="E852" t="n">
+        <v>113432.6861886893</v>
+      </c>
+      <c r="F852" t="n">
+        <v>0.01519265919609604</v>
+      </c>
+      <c r="G852" t="n">
+        <v>0.1554297902898029</v>
+      </c>
+      <c r="H852" t="n">
+        <v>-0.6966288237316405</v>
+      </c>
+      <c r="I852" t="n">
+        <v>5.976765079822982</v>
+      </c>
+      <c r="J852" t="inlineStr"/>
+      <c r="K852" t="inlineStr"/>
+      <c r="L852" t="inlineStr"/>
+      <c r="M852" t="inlineStr"/>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D853" t="n">
+        <v>0.08767123287671233</v>
+      </c>
+      <c r="E853" t="n">
+        <v>113506.1505157483</v>
+      </c>
+      <c r="F853" t="n">
+        <v>0.01119191427840498</v>
+      </c>
+      <c r="G853" t="n">
+        <v>0.1510260353990546</v>
+      </c>
+      <c r="H853" t="n">
+        <v>-0.5673556417208362</v>
+      </c>
+      <c r="I853" t="n">
+        <v>5.362469780063074</v>
+      </c>
+      <c r="J853" t="inlineStr"/>
+      <c r="K853" t="inlineStr"/>
+      <c r="L853" t="inlineStr"/>
+      <c r="M853" t="inlineStr"/>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D854" t="n">
+        <v>0.04657534246575343</v>
+      </c>
+      <c r="E854" t="n">
+        <v>111692.8557318299</v>
+      </c>
+      <c r="F854" t="n">
+        <v>-0.02978019917966164</v>
+      </c>
+      <c r="G854" t="n">
+        <v>0.151382802620357</v>
+      </c>
+      <c r="H854" t="n">
+        <v>-0.9054379426187182</v>
+      </c>
+      <c r="I854" t="n">
+        <v>7.342438936742024</v>
+      </c>
+      <c r="J854" t="inlineStr"/>
+      <c r="K854" t="inlineStr"/>
+      <c r="L854" t="inlineStr"/>
+      <c r="M854" t="inlineStr"/>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D855" t="n">
+        <v>0.1424657534246575</v>
+      </c>
+      <c r="E855" t="n">
+        <v>112533.3663530384</v>
+      </c>
+      <c r="F855" t="n">
+        <v>-0.01909430404073182</v>
+      </c>
+      <c r="G855" t="n">
+        <v>0.1728155143652927</v>
+      </c>
+      <c r="H855" t="n">
+        <v>-1.197035217388404</v>
+      </c>
+      <c r="I855" t="n">
+        <v>10.83309386973573</v>
+      </c>
+      <c r="J855" t="inlineStr"/>
+      <c r="K855" t="inlineStr"/>
+      <c r="L855" t="inlineStr"/>
+      <c r="M855" t="inlineStr"/>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D856" t="n">
+        <v>0.2191780821917808</v>
+      </c>
+      <c r="E856" t="n">
+        <v>113288.9772318856</v>
+      </c>
+      <c r="F856" t="n">
+        <v>-0.01747892637678835</v>
+      </c>
+      <c r="G856" t="n">
+        <v>0.1849611553562259</v>
+      </c>
+      <c r="H856" t="n">
+        <v>-1.072600169010829</v>
+      </c>
+      <c r="I856" t="n">
+        <v>9.790210802075562</v>
+      </c>
+      <c r="J856" t="inlineStr"/>
+      <c r="K856" t="inlineStr"/>
+      <c r="L856" t="inlineStr"/>
+      <c r="M856" t="inlineStr"/>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D857" t="n">
+        <v>0.2958904109589041</v>
+      </c>
+      <c r="E857" t="n">
+        <v>113900.3231499783</v>
+      </c>
+      <c r="F857" t="n">
+        <v>-0.02368654860695967</v>
+      </c>
+      <c r="G857" t="n">
+        <v>0.2163594752020082</v>
+      </c>
+      <c r="H857" t="n">
+        <v>-1.339703353023801</v>
+      </c>
+      <c r="I857" t="n">
+        <v>10.59577337693559</v>
+      </c>
+      <c r="J857" t="inlineStr"/>
+      <c r="K857" t="inlineStr"/>
+      <c r="L857" t="inlineStr"/>
+      <c r="M857" t="inlineStr"/>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D858" t="n">
+        <v>0.3917808219178082</v>
+      </c>
+      <c r="E858" t="n">
+        <v>115144.3146739977</v>
+      </c>
+      <c r="F858" t="n">
+        <v>-0.01639491294144225</v>
+      </c>
+      <c r="G858" t="n">
+        <v>0.1993073123251151</v>
+      </c>
+      <c r="H858" t="n">
+        <v>-0.7577353613084802</v>
+      </c>
+      <c r="I858" t="n">
+        <v>7.358984147436302</v>
+      </c>
+      <c r="J858" t="inlineStr"/>
+      <c r="K858" t="inlineStr"/>
+      <c r="L858" t="inlineStr"/>
+      <c r="M858" t="inlineStr"/>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D859" t="n">
+        <v>0.4684931506849315</v>
+      </c>
+      <c r="E859" t="n">
+        <v>115387.2238974011</v>
+      </c>
+      <c r="F859" t="n">
+        <v>-0.02329718423332614</v>
+      </c>
+      <c r="G859" t="n">
+        <v>0.1995879168664023</v>
+      </c>
+      <c r="H859" t="n">
+        <v>-0.458548781342674</v>
+      </c>
+      <c r="I859" t="n">
+        <v>4.907928602178837</v>
+      </c>
+      <c r="J859" t="inlineStr"/>
+      <c r="K859" t="inlineStr"/>
+      <c r="L859" t="inlineStr"/>
+      <c r="M859" t="inlineStr"/>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D860" t="n">
+        <v>0.7178082191780822</v>
+      </c>
+      <c r="E860" t="n">
+        <v>115643.8970641071</v>
+      </c>
+      <c r="F860" t="n">
+        <v>-0.03772782925476648</v>
+      </c>
+      <c r="G860" t="n">
+        <v>0.1979718113957536</v>
+      </c>
+      <c r="H860" t="n">
+        <v>-1.26383357387501</v>
+      </c>
+      <c r="I860" t="n">
+        <v>8.61775566765486</v>
+      </c>
+      <c r="J860" t="inlineStr"/>
+      <c r="K860" t="inlineStr"/>
+      <c r="L860" t="inlineStr"/>
+      <c r="M860" t="inlineStr"/>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D861" t="n">
+        <v>0.7945205479452054</v>
+      </c>
+      <c r="E861" t="n">
+        <v>117145.8746894842</v>
+      </c>
+      <c r="F861" t="n">
+        <v>-0.06899021943994139</v>
+      </c>
+      <c r="G861" t="n">
+        <v>0.3365088729482733</v>
+      </c>
+      <c r="H861" t="n">
+        <v>-2.147626684546458</v>
+      </c>
+      <c r="I861" t="n">
+        <v>14.56777003057582</v>
+      </c>
+      <c r="J861" t="inlineStr"/>
+      <c r="K861" t="inlineStr"/>
+      <c r="L861" t="inlineStr"/>
+      <c r="M861" t="inlineStr"/>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D862" t="n">
+        <v>1.043835616438356</v>
+      </c>
+      <c r="E862" t="n">
+        <v>119065.8908675039</v>
+      </c>
+      <c r="F862" t="n">
+        <v>-0.09262717413222762</v>
+      </c>
+      <c r="G862" t="n">
+        <v>0.3716522798905745</v>
+      </c>
+      <c r="H862" t="n">
+        <v>-1.568533238273599</v>
+      </c>
+      <c r="I862" t="n">
+        <v>7.749363819803936</v>
+      </c>
+      <c r="J862" t="inlineStr"/>
+      <c r="K862" t="inlineStr"/>
+      <c r="L862" t="inlineStr"/>
+      <c r="M862" t="inlineStr"/>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D863" t="n">
+        <v>1.29041095890411</v>
+      </c>
+      <c r="E863" t="n">
+        <v>120553.510853111</v>
+      </c>
+      <c r="F863" t="n">
+        <v>-0.1721178514439965</v>
+      </c>
+      <c r="G863" t="n">
+        <v>0.6900071227775538</v>
+      </c>
+      <c r="H863" t="n">
+        <v>-2.465197232454836</v>
+      </c>
+      <c r="I863" t="n">
+        <v>11.56419141630363</v>
+      </c>
+      <c r="J863" t="inlineStr"/>
+      <c r="K863" t="inlineStr"/>
+      <c r="L863" t="inlineStr"/>
+      <c r="M863" t="inlineStr"/>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D864" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E864" t="n">
+        <v>111670.0798448132</v>
+      </c>
+      <c r="F864" t="n">
+        <v>-0.03411409254850937</v>
+      </c>
+      <c r="G864" t="n">
+        <v>0.1370553137700598</v>
+      </c>
+      <c r="H864" t="n">
+        <v>-0.765143271326474</v>
+      </c>
+      <c r="I864" t="n">
+        <v>5.569029515826807</v>
+      </c>
+      <c r="J864" t="inlineStr"/>
+      <c r="K864" t="inlineStr"/>
+      <c r="L864" t="inlineStr"/>
+      <c r="M864" t="inlineStr"/>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D865" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E865" t="n">
+        <v>111665.0203247202</v>
+      </c>
+      <c r="F865" t="n">
+        <v>-0.03576786013764902</v>
+      </c>
+      <c r="G865" t="n">
+        <v>0.177376198156932</v>
+      </c>
+      <c r="H865" t="n">
+        <v>-2.068079523258437</v>
+      </c>
+      <c r="I865" t="n">
+        <v>20.1619959523439</v>
+      </c>
+      <c r="J865" t="inlineStr"/>
+      <c r="K865" t="inlineStr"/>
+      <c r="L865" t="inlineStr"/>
+      <c r="M865" t="inlineStr"/>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D866" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E866" t="n">
+        <v>111688.7990336683</v>
+      </c>
+      <c r="F866" t="n">
+        <v>-0.06296146532803061</v>
+      </c>
+      <c r="G866" t="n">
+        <v>0.1584295623194165</v>
+      </c>
+      <c r="H866" t="n">
+        <v>-0.2874276068137356</v>
+      </c>
+      <c r="I866" t="n">
+        <v>3.532153242931081</v>
+      </c>
+      <c r="J866" t="n">
+        <v>0.3508879035018694</v>
+      </c>
+      <c r="K866" t="inlineStr"/>
+      <c r="L866" t="inlineStr"/>
+      <c r="M866" t="inlineStr"/>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D867" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E867" t="n">
+        <v>111679.8640223027</v>
+      </c>
+      <c r="F867" t="n">
+        <v>-0.03284312000629162</v>
+      </c>
+      <c r="G867" t="n">
+        <v>0.154014745352272</v>
+      </c>
+      <c r="H867" t="n">
+        <v>-0.7949601440235577</v>
+      </c>
+      <c r="I867" t="n">
+        <v>6.163366665062721</v>
+      </c>
+      <c r="J867" t="inlineStr"/>
+      <c r="K867" t="inlineStr"/>
+      <c r="L867" t="inlineStr"/>
+      <c r="M867" t="inlineStr"/>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D868" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E868" t="n">
+        <v>111666.0790384044</v>
+      </c>
+      <c r="F868" t="n">
+        <v>-0.05063734851008633</v>
+      </c>
+      <c r="G868" t="n">
+        <v>0.1645880042060623</v>
+      </c>
+      <c r="H868" t="n">
+        <v>-0.6960658641234545</v>
+      </c>
+      <c r="I868" t="n">
+        <v>5.014656566263765</v>
+      </c>
+      <c r="J868" t="n">
+        <v>0.372167060167827</v>
+      </c>
+      <c r="K868" t="n">
+        <v>0.0004528025084143649</v>
+      </c>
+      <c r="L868" t="n">
+        <v>0</v>
+      </c>
+      <c r="M868" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D869" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E869" t="n">
+        <v>111832.5791653157</v>
+      </c>
+      <c r="F869" t="n">
+        <v>-0.02580327913082217</v>
+      </c>
+      <c r="G869" t="n">
+        <v>0.1321951162532141</v>
+      </c>
+      <c r="H869" t="n">
+        <v>-0.1376978415711794</v>
+      </c>
+      <c r="I869" t="n">
+        <v>3.261113816929032</v>
+      </c>
+      <c r="J869" t="n">
+        <v>0.4277346191916581</v>
+      </c>
+      <c r="K869" t="n">
+        <v>0.006477375570676819</v>
+      </c>
+      <c r="L869" t="n">
+        <v>0.5617269463841342</v>
+      </c>
+      <c r="M869" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D870" t="n">
+        <v>0.0273972602739726</v>
+      </c>
+      <c r="E870" t="n">
+        <v>111692.7655187572</v>
+      </c>
+      <c r="F870" t="n">
+        <v>-0.03077740083379396</v>
+      </c>
+      <c r="G870" t="n">
+        <v>0.1498019996298361</v>
+      </c>
+      <c r="H870" t="n">
+        <v>-0.659716127185082</v>
+      </c>
+      <c r="I870" t="n">
+        <v>4.395867897681192</v>
+      </c>
+      <c r="J870" t="inlineStr"/>
+      <c r="K870" t="inlineStr"/>
+      <c r="L870" t="inlineStr"/>
+      <c r="M870" t="inlineStr"/>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D871" t="n">
+        <v>0.06575342465753424</v>
+      </c>
+      <c r="E871" t="n">
+        <v>112661.4737912152</v>
+      </c>
+      <c r="F871" t="n">
+        <v>0.0005820466789978624</v>
+      </c>
+      <c r="G871" t="n">
+        <v>0.1607083540159102</v>
+      </c>
+      <c r="H871" t="n">
+        <v>-0.7126075700381211</v>
+      </c>
+      <c r="I871" t="n">
+        <v>6.152338567716306</v>
+      </c>
+      <c r="J871" t="inlineStr"/>
+      <c r="K871" t="inlineStr"/>
+      <c r="L871" t="inlineStr"/>
+      <c r="M871" t="inlineStr"/>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D872" t="n">
+        <v>0.08493150684931507</v>
+      </c>
+      <c r="E872" t="n">
+        <v>112740.4488893053</v>
+      </c>
+      <c r="F872" t="n">
+        <v>-0.001688626208177548</v>
+      </c>
+      <c r="G872" t="n">
+        <v>0.1556460445123202</v>
+      </c>
+      <c r="H872" t="n">
+        <v>-0.5878175865459662</v>
+      </c>
+      <c r="I872" t="n">
+        <v>5.49745497074329</v>
+      </c>
+      <c r="J872" t="inlineStr"/>
+      <c r="K872" t="inlineStr"/>
+      <c r="L872" t="inlineStr"/>
+      <c r="M872" t="inlineStr"/>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D873" t="n">
+        <v>0.04383561643835616</v>
+      </c>
+      <c r="E873" t="n">
+        <v>113966.0020390408</v>
+      </c>
+      <c r="F873" t="n">
+        <v>-0.02019068875068475</v>
+      </c>
+      <c r="G873" t="n">
+        <v>0.1422298944151117</v>
+      </c>
+      <c r="H873" t="n">
+        <v>-1.155574717578378</v>
+      </c>
+      <c r="I873" t="n">
+        <v>9.067577376010485</v>
+      </c>
+      <c r="J873" t="inlineStr"/>
+      <c r="K873" t="inlineStr"/>
+      <c r="L873" t="inlineStr"/>
+      <c r="M873" t="inlineStr"/>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D874" t="n">
+        <v>0.1397260273972603</v>
+      </c>
+      <c r="E874" t="n">
+        <v>114844.0209407878</v>
+      </c>
+      <c r="F874" t="n">
+        <v>-0.01147814113835749</v>
+      </c>
+      <c r="G874" t="n">
+        <v>0.1601478971891726</v>
+      </c>
+      <c r="H874" t="n">
+        <v>-0.9580917562449961</v>
+      </c>
+      <c r="I874" t="n">
+        <v>8.774752746187053</v>
+      </c>
+      <c r="J874" t="inlineStr"/>
+      <c r="K874" t="inlineStr"/>
+      <c r="L874" t="inlineStr"/>
+      <c r="M874" t="inlineStr"/>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D875" t="n">
+        <v>0.2164383561643836</v>
+      </c>
+      <c r="E875" t="n">
+        <v>115515.869752923</v>
+      </c>
+      <c r="F875" t="n">
+        <v>-0.01592502307528787</v>
+      </c>
+      <c r="G875" t="n">
+        <v>0.1990772191342972</v>
+      </c>
+      <c r="H875" t="n">
+        <v>-2.054822895080575</v>
+      </c>
+      <c r="I875" t="n">
+        <v>22.59032950166808</v>
+      </c>
+      <c r="J875" t="inlineStr"/>
+      <c r="K875" t="inlineStr"/>
+      <c r="L875" t="inlineStr"/>
+      <c r="M875" t="inlineStr"/>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D876" t="n">
+        <v>0.2931506849315069</v>
+      </c>
+      <c r="E876" t="n">
+        <v>116211.0805787633</v>
+      </c>
+      <c r="F876" t="n">
+        <v>-0.01862042913758765</v>
+      </c>
+      <c r="G876" t="n">
+        <v>0.2098840880663143</v>
+      </c>
+      <c r="H876" t="n">
+        <v>-1.346662516236812</v>
+      </c>
+      <c r="I876" t="n">
+        <v>11.11023615142587</v>
+      </c>
+      <c r="J876" t="inlineStr"/>
+      <c r="K876" t="inlineStr"/>
+      <c r="L876" t="inlineStr"/>
+      <c r="M876" t="inlineStr"/>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D877" t="n">
+        <v>0.389041095890411</v>
+      </c>
+      <c r="E877" t="n">
+        <v>117085.3086362548</v>
+      </c>
+      <c r="F877" t="n">
+        <v>-0.01804408797976221</v>
+      </c>
+      <c r="G877" t="n">
+        <v>0.1957327655809966</v>
+      </c>
+      <c r="H877" t="n">
+        <v>-0.5089991861496532</v>
+      </c>
+      <c r="I877" t="n">
+        <v>5.447365761971636</v>
+      </c>
+      <c r="J877" t="inlineStr"/>
+      <c r="K877" t="inlineStr"/>
+      <c r="L877" t="inlineStr"/>
+      <c r="M877" t="inlineStr"/>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D878" t="n">
+        <v>0.4657534246575342</v>
+      </c>
+      <c r="E878" t="n">
+        <v>117651.688109483</v>
+      </c>
+      <c r="F878" t="n">
+        <v>-0.02112700459447586</v>
+      </c>
+      <c r="G878" t="n">
+        <v>0.1985533269114679</v>
+      </c>
+      <c r="H878" t="n">
+        <v>-0.447509631384117</v>
+      </c>
+      <c r="I878" t="n">
+        <v>4.924906125811309</v>
+      </c>
+      <c r="J878" t="inlineStr"/>
+      <c r="K878" t="inlineStr"/>
+      <c r="L878" t="inlineStr"/>
+      <c r="M878" t="inlineStr"/>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D879" t="n">
+        <v>0.7150684931506849</v>
+      </c>
+      <c r="E879" t="n">
+        <v>118033.0961083623</v>
+      </c>
+      <c r="F879" t="n">
+        <v>-0.03100746028196988</v>
+      </c>
+      <c r="G879" t="n">
+        <v>0.1829234050421697</v>
+      </c>
+      <c r="H879" t="n">
+        <v>-1.044357573098943</v>
+      </c>
+      <c r="I879" t="n">
+        <v>7.623420468169047</v>
+      </c>
+      <c r="J879" t="inlineStr"/>
+      <c r="K879" t="inlineStr"/>
+      <c r="L879" t="inlineStr"/>
+      <c r="M879" t="inlineStr"/>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D880" t="n">
+        <v>0.7917808219178082</v>
+      </c>
+      <c r="E880" t="n">
+        <v>119644.0947283433</v>
+      </c>
+      <c r="F880" t="n">
+        <v>-0.05873003840620205</v>
+      </c>
+      <c r="G880" t="n">
+        <v>0.2998770116182286</v>
+      </c>
+      <c r="H880" t="n">
+        <v>-1.639501452798533</v>
+      </c>
+      <c r="I880" t="n">
+        <v>10.22861815132921</v>
+      </c>
+      <c r="J880" t="inlineStr"/>
+      <c r="K880" t="inlineStr"/>
+      <c r="L880" t="inlineStr"/>
+      <c r="M880" t="inlineStr"/>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D881" t="n">
+        <v>1.041095890410959</v>
+      </c>
+      <c r="E881" t="n">
+        <v>121131.23864154</v>
+      </c>
+      <c r="F881" t="n">
+        <v>-0.09440700874141618</v>
+      </c>
+      <c r="G881" t="n">
+        <v>0.3724649451006405</v>
+      </c>
+      <c r="H881" t="n">
+        <v>-1.539195331449584</v>
+      </c>
+      <c r="I881" t="n">
+        <v>7.638666498372044</v>
+      </c>
+      <c r="J881" t="inlineStr"/>
+      <c r="K881" t="inlineStr"/>
+      <c r="L881" t="inlineStr"/>
+      <c r="M881" t="inlineStr"/>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D882" t="n">
+        <v>1.287671232876712</v>
+      </c>
+      <c r="E882" t="n">
+        <v>123015.1402100438</v>
+      </c>
+      <c r="F882" t="n">
+        <v>-0.1663162442947912</v>
+      </c>
+      <c r="G882" t="n">
+        <v>0.6741482216423634</v>
+      </c>
+      <c r="H882" t="n">
+        <v>-2.481752741124204</v>
+      </c>
+      <c r="I882" t="n">
+        <v>11.77182058450353</v>
+      </c>
+      <c r="J882" t="inlineStr"/>
+      <c r="K882" t="inlineStr"/>
+      <c r="L882" t="inlineStr"/>
+      <c r="M882" t="inlineStr"/>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D883" t="n">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="E883" t="n">
+        <v>113993.9418785267</v>
+      </c>
+      <c r="F883" t="n">
+        <v>-0.01465248833798145</v>
+      </c>
+      <c r="G883" t="n">
+        <v>0.1033554704649684</v>
+      </c>
+      <c r="H883" t="n">
+        <v>-0.4606119637827947</v>
+      </c>
+      <c r="I883" t="n">
+        <v>4.846217837762755</v>
+      </c>
+      <c r="J883" t="inlineStr"/>
+      <c r="K883" t="inlineStr"/>
+      <c r="L883" t="inlineStr"/>
+      <c r="M883" t="inlineStr"/>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D884" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E884" t="n">
+        <v>113964.1828323864</v>
+      </c>
+      <c r="F884" t="n">
+        <v>-0.01790247203149638</v>
+      </c>
+      <c r="G884" t="n">
+        <v>0.1248690766954584</v>
+      </c>
+      <c r="H884" t="n">
+        <v>-0.6019047713575554</v>
+      </c>
+      <c r="I884" t="n">
+        <v>6.231117724616652</v>
+      </c>
+      <c r="J884" t="inlineStr"/>
+      <c r="K884" t="inlineStr"/>
+      <c r="L884" t="inlineStr"/>
+      <c r="M884" t="inlineStr"/>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D885" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E885" t="n">
+        <v>113973.5165954895</v>
+      </c>
+      <c r="F885" t="n">
+        <v>-0.01800359444710063</v>
+      </c>
+      <c r="G885" t="n">
+        <v>0.1362922172484409</v>
+      </c>
+      <c r="H885" t="n">
+        <v>-0.7495326897990063</v>
+      </c>
+      <c r="I885" t="n">
+        <v>8.339794479936625</v>
+      </c>
+      <c r="J885" t="inlineStr"/>
+      <c r="K885" t="inlineStr"/>
+      <c r="L885" t="inlineStr"/>
+      <c r="M885" t="inlineStr"/>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D886" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E886" t="n">
+        <v>113965.5365941751</v>
+      </c>
+      <c r="F886" t="n">
+        <v>-0.02906250579649617</v>
+      </c>
+      <c r="G886" t="n">
+        <v>0.1937452402338606</v>
+      </c>
+      <c r="H886" t="n">
+        <v>-0.3055711069215656</v>
+      </c>
+      <c r="I886" t="n">
+        <v>3.737845614877521</v>
+      </c>
+      <c r="J886" t="n">
+        <v>0.04255831333191579</v>
+      </c>
+      <c r="K886" t="inlineStr"/>
+      <c r="L886" t="inlineStr"/>
+      <c r="M886" t="inlineStr"/>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D887" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E887" t="n">
+        <v>113968.4134717482</v>
+      </c>
+      <c r="F887" t="n">
+        <v>-0.01871483372635751</v>
+      </c>
+      <c r="G887" t="n">
+        <v>0.1412410803627646</v>
+      </c>
+      <c r="H887" t="n">
+        <v>-1.051959857265147</v>
+      </c>
+      <c r="I887" t="n">
+        <v>9.44350494178971</v>
+      </c>
+      <c r="J887" t="inlineStr"/>
+      <c r="K887" t="inlineStr"/>
+      <c r="L887" t="inlineStr"/>
+      <c r="M887" t="inlineStr"/>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D888" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E888" t="n">
+        <v>113870.6143231212</v>
+      </c>
+      <c r="F888" t="n">
+        <v>-0.03457679372244465</v>
+      </c>
+      <c r="G888" t="n">
+        <v>0.1754765463214087</v>
+      </c>
+      <c r="H888" t="n">
+        <v>-2.875323048374219</v>
+      </c>
+      <c r="I888" t="n">
+        <v>41.74605748340719</v>
+      </c>
+      <c r="J888" t="n">
+        <v>0.1152700735346838</v>
+      </c>
+      <c r="K888" t="n">
+        <v>0.005287000071784839</v>
+      </c>
+      <c r="L888" t="n">
+        <v>2.820306437580456e-16</v>
+      </c>
+      <c r="M888" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D889" t="n">
+        <v>0.02465753424657534</v>
+      </c>
+      <c r="E889" t="n">
+        <v>113662.2692810884</v>
+      </c>
+      <c r="F889" t="n">
+        <v>-0.03501634020698981</v>
+      </c>
+      <c r="G889" t="n">
+        <v>0.1249154147729686</v>
+      </c>
+      <c r="H889" t="n">
+        <v>-0.977151454675463</v>
+      </c>
+      <c r="I889" t="n">
+        <v>4.886035991046247</v>
+      </c>
+      <c r="J889" t="inlineStr"/>
+      <c r="K889" t="inlineStr"/>
+      <c r="L889" t="inlineStr"/>
+      <c r="M889" t="inlineStr"/>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D890" t="n">
+        <v>0.06301369863013699</v>
+      </c>
+      <c r="E890" t="n">
+        <v>114852.3618998145</v>
+      </c>
+      <c r="F890" t="n">
+        <v>0.004737104570537671</v>
+      </c>
+      <c r="G890" t="n">
+        <v>0.1681804327611288</v>
+      </c>
+      <c r="H890" t="n">
+        <v>-1.554544496040412</v>
+      </c>
+      <c r="I890" t="n">
+        <v>13.66311307545645</v>
+      </c>
+      <c r="J890" t="inlineStr"/>
+      <c r="K890" t="inlineStr"/>
+      <c r="L890" t="inlineStr"/>
+      <c r="M890" t="inlineStr"/>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D891" t="n">
+        <v>0.0821917808219178</v>
+      </c>
+      <c r="E891" t="n">
+        <v>114919.1486275211</v>
+      </c>
+      <c r="F891" t="n">
+        <v>0.00262655417426444</v>
+      </c>
+      <c r="G891" t="n">
+        <v>0.1529268621405513</v>
+      </c>
+      <c r="H891" t="n">
+        <v>-0.7141480375004229</v>
+      </c>
+      <c r="I891" t="n">
+        <v>6.127519854420505</v>
+      </c>
+      <c r="J891" t="inlineStr"/>
+      <c r="K891" t="inlineStr"/>
+      <c r="L891" t="inlineStr"/>
+      <c r="M891" t="inlineStr"/>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D892" t="n">
+        <v>0.0410958904109589</v>
+      </c>
+      <c r="E892" t="n">
+        <v>114918.5308086081</v>
+      </c>
+      <c r="F892" t="n">
+        <v>0.01118684779909018</v>
+      </c>
+      <c r="G892" t="n">
+        <v>0.1314238568440338</v>
+      </c>
+      <c r="H892" t="n">
+        <v>-1.16181985114501</v>
+      </c>
+      <c r="I892" t="n">
+        <v>11.197878828116</v>
+      </c>
+      <c r="J892" t="inlineStr"/>
+      <c r="K892" t="inlineStr"/>
+      <c r="L892" t="inlineStr"/>
+      <c r="M892" t="inlineStr"/>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D893" t="n">
+        <v>0.136986301369863</v>
+      </c>
+      <c r="E893" t="n">
+        <v>115796.9201424547</v>
+      </c>
+      <c r="F893" t="n">
+        <v>0.006491812400758156</v>
+      </c>
+      <c r="G893" t="n">
+        <v>0.1534774055175853</v>
+      </c>
+      <c r="H893" t="n">
+        <v>-1.005341598809046</v>
+      </c>
+      <c r="I893" t="n">
+        <v>9.359814936911434</v>
+      </c>
+      <c r="J893" t="inlineStr"/>
+      <c r="K893" t="inlineStr"/>
+      <c r="L893" t="inlineStr"/>
+      <c r="M893" t="inlineStr"/>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D894" t="n">
+        <v>0.2136986301369863</v>
+      </c>
+      <c r="E894" t="n">
+        <v>116449.0693108803</v>
+      </c>
+      <c r="F894" t="n">
+        <v>-0.0005002575585284747</v>
+      </c>
+      <c r="G894" t="n">
+        <v>0.1858648855850594</v>
+      </c>
+      <c r="H894" t="n">
+        <v>-1.997911804475045</v>
+      </c>
+      <c r="I894" t="n">
+        <v>24.79221564491825</v>
+      </c>
+      <c r="J894" t="inlineStr"/>
+      <c r="K894" t="inlineStr"/>
+      <c r="L894" t="inlineStr"/>
+      <c r="M894" t="inlineStr"/>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D895" t="n">
+        <v>0.2904109589041096</v>
+      </c>
+      <c r="E895" t="n">
+        <v>117150.6044848357</v>
+      </c>
+      <c r="F895" t="n">
+        <v>-0.005997622062143608</v>
+      </c>
+      <c r="G895" t="n">
+        <v>0.2038613149371446</v>
+      </c>
+      <c r="H895" t="n">
+        <v>-1.36640288000329</v>
+      </c>
+      <c r="I895" t="n">
+        <v>11.67456551442118</v>
+      </c>
+      <c r="J895" t="inlineStr"/>
+      <c r="K895" t="inlineStr"/>
+      <c r="L895" t="inlineStr"/>
+      <c r="M895" t="inlineStr"/>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D896" t="n">
+        <v>0.3863013698630137</v>
+      </c>
+      <c r="E896" t="n">
+        <v>118340.540732479</v>
+      </c>
+      <c r="F896" t="n">
+        <v>-0.003068942802712522</v>
+      </c>
+      <c r="G896" t="n">
+        <v>0.1930367445363273</v>
+      </c>
+      <c r="H896" t="n">
+        <v>-0.7290535773892177</v>
+      </c>
+      <c r="I896" t="n">
+        <v>7.575851361816929</v>
+      </c>
+      <c r="J896" t="inlineStr"/>
+      <c r="K896" t="inlineStr"/>
+      <c r="L896" t="inlineStr"/>
+      <c r="M896" t="inlineStr"/>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D897" t="n">
+        <v>0.463013698630137</v>
+      </c>
+      <c r="E897" t="n">
+        <v>119127.5604092949</v>
+      </c>
+      <c r="F897" t="n">
+        <v>-0.004464042831141681</v>
+      </c>
+      <c r="G897" t="n">
+        <v>0.1943644839292936</v>
+      </c>
+      <c r="H897" t="n">
+        <v>-0.5980225829751022</v>
+      </c>
+      <c r="I897" t="n">
+        <v>6.744307934915907</v>
+      </c>
+      <c r="J897" t="inlineStr"/>
+      <c r="K897" t="inlineStr"/>
+      <c r="L897" t="inlineStr"/>
+      <c r="M897" t="inlineStr"/>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D898" t="n">
+        <v>0.7123287671232876</v>
+      </c>
+      <c r="E898" t="n">
+        <v>118904.8725118622</v>
+      </c>
+      <c r="F898" t="n">
+        <v>-0.02796733025776764</v>
+      </c>
+      <c r="G898" t="n">
+        <v>0.2081743371558379</v>
+      </c>
+      <c r="H898" t="n">
+        <v>-2.281703596102505</v>
+      </c>
+      <c r="I898" t="n">
+        <v>21.23155279173184</v>
+      </c>
+      <c r="J898" t="inlineStr"/>
+      <c r="K898" t="inlineStr"/>
+      <c r="L898" t="inlineStr"/>
+      <c r="M898" t="inlineStr"/>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D899" t="n">
+        <v>0.7890410958904109</v>
+      </c>
+      <c r="E899" t="n">
+        <v>120402.3797145811</v>
+      </c>
+      <c r="F899" t="n">
+        <v>-0.05890508454771556</v>
+      </c>
+      <c r="G899" t="n">
+        <v>0.3320216454383011</v>
+      </c>
+      <c r="H899" t="n">
+        <v>-2.225657344303349</v>
+      </c>
+      <c r="I899" t="n">
+        <v>15.64812030733237</v>
+      </c>
+      <c r="J899" t="inlineStr"/>
+      <c r="K899" t="inlineStr"/>
+      <c r="L899" t="inlineStr"/>
+      <c r="M899" t="inlineStr"/>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D900" t="n">
+        <v>1.038356164383562</v>
+      </c>
+      <c r="E900" t="n">
+        <v>122396.7385939461</v>
+      </c>
+      <c r="F900" t="n">
+        <v>-0.08230125668399267</v>
+      </c>
+      <c r="G900" t="n">
+        <v>0.3608128632518757</v>
+      </c>
+      <c r="H900" t="n">
+        <v>-1.555847424069358</v>
+      </c>
+      <c r="I900" t="n">
+        <v>7.978259481991468</v>
+      </c>
+      <c r="J900" t="inlineStr"/>
+      <c r="K900" t="inlineStr"/>
+      <c r="L900" t="inlineStr"/>
+      <c r="M900" t="inlineStr"/>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D901" t="n">
+        <v>1.284931506849315</v>
+      </c>
+      <c r="E901" t="n">
+        <v>123956.9059203563</v>
+      </c>
+      <c r="F901" t="n">
+        <v>-0.1555348028303687</v>
+      </c>
+      <c r="G901" t="n">
+        <v>0.635867501115666</v>
+      </c>
+      <c r="H901" t="n">
+        <v>-2.316233665953103</v>
+      </c>
+      <c r="I901" t="n">
+        <v>10.40252333034482</v>
+      </c>
+      <c r="J901" t="inlineStr"/>
+      <c r="K901" t="inlineStr"/>
+      <c r="L901" t="inlineStr"/>
+      <c r="M901" t="inlineStr"/>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D902" t="n">
+        <v>0.01095890410958904</v>
+      </c>
+      <c r="E902" t="n">
+        <v>114907.1611602911</v>
+      </c>
+      <c r="F902" t="n">
+        <v>0.04110106206138803</v>
+      </c>
+      <c r="G902" t="n">
+        <v>0.08100610714862778</v>
+      </c>
+      <c r="H902" t="n">
+        <v>-0.3779824366373084</v>
+      </c>
+      <c r="I902" t="n">
+        <v>4.32887360222632</v>
+      </c>
+      <c r="J902" t="inlineStr"/>
+      <c r="K902" t="inlineStr"/>
+      <c r="L902" t="inlineStr"/>
+      <c r="M902" t="inlineStr"/>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D903" t="n">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="E903" t="n">
+        <v>114907.0504968996</v>
+      </c>
+      <c r="F903" t="n">
+        <v>0.0342434638350548</v>
+      </c>
+      <c r="G903" t="n">
+        <v>0.1073213503608973</v>
+      </c>
+      <c r="H903" t="n">
+        <v>-0.6775292914356353</v>
+      </c>
+      <c r="I903" t="n">
+        <v>6.837531519633435</v>
+      </c>
+      <c r="J903" t="inlineStr"/>
+      <c r="K903" t="inlineStr"/>
+      <c r="L903" t="inlineStr"/>
+      <c r="M903" t="inlineStr"/>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D904" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E904" t="n">
+        <v>114913.2812801584</v>
+      </c>
+      <c r="F904" t="n">
+        <v>0.03002364862387137</v>
+      </c>
+      <c r="G904" t="n">
+        <v>0.1157903226938213</v>
+      </c>
+      <c r="H904" t="n">
+        <v>-0.6842554309232842</v>
+      </c>
+      <c r="I904" t="n">
+        <v>6.917147901119264</v>
+      </c>
+      <c r="J904" t="inlineStr"/>
+      <c r="K904" t="inlineStr"/>
+      <c r="L904" t="inlineStr"/>
+      <c r="M904" t="inlineStr"/>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D905" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E905" t="n">
+        <v>114919.3780948793</v>
+      </c>
+      <c r="F905" t="n">
+        <v>0.0266177752194584</v>
+      </c>
+      <c r="G905" t="n">
+        <v>0.1220424823457438</v>
+      </c>
+      <c r="H905" t="n">
+        <v>-0.5896884140553141</v>
+      </c>
+      <c r="I905" t="n">
+        <v>6.245935127005477</v>
+      </c>
+      <c r="J905" t="inlineStr"/>
+      <c r="K905" t="inlineStr"/>
+      <c r="L905" t="inlineStr"/>
+      <c r="M905" t="inlineStr"/>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D906" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E906" t="n">
+        <v>114895.4938747079</v>
+      </c>
+      <c r="F906" t="n">
+        <v>0.08509746701371777</v>
+      </c>
+      <c r="G906" t="n">
+        <v>0.1393197082059368</v>
+      </c>
+      <c r="H906" t="n">
+        <v>-0.1758196602645248</v>
+      </c>
+      <c r="I906" t="n">
+        <v>2.677979182211032</v>
+      </c>
+      <c r="J906" t="n">
+        <v>0.1454235204055392</v>
+      </c>
+      <c r="K906" t="inlineStr"/>
+      <c r="L906" t="inlineStr"/>
+      <c r="M906" t="inlineStr"/>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D907" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E907" t="n">
+        <v>114835.7125178231</v>
+      </c>
+      <c r="F907" t="n">
+        <v>0.01876034836425523</v>
+      </c>
+      <c r="G907" t="n">
+        <v>0.1228341155971844</v>
+      </c>
+      <c r="H907" t="n">
+        <v>-0.9097778929356922</v>
+      </c>
+      <c r="I907" t="n">
+        <v>6.016509364523203</v>
+      </c>
+      <c r="J907" t="inlineStr"/>
+      <c r="K907" t="inlineStr"/>
+      <c r="L907" t="inlineStr"/>
+      <c r="M907" t="inlineStr"/>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D908" t="n">
+        <v>0.06027397260273973</v>
+      </c>
+      <c r="E908" t="n">
+        <v>115786.5778048187</v>
+      </c>
+      <c r="F908" t="n">
+        <v>0.03135289385886732</v>
+      </c>
+      <c r="G908" t="n">
+        <v>0.153489402768434</v>
+      </c>
+      <c r="H908" t="n">
+        <v>-1.438802980095279</v>
+      </c>
+      <c r="I908" t="n">
+        <v>13.76763375469023</v>
+      </c>
+      <c r="J908" t="inlineStr"/>
+      <c r="K908" t="inlineStr"/>
+      <c r="L908" t="inlineStr"/>
+      <c r="M908" t="inlineStr"/>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D909" t="n">
+        <v>0.07945205479452055</v>
+      </c>
+      <c r="E909" t="n">
+        <v>115814.2537922122</v>
+      </c>
+      <c r="F909" t="n">
+        <v>0.02382300163682413</v>
+      </c>
+      <c r="G909" t="n">
+        <v>0.1461734146402583</v>
+      </c>
+      <c r="H909" t="n">
+        <v>-0.5896684427599178</v>
+      </c>
+      <c r="I909" t="n">
+        <v>5.479943412847926</v>
+      </c>
+      <c r="J909" t="inlineStr"/>
+      <c r="K909" t="inlineStr"/>
+      <c r="L909" t="inlineStr"/>
+      <c r="M909" t="inlineStr"/>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D910" t="n">
+        <v>0.09863013698630137</v>
+      </c>
+      <c r="E910" t="n">
+        <v>116004.9588301066</v>
+      </c>
+      <c r="F910" t="n">
+        <v>0.02250472055527215</v>
+      </c>
+      <c r="G910" t="n">
+        <v>0.1409292166276038</v>
+      </c>
+      <c r="H910" t="n">
+        <v>-0.5441822519686473</v>
+      </c>
+      <c r="I910" t="n">
+        <v>5.834648396060894</v>
+      </c>
+      <c r="J910" t="inlineStr"/>
+      <c r="K910" t="inlineStr"/>
+      <c r="L910" t="inlineStr"/>
+      <c r="M910" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update of moment analysis data
</commit_message>
<xml_diff>
--- a/data_analyzed/moment.xlsx
+++ b/data_analyzed/moment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M910"/>
+  <dimension ref="A1:M986"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35823,10 +35823,18 @@
       <c r="I827" t="n">
         <v>7.011937907066979</v>
       </c>
-      <c r="J827" t="inlineStr"/>
-      <c r="K827" t="inlineStr"/>
-      <c r="L827" t="inlineStr"/>
-      <c r="M827" t="inlineStr"/>
+      <c r="J827" t="n">
+        <v>0.3779298801345128</v>
+      </c>
+      <c r="K827" t="n">
+        <v>0.08732206993011483</v>
+      </c>
+      <c r="L827" t="n">
+        <v>-0.3326748274291247</v>
+      </c>
+      <c r="M827" t="n">
+        <v>1.552525783804963</v>
+      </c>
     </row>
     <row r="828">
       <c r="A828" t="inlineStr">
@@ -36557,10 +36565,18 @@
       <c r="I845" t="n">
         <v>6.288697433255122</v>
       </c>
-      <c r="J845" t="inlineStr"/>
-      <c r="K845" t="inlineStr"/>
-      <c r="L845" t="inlineStr"/>
-      <c r="M845" t="inlineStr"/>
+      <c r="J845" t="n">
+        <v>0.368443878262713</v>
+      </c>
+      <c r="K845" t="n">
+        <v>0.03920614569937778</v>
+      </c>
+      <c r="L845" t="n">
+        <v>-1.127910942023814</v>
+      </c>
+      <c r="M845" t="n">
+        <v>3.329723141697085</v>
+      </c>
     </row>
     <row r="846">
       <c r="A846" t="inlineStr">
@@ -36637,10 +36653,18 @@
       <c r="I847" t="n">
         <v>5.450011004942664</v>
       </c>
-      <c r="J847" t="inlineStr"/>
-      <c r="K847" t="inlineStr"/>
-      <c r="L847" t="inlineStr"/>
-      <c r="M847" t="inlineStr"/>
+      <c r="J847" t="n">
+        <v>0.3802977549935186</v>
+      </c>
+      <c r="K847" t="n">
+        <v>0.03528897824179948</v>
+      </c>
+      <c r="L847" t="n">
+        <v>-1.329203199933692</v>
+      </c>
+      <c r="M847" t="n">
+        <v>3.915931171864705</v>
+      </c>
     </row>
     <row r="848">
       <c r="A848" t="inlineStr">
@@ -37324,10 +37348,18 @@
       <c r="I864" t="n">
         <v>5.569029515826807</v>
       </c>
-      <c r="J864" t="inlineStr"/>
-      <c r="K864" t="inlineStr"/>
-      <c r="L864" t="inlineStr"/>
-      <c r="M864" t="inlineStr"/>
+      <c r="J864" t="n">
+        <v>0.4959967553826868</v>
+      </c>
+      <c r="K864" t="n">
+        <v>0.01059582026591913</v>
+      </c>
+      <c r="L864" t="n">
+        <v>-0.01514285199917103</v>
+      </c>
+      <c r="M864" t="n">
+        <v>1.663557790814084</v>
+      </c>
     </row>
     <row r="865">
       <c r="A865" t="inlineStr">
@@ -37363,10 +37395,18 @@
       <c r="I865" t="n">
         <v>4.878534593564482</v>
       </c>
-      <c r="J865" t="inlineStr"/>
-      <c r="K865" t="inlineStr"/>
-      <c r="L865" t="inlineStr"/>
-      <c r="M865" t="inlineStr"/>
+      <c r="J865" t="n">
+        <v>0.4994216603121239</v>
+      </c>
+      <c r="K865" t="n">
+        <v>0.009152511499156205</v>
+      </c>
+      <c r="L865" t="n">
+        <v>-0.1213644036507729</v>
+      </c>
+      <c r="M865" t="n">
+        <v>1.921334939992117</v>
+      </c>
     </row>
     <row r="866">
       <c r="A866" t="inlineStr">
@@ -37443,10 +37483,18 @@
       <c r="I867" t="n">
         <v>6.163366665062721</v>
       </c>
-      <c r="J867" t="inlineStr"/>
-      <c r="K867" t="inlineStr"/>
-      <c r="L867" t="inlineStr"/>
-      <c r="M867" t="inlineStr"/>
+      <c r="J867" t="n">
+        <v>0.5169561186157083</v>
+      </c>
+      <c r="K867" t="n">
+        <v>0.01016064815776268</v>
+      </c>
+      <c r="L867" t="n">
+        <v>-0.2810304976759443</v>
+      </c>
+      <c r="M867" t="n">
+        <v>1.845989007204349</v>
+      </c>
     </row>
     <row r="868">
       <c r="A868" t="inlineStr">
@@ -38083,10 +38131,18 @@
       <c r="I883" t="n">
         <v>4.846217837762755</v>
       </c>
-      <c r="J883" t="inlineStr"/>
-      <c r="K883" t="inlineStr"/>
-      <c r="L883" t="inlineStr"/>
-      <c r="M883" t="inlineStr"/>
+      <c r="J883" t="n">
+        <v>0.1741306222569814</v>
+      </c>
+      <c r="K883" t="n">
+        <v>0.007661405384502213</v>
+      </c>
+      <c r="L883" t="n">
+        <v>-0.1494289167025337</v>
+      </c>
+      <c r="M883" t="n">
+        <v>1.834056543320003</v>
+      </c>
     </row>
     <row r="884">
       <c r="A884" t="inlineStr">
@@ -38122,10 +38178,18 @@
       <c r="I884" t="n">
         <v>4.9482245951439</v>
       </c>
-      <c r="J884" t="inlineStr"/>
-      <c r="K884" t="inlineStr"/>
-      <c r="L884" t="inlineStr"/>
-      <c r="M884" t="inlineStr"/>
+      <c r="J884" t="n">
+        <v>0.1732893829452975</v>
+      </c>
+      <c r="K884" t="n">
+        <v>0.006388042904982789</v>
+      </c>
+      <c r="L884" t="n">
+        <v>-0.1320200159195386</v>
+      </c>
+      <c r="M884" t="n">
+        <v>2.192210077531122</v>
+      </c>
     </row>
     <row r="885">
       <c r="A885" t="inlineStr">
@@ -38161,10 +38225,18 @@
       <c r="I885" t="n">
         <v>8.359587161463592</v>
       </c>
-      <c r="J885" t="inlineStr"/>
-      <c r="K885" t="inlineStr"/>
-      <c r="L885" t="inlineStr"/>
-      <c r="M885" t="inlineStr"/>
+      <c r="J885" t="n">
+        <v>0.1897922458443881</v>
+      </c>
+      <c r="K885" t="n">
+        <v>0.00710953225032518</v>
+      </c>
+      <c r="L885" t="n">
+        <v>-0.3236641155507869</v>
+      </c>
+      <c r="M885" t="n">
+        <v>2.042420822161466</v>
+      </c>
     </row>
     <row r="886">
       <c r="A886" t="inlineStr">
@@ -38241,10 +38313,18 @@
       <c r="I887" t="n">
         <v>9.44350494178971</v>
       </c>
-      <c r="J887" t="inlineStr"/>
-      <c r="K887" t="inlineStr"/>
-      <c r="L887" t="inlineStr"/>
-      <c r="M887" t="inlineStr"/>
+      <c r="J887" t="n">
+        <v>0.2410106334485396</v>
+      </c>
+      <c r="K887" t="n">
+        <v>0.02458410332041821</v>
+      </c>
+      <c r="L887" t="n">
+        <v>1.171992255373215</v>
+      </c>
+      <c r="M887" t="n">
+        <v>3.796393522117083</v>
+      </c>
     </row>
     <row r="888">
       <c r="A888" t="inlineStr">
@@ -38834,10 +38914,18 @@
       <c r="I902" t="n">
         <v>4.32887360222632</v>
       </c>
-      <c r="J902" t="inlineStr"/>
-      <c r="K902" t="inlineStr"/>
-      <c r="L902" t="inlineStr"/>
-      <c r="M902" t="inlineStr"/>
+      <c r="J902" t="n">
+        <v>0.1644653861563335</v>
+      </c>
+      <c r="K902" t="n">
+        <v>0.004166984081917661</v>
+      </c>
+      <c r="L902" t="n">
+        <v>-0.009744353085738667</v>
+      </c>
+      <c r="M902" t="n">
+        <v>1.829707928933755</v>
+      </c>
     </row>
     <row r="903">
       <c r="A903" t="inlineStr">
@@ -38873,10 +38961,18 @@
       <c r="I903" t="n">
         <v>6.83385722220373</v>
       </c>
-      <c r="J903" t="inlineStr"/>
-      <c r="K903" t="inlineStr"/>
-      <c r="L903" t="inlineStr"/>
-      <c r="M903" t="inlineStr"/>
+      <c r="J903" t="n">
+        <v>0.1568772835360597</v>
+      </c>
+      <c r="K903" t="n">
+        <v>0.003563904471037351</v>
+      </c>
+      <c r="L903" t="n">
+        <v>0.3221801397222507</v>
+      </c>
+      <c r="M903" t="n">
+        <v>2.100310050176578</v>
+      </c>
     </row>
     <row r="904">
       <c r="A904" t="inlineStr">
@@ -38912,10 +39008,18 @@
       <c r="I904" t="n">
         <v>6.931938019205041</v>
       </c>
-      <c r="J904" t="inlineStr"/>
-      <c r="K904" t="inlineStr"/>
-      <c r="L904" t="inlineStr"/>
-      <c r="M904" t="inlineStr"/>
+      <c r="J904" t="n">
+        <v>0.1717729212645522</v>
+      </c>
+      <c r="K904" t="n">
+        <v>0.004079320509223575</v>
+      </c>
+      <c r="L904" t="n">
+        <v>-0.03643626733293952</v>
+      </c>
+      <c r="M904" t="n">
+        <v>1.679618112128374</v>
+      </c>
     </row>
     <row r="905">
       <c r="A905" t="inlineStr">
@@ -38951,10 +39055,18 @@
       <c r="I905" t="n">
         <v>6.245935127005477</v>
       </c>
-      <c r="J905" t="inlineStr"/>
-      <c r="K905" t="inlineStr"/>
-      <c r="L905" t="inlineStr"/>
-      <c r="M905" t="inlineStr"/>
+      <c r="J905" t="n">
+        <v>0.2268026515618569</v>
+      </c>
+      <c r="K905" t="n">
+        <v>0.02166618773604188</v>
+      </c>
+      <c r="L905" t="n">
+        <v>1.384061321255182</v>
+      </c>
+      <c r="M905" t="n">
+        <v>3.823793060073173</v>
+      </c>
     </row>
     <row r="906">
       <c r="A906" t="inlineStr">
@@ -39153,6 +39265,3032 @@
       <c r="L910" t="inlineStr"/>
       <c r="M910" t="inlineStr"/>
     </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D911" t="n">
+        <v>0.03835616438356165</v>
+      </c>
+      <c r="E911" t="n">
+        <v>117250.6646791917</v>
+      </c>
+      <c r="F911" t="n">
+        <v>0.07714818357581613</v>
+      </c>
+      <c r="G911" t="n">
+        <v>0.1214329407171924</v>
+      </c>
+      <c r="H911" t="n">
+        <v>-1.226353334601541</v>
+      </c>
+      <c r="I911" t="n">
+        <v>12.77716345986741</v>
+      </c>
+      <c r="J911" t="inlineStr"/>
+      <c r="K911" t="inlineStr"/>
+      <c r="L911" t="inlineStr"/>
+      <c r="M911" t="inlineStr"/>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D912" t="n">
+        <v>0.1342465753424658</v>
+      </c>
+      <c r="E912" t="n">
+        <v>118131.0625543694</v>
+      </c>
+      <c r="F912" t="n">
+        <v>0.04115282734244539</v>
+      </c>
+      <c r="G912" t="n">
+        <v>0.1520392390788521</v>
+      </c>
+      <c r="H912" t="n">
+        <v>-1.115499296337649</v>
+      </c>
+      <c r="I912" t="n">
+        <v>10.52864733864939</v>
+      </c>
+      <c r="J912" t="inlineStr"/>
+      <c r="K912" t="inlineStr"/>
+      <c r="L912" t="inlineStr"/>
+      <c r="M912" t="inlineStr"/>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D913" t="n">
+        <v>0.210958904109589</v>
+      </c>
+      <c r="E913" t="n">
+        <v>118864.6027847091</v>
+      </c>
+      <c r="F913" t="n">
+        <v>0.02998690542077836</v>
+      </c>
+      <c r="G913" t="n">
+        <v>0.1705372080604419</v>
+      </c>
+      <c r="H913" t="n">
+        <v>-1.078272026540769</v>
+      </c>
+      <c r="I913" t="n">
+        <v>10.64523010100589</v>
+      </c>
+      <c r="J913" t="inlineStr"/>
+      <c r="K913" t="inlineStr"/>
+      <c r="L913" t="inlineStr"/>
+      <c r="M913" t="inlineStr"/>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D914" t="n">
+        <v>0.2876712328767123</v>
+      </c>
+      <c r="E914" t="n">
+        <v>119530.7918885916</v>
+      </c>
+      <c r="F914" t="n">
+        <v>0.01778517691593047</v>
+      </c>
+      <c r="G914" t="n">
+        <v>0.2037885530668088</v>
+      </c>
+      <c r="H914" t="n">
+        <v>-1.376302409928244</v>
+      </c>
+      <c r="I914" t="n">
+        <v>11.79722082354386</v>
+      </c>
+      <c r="J914" t="inlineStr"/>
+      <c r="K914" t="inlineStr"/>
+      <c r="L914" t="inlineStr"/>
+      <c r="M914" t="inlineStr"/>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D915" t="n">
+        <v>0.3835616438356164</v>
+      </c>
+      <c r="E915" t="n">
+        <v>120404.3596888673</v>
+      </c>
+      <c r="F915" t="n">
+        <v>0.01289090820033025</v>
+      </c>
+      <c r="G915" t="n">
+        <v>0.1938711304487538</v>
+      </c>
+      <c r="H915" t="n">
+        <v>-0.6378818179877589</v>
+      </c>
+      <c r="I915" t="n">
+        <v>6.326109792932535</v>
+      </c>
+      <c r="J915" t="inlineStr"/>
+      <c r="K915" t="inlineStr"/>
+      <c r="L915" t="inlineStr"/>
+      <c r="M915" t="inlineStr"/>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D916" t="n">
+        <v>0.4602739726027397</v>
+      </c>
+      <c r="E916" t="n">
+        <v>121033.780157313</v>
+      </c>
+      <c r="F916" t="n">
+        <v>0.006831362070791325</v>
+      </c>
+      <c r="G916" t="n">
+        <v>0.1999954663889719</v>
+      </c>
+      <c r="H916" t="n">
+        <v>-0.5802440706894725</v>
+      </c>
+      <c r="I916" t="n">
+        <v>5.858325544873711</v>
+      </c>
+      <c r="J916" t="inlineStr"/>
+      <c r="K916" t="inlineStr"/>
+      <c r="L916" t="inlineStr"/>
+      <c r="M916" t="inlineStr"/>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D917" t="n">
+        <v>0.7095890410958904</v>
+      </c>
+      <c r="E917" t="n">
+        <v>121275.4503200592</v>
+      </c>
+      <c r="F917" t="n">
+        <v>-0.009322891678381491</v>
+      </c>
+      <c r="G917" t="n">
+        <v>0.1831629728301987</v>
+      </c>
+      <c r="H917" t="n">
+        <v>-1.213941120755275</v>
+      </c>
+      <c r="I917" t="n">
+        <v>8.985744013401083</v>
+      </c>
+      <c r="J917" t="inlineStr"/>
+      <c r="K917" t="inlineStr"/>
+      <c r="L917" t="inlineStr"/>
+      <c r="M917" t="inlineStr"/>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D918" t="n">
+        <v>0.7863013698630137</v>
+      </c>
+      <c r="E918" t="n">
+        <v>122767.5126752124</v>
+      </c>
+      <c r="F918" t="n">
+        <v>-0.04222667747188644</v>
+      </c>
+      <c r="G918" t="n">
+        <v>0.3172840645435622</v>
+      </c>
+      <c r="H918" t="n">
+        <v>-1.969085119927182</v>
+      </c>
+      <c r="I918" t="n">
+        <v>12.38520844366341</v>
+      </c>
+      <c r="J918" t="inlineStr"/>
+      <c r="K918" t="inlineStr"/>
+      <c r="L918" t="inlineStr"/>
+      <c r="M918" t="inlineStr"/>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D919" t="n">
+        <v>1.035616438356164</v>
+      </c>
+      <c r="E919" t="n">
+        <v>124354.2299555857</v>
+      </c>
+      <c r="F919" t="n">
+        <v>-0.08029192337556597</v>
+      </c>
+      <c r="G919" t="n">
+        <v>0.392754437386377</v>
+      </c>
+      <c r="H919" t="n">
+        <v>-1.852772122091808</v>
+      </c>
+      <c r="I919" t="n">
+        <v>9.926316636906009</v>
+      </c>
+      <c r="J919" t="inlineStr"/>
+      <c r="K919" t="inlineStr"/>
+      <c r="L919" t="inlineStr"/>
+      <c r="M919" t="inlineStr"/>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D920" t="n">
+        <v>1.282191780821918</v>
+      </c>
+      <c r="E920" t="n">
+        <v>126352.3927678542</v>
+      </c>
+      <c r="F920" t="n">
+        <v>-0.1461094578992783</v>
+      </c>
+      <c r="G920" t="n">
+        <v>0.6571274269691558</v>
+      </c>
+      <c r="H920" t="n">
+        <v>-2.532209624730751</v>
+      </c>
+      <c r="I920" t="n">
+        <v>12.31282035746453</v>
+      </c>
+      <c r="J920" t="inlineStr"/>
+      <c r="K920" t="inlineStr"/>
+      <c r="L920" t="inlineStr"/>
+      <c r="M920" t="inlineStr"/>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D921" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E921" t="n">
+        <v>117243.5824423559</v>
+      </c>
+      <c r="F921" t="n">
+        <v>0.1871104740968699</v>
+      </c>
+      <c r="G921" t="n">
+        <v>0.07441708976951739</v>
+      </c>
+      <c r="H921" t="n">
+        <v>-0.3892419742533572</v>
+      </c>
+      <c r="I921" t="n">
+        <v>5.694989720529963</v>
+      </c>
+      <c r="J921" t="n">
+        <v>0.02538915433439373</v>
+      </c>
+      <c r="K921" t="n">
+        <v>0.005394826486436175</v>
+      </c>
+      <c r="L921" t="n">
+        <v>-0.2629081428452572</v>
+      </c>
+      <c r="M921" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D922" t="n">
+        <v>0.0273972602739726</v>
+      </c>
+      <c r="E922" t="n">
+        <v>117288.8373536223</v>
+      </c>
+      <c r="F922" t="n">
+        <v>0.09711957839296059</v>
+      </c>
+      <c r="G922" t="n">
+        <v>0.1155419997448188</v>
+      </c>
+      <c r="H922" t="n">
+        <v>-0.8443424577724018</v>
+      </c>
+      <c r="I922" t="n">
+        <v>9.628057125794983</v>
+      </c>
+      <c r="J922" t="inlineStr"/>
+      <c r="K922" t="inlineStr"/>
+      <c r="L922" t="inlineStr"/>
+      <c r="M922" t="inlineStr"/>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D923" t="n">
+        <v>0.01095890410958904</v>
+      </c>
+      <c r="E923" t="n">
+        <v>117269.2265082631</v>
+      </c>
+      <c r="F923" t="n">
+        <v>0.1626413725246243</v>
+      </c>
+      <c r="G923" t="n">
+        <v>0.08425522926219284</v>
+      </c>
+      <c r="H923" t="n">
+        <v>-0.222155325015116</v>
+      </c>
+      <c r="I923" t="n">
+        <v>4.323408154166935</v>
+      </c>
+      <c r="J923" t="n">
+        <v>0.01431720391315161</v>
+      </c>
+      <c r="K923" t="n">
+        <v>0.004413884123218463</v>
+      </c>
+      <c r="L923" t="n">
+        <v>0.1640915620408306</v>
+      </c>
+      <c r="M923" t="n">
+        <v>1.671946117951479</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D924" t="n">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="E924" t="n">
+        <v>117207.4900648898</v>
+      </c>
+      <c r="F924" t="n">
+        <v>0.1390160235293125</v>
+      </c>
+      <c r="G924" t="n">
+        <v>0.1012491435117097</v>
+      </c>
+      <c r="H924" t="n">
+        <v>-0.693737401876694</v>
+      </c>
+      <c r="I924" t="n">
+        <v>6.661062592193561</v>
+      </c>
+      <c r="J924" t="n">
+        <v>0.03161928103081686</v>
+      </c>
+      <c r="K924" t="n">
+        <v>0.004728554788917312</v>
+      </c>
+      <c r="L924" t="n">
+        <v>-0.2541427140166077</v>
+      </c>
+      <c r="M924" t="n">
+        <v>1.538388068439291</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D925" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E925" t="n">
+        <v>117267.9785506385</v>
+      </c>
+      <c r="F925" t="n">
+        <v>0.1292054428984758</v>
+      </c>
+      <c r="G925" t="n">
+        <v>0.1110550072809432</v>
+      </c>
+      <c r="H925" t="n">
+        <v>-0.4547091680753564</v>
+      </c>
+      <c r="I925" t="n">
+        <v>6.324924510814944</v>
+      </c>
+      <c r="J925" t="n">
+        <v>0.09494231968237128</v>
+      </c>
+      <c r="K925" t="n">
+        <v>0.02398949844442904</v>
+      </c>
+      <c r="L925" t="n">
+        <v>1.146734435186549</v>
+      </c>
+      <c r="M925" t="n">
+        <v>3.178402480160985</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D926" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E926" t="n">
+        <v>117268.3467627528</v>
+      </c>
+      <c r="F926" t="n">
+        <v>0.1185069757863117</v>
+      </c>
+      <c r="G926" t="n">
+        <v>0.1114465726449506</v>
+      </c>
+      <c r="H926" t="n">
+        <v>-0.3436436233073483</v>
+      </c>
+      <c r="I926" t="n">
+        <v>5.293005229764328</v>
+      </c>
+      <c r="J926" t="inlineStr"/>
+      <c r="K926" t="inlineStr"/>
+      <c r="L926" t="inlineStr"/>
+      <c r="M926" t="inlineStr"/>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D927" t="n">
+        <v>0.05753424657534247</v>
+      </c>
+      <c r="E927" t="n">
+        <v>118184.2318838252</v>
+      </c>
+      <c r="F927" t="n">
+        <v>0.08873828779734873</v>
+      </c>
+      <c r="G927" t="n">
+        <v>0.133603444840359</v>
+      </c>
+      <c r="H927" t="n">
+        <v>-0.7656343299127967</v>
+      </c>
+      <c r="I927" t="n">
+        <v>7.777405239588595</v>
+      </c>
+      <c r="J927" t="inlineStr"/>
+      <c r="K927" t="inlineStr"/>
+      <c r="L927" t="inlineStr"/>
+      <c r="M927" t="inlineStr"/>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D928" t="n">
+        <v>0.07671232876712329</v>
+      </c>
+      <c r="E928" t="n">
+        <v>118173.3428349895</v>
+      </c>
+      <c r="F928" t="n">
+        <v>0.0712238324412736</v>
+      </c>
+      <c r="G928" t="n">
+        <v>0.1397275262736631</v>
+      </c>
+      <c r="H928" t="n">
+        <v>-0.6400421741889533</v>
+      </c>
+      <c r="I928" t="n">
+        <v>6.477308024687465</v>
+      </c>
+      <c r="J928" t="inlineStr"/>
+      <c r="K928" t="inlineStr"/>
+      <c r="L928" t="inlineStr"/>
+      <c r="M928" t="inlineStr"/>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D929" t="n">
+        <v>0.0958904109589041</v>
+      </c>
+      <c r="E929" t="n">
+        <v>118280.9648804801</v>
+      </c>
+      <c r="F929" t="n">
+        <v>0.06316614154918503</v>
+      </c>
+      <c r="G929" t="n">
+        <v>0.1337982982085132</v>
+      </c>
+      <c r="H929" t="n">
+        <v>-0.3777182315593056</v>
+      </c>
+      <c r="I929" t="n">
+        <v>5.484758287719742</v>
+      </c>
+      <c r="J929" t="inlineStr"/>
+      <c r="K929" t="inlineStr"/>
+      <c r="L929" t="inlineStr"/>
+      <c r="M929" t="inlineStr"/>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D930" t="n">
+        <v>0.03013698630136986</v>
+      </c>
+      <c r="E930" t="n">
+        <v>115579.5320580891</v>
+      </c>
+      <c r="F930" t="n">
+        <v>0.02595664126462834</v>
+      </c>
+      <c r="G930" t="n">
+        <v>0.1500083007271827</v>
+      </c>
+      <c r="H930" t="n">
+        <v>-1.249313363057696</v>
+      </c>
+      <c r="I930" t="n">
+        <v>13.52297642088387</v>
+      </c>
+      <c r="J930" t="inlineStr"/>
+      <c r="K930" t="inlineStr"/>
+      <c r="L930" t="inlineStr"/>
+      <c r="M930" t="inlineStr"/>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D931" t="n">
+        <v>0.126027397260274</v>
+      </c>
+      <c r="E931" t="n">
+        <v>116437.8607119196</v>
+      </c>
+      <c r="F931" t="n">
+        <v>0.01351260491757434</v>
+      </c>
+      <c r="G931" t="n">
+        <v>0.1545833169281959</v>
+      </c>
+      <c r="H931" t="n">
+        <v>-1.223941177282235</v>
+      </c>
+      <c r="I931" t="n">
+        <v>11.57436934395236</v>
+      </c>
+      <c r="J931" t="inlineStr"/>
+      <c r="K931" t="inlineStr"/>
+      <c r="L931" t="inlineStr"/>
+      <c r="M931" t="inlineStr"/>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D932" t="n">
+        <v>0.2027397260273973</v>
+      </c>
+      <c r="E932" t="n">
+        <v>117141.4544279742</v>
+      </c>
+      <c r="F932" t="n">
+        <v>0.007546176649098554</v>
+      </c>
+      <c r="G932" t="n">
+        <v>0.1722799591919066</v>
+      </c>
+      <c r="H932" t="n">
+        <v>-1.172237665984363</v>
+      </c>
+      <c r="I932" t="n">
+        <v>11.68552066330636</v>
+      </c>
+      <c r="J932" t="inlineStr"/>
+      <c r="K932" t="inlineStr"/>
+      <c r="L932" t="inlineStr"/>
+      <c r="M932" t="inlineStr"/>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D933" t="n">
+        <v>0.2794520547945206</v>
+      </c>
+      <c r="E933" t="n">
+        <v>117883.942212601</v>
+      </c>
+      <c r="F933" t="n">
+        <v>0.0006671652864473709</v>
+      </c>
+      <c r="G933" t="n">
+        <v>0.2005005136092679</v>
+      </c>
+      <c r="H933" t="n">
+        <v>-1.258069093950971</v>
+      </c>
+      <c r="I933" t="n">
+        <v>10.68256342480368</v>
+      </c>
+      <c r="J933" t="inlineStr"/>
+      <c r="K933" t="inlineStr"/>
+      <c r="L933" t="inlineStr"/>
+      <c r="M933" t="inlineStr"/>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D934" t="n">
+        <v>0.3753424657534247</v>
+      </c>
+      <c r="E934" t="n">
+        <v>118602.9292911225</v>
+      </c>
+      <c r="F934" t="n">
+        <v>-0.01461722479219837</v>
+      </c>
+      <c r="G934" t="n">
+        <v>0.2655390905253522</v>
+      </c>
+      <c r="H934" t="n">
+        <v>-2.858712953962472</v>
+      </c>
+      <c r="I934" t="n">
+        <v>25.83924743997575</v>
+      </c>
+      <c r="J934" t="inlineStr"/>
+      <c r="K934" t="inlineStr"/>
+      <c r="L934" t="inlineStr"/>
+      <c r="M934" t="inlineStr"/>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D935" t="n">
+        <v>0.4520547945205479</v>
+      </c>
+      <c r="E935" t="n">
+        <v>119310.6097676981</v>
+      </c>
+      <c r="F935" t="n">
+        <v>-0.007431952126198738</v>
+      </c>
+      <c r="G935" t="n">
+        <v>0.1998136053875798</v>
+      </c>
+      <c r="H935" t="n">
+        <v>-0.6203418047285336</v>
+      </c>
+      <c r="I935" t="n">
+        <v>5.841112321504236</v>
+      </c>
+      <c r="J935" t="inlineStr"/>
+      <c r="K935" t="inlineStr"/>
+      <c r="L935" t="inlineStr"/>
+      <c r="M935" t="inlineStr"/>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D936" t="n">
+        <v>0.7013698630136986</v>
+      </c>
+      <c r="E936" t="n">
+        <v>119600.2272974841</v>
+      </c>
+      <c r="F936" t="n">
+        <v>-0.02018208511547447</v>
+      </c>
+      <c r="G936" t="n">
+        <v>0.1813202265097833</v>
+      </c>
+      <c r="H936" t="n">
+        <v>-1.209625485831285</v>
+      </c>
+      <c r="I936" t="n">
+        <v>9.036102402254345</v>
+      </c>
+      <c r="J936" t="inlineStr"/>
+      <c r="K936" t="inlineStr"/>
+      <c r="L936" t="inlineStr"/>
+      <c r="M936" t="inlineStr"/>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D937" t="n">
+        <v>0.7780821917808219</v>
+      </c>
+      <c r="E937" t="n">
+        <v>121103.1744497202</v>
+      </c>
+      <c r="F937" t="n">
+        <v>-0.05144446095270336</v>
+      </c>
+      <c r="G937" t="n">
+        <v>0.3136802165217599</v>
+      </c>
+      <c r="H937" t="n">
+        <v>-1.975317167213251</v>
+      </c>
+      <c r="I937" t="n">
+        <v>12.47551197118902</v>
+      </c>
+      <c r="J937" t="inlineStr"/>
+      <c r="K937" t="inlineStr"/>
+      <c r="L937" t="inlineStr"/>
+      <c r="M937" t="inlineStr"/>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D938" t="n">
+        <v>1.027397260273973</v>
+      </c>
+      <c r="E938" t="n">
+        <v>122788.4025037009</v>
+      </c>
+      <c r="F938" t="n">
+        <v>-0.08901643174474598</v>
+      </c>
+      <c r="G938" t="n">
+        <v>0.3949850563763727</v>
+      </c>
+      <c r="H938" t="n">
+        <v>-1.844148480071863</v>
+      </c>
+      <c r="I938" t="n">
+        <v>9.782794413607794</v>
+      </c>
+      <c r="J938" t="inlineStr"/>
+      <c r="K938" t="inlineStr"/>
+      <c r="L938" t="inlineStr"/>
+      <c r="M938" t="inlineStr"/>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D939" t="n">
+        <v>1.273972602739726</v>
+      </c>
+      <c r="E939" t="n">
+        <v>124750.303207982</v>
+      </c>
+      <c r="F939" t="n">
+        <v>-0.1545661038692219</v>
+      </c>
+      <c r="G939" t="n">
+        <v>0.6619810155237301</v>
+      </c>
+      <c r="H939" t="n">
+        <v>-2.525063303949898</v>
+      </c>
+      <c r="I939" t="n">
+        <v>12.23608521588394</v>
+      </c>
+      <c r="J939" t="inlineStr"/>
+      <c r="K939" t="inlineStr"/>
+      <c r="L939" t="inlineStr"/>
+      <c r="M939" t="inlineStr"/>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D940" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E940" t="n">
+        <v>115573.5118193813</v>
+      </c>
+      <c r="F940" t="n">
+        <v>0.0372933522742661</v>
+      </c>
+      <c r="G940" t="n">
+        <v>0.1497465764053942</v>
+      </c>
+      <c r="H940" t="n">
+        <v>-0.9666848279534654</v>
+      </c>
+      <c r="I940" t="n">
+        <v>9.158323151786888</v>
+      </c>
+      <c r="J940" t="inlineStr"/>
+      <c r="K940" t="inlineStr"/>
+      <c r="L940" t="inlineStr"/>
+      <c r="M940" t="inlineStr"/>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D941" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E941" t="n">
+        <v>115089.7103414434</v>
+      </c>
+      <c r="F941" t="n">
+        <v>0.04425206250406902</v>
+      </c>
+      <c r="G941" t="n">
+        <v>0.06840124960253047</v>
+      </c>
+      <c r="H941" t="n">
+        <v>-1.029378594740445</v>
+      </c>
+      <c r="I941" t="n">
+        <v>3.015314299905404</v>
+      </c>
+      <c r="J941" t="n">
+        <v>0.05152224139030301</v>
+      </c>
+      <c r="K941" t="inlineStr"/>
+      <c r="L941" t="inlineStr"/>
+      <c r="M941" t="inlineStr"/>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D942" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E942" t="n">
+        <v>115569.7619538604</v>
+      </c>
+      <c r="F942" t="n">
+        <v>0.03374051940936252</v>
+      </c>
+      <c r="G942" t="n">
+        <v>0.1437542567338728</v>
+      </c>
+      <c r="H942" t="n">
+        <v>-0.827904072903654</v>
+      </c>
+      <c r="I942" t="n">
+        <v>8.166986038398656</v>
+      </c>
+      <c r="J942" t="inlineStr"/>
+      <c r="K942" t="inlineStr"/>
+      <c r="L942" t="inlineStr"/>
+      <c r="M942" t="inlineStr"/>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D943" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E943" t="n">
+        <v>115709.9173001613</v>
+      </c>
+      <c r="F943" t="n">
+        <v>0.100698445198168</v>
+      </c>
+      <c r="G943" t="n">
+        <v>0.1201249823975057</v>
+      </c>
+      <c r="H943" t="n">
+        <v>0.4888285800173214</v>
+      </c>
+      <c r="I943" t="n">
+        <v>4.940708217255506</v>
+      </c>
+      <c r="J943" t="n">
+        <v>0.1113853598163298</v>
+      </c>
+      <c r="K943" t="n">
+        <v>0.003583592947688513</v>
+      </c>
+      <c r="L943" t="n">
+        <v>0</v>
+      </c>
+      <c r="M943" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D944" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E944" t="n">
+        <v>115613.021807891</v>
+      </c>
+      <c r="F944" t="n">
+        <v>0.06983442023580318</v>
+      </c>
+      <c r="G944" t="n">
+        <v>0.1491046669228473</v>
+      </c>
+      <c r="H944" t="n">
+        <v>0.03491664728520097</v>
+      </c>
+      <c r="I944" t="n">
+        <v>4.654584489446504</v>
+      </c>
+      <c r="J944" t="n">
+        <v>0.2349163737712275</v>
+      </c>
+      <c r="K944" t="n">
+        <v>0.0329088847825759</v>
+      </c>
+      <c r="L944" t="n">
+        <v>0.4832169786564608</v>
+      </c>
+      <c r="M944" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D945" t="n">
+        <v>0.01095890410958904</v>
+      </c>
+      <c r="E945" t="n">
+        <v>115436.3347730561</v>
+      </c>
+      <c r="F945" t="n">
+        <v>0.0436320881701142</v>
+      </c>
+      <c r="G945" t="n">
+        <v>0.1560553075110627</v>
+      </c>
+      <c r="H945" t="n">
+        <v>-1.295248854566389</v>
+      </c>
+      <c r="I945" t="n">
+        <v>9.003855347563105</v>
+      </c>
+      <c r="J945" t="inlineStr"/>
+      <c r="K945" t="inlineStr"/>
+      <c r="L945" t="inlineStr"/>
+      <c r="M945" t="inlineStr"/>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D946" t="n">
+        <v>0.04931506849315068</v>
+      </c>
+      <c r="E946" t="n">
+        <v>116505.1719115963</v>
+      </c>
+      <c r="F946" t="n">
+        <v>0.05060139388372915</v>
+      </c>
+      <c r="G946" t="n">
+        <v>0.1375751724682175</v>
+      </c>
+      <c r="H946" t="n">
+        <v>-0.832125406976703</v>
+      </c>
+      <c r="I946" t="n">
+        <v>8.958770030864056</v>
+      </c>
+      <c r="J946" t="inlineStr"/>
+      <c r="K946" t="inlineStr"/>
+      <c r="L946" t="inlineStr"/>
+      <c r="M946" t="inlineStr"/>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D947" t="n">
+        <v>0.0684931506849315</v>
+      </c>
+      <c r="E947" t="n">
+        <v>116545.8778038837</v>
+      </c>
+      <c r="F947" t="n">
+        <v>0.0380339814334387</v>
+      </c>
+      <c r="G947" t="n">
+        <v>0.1436367897004675</v>
+      </c>
+      <c r="H947" t="n">
+        <v>-0.4955570443498888</v>
+      </c>
+      <c r="I947" t="n">
+        <v>6.678315202598641</v>
+      </c>
+      <c r="J947" t="inlineStr"/>
+      <c r="K947" t="inlineStr"/>
+      <c r="L947" t="inlineStr"/>
+      <c r="M947" t="inlineStr"/>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D948" t="n">
+        <v>0.08767123287671233</v>
+      </c>
+      <c r="E948" t="n">
+        <v>116705.33864515</v>
+      </c>
+      <c r="F948" t="n">
+        <v>0.03368722597024811</v>
+      </c>
+      <c r="G948" t="n">
+        <v>0.1400491480122466</v>
+      </c>
+      <c r="H948" t="n">
+        <v>-0.4462187529018185</v>
+      </c>
+      <c r="I948" t="n">
+        <v>6.499995497826918</v>
+      </c>
+      <c r="J948" t="inlineStr"/>
+      <c r="K948" t="inlineStr"/>
+      <c r="L948" t="inlineStr"/>
+      <c r="M948" t="inlineStr"/>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D949" t="n">
+        <v>0.0273972602739726</v>
+      </c>
+      <c r="E949" t="n">
+        <v>117086.057201255</v>
+      </c>
+      <c r="F949" t="n">
+        <v>0.08880067104379755</v>
+      </c>
+      <c r="G949" t="n">
+        <v>0.1707131998264829</v>
+      </c>
+      <c r="H949" t="n">
+        <v>-1.520471032894363</v>
+      </c>
+      <c r="I949" t="n">
+        <v>14.23718895045043</v>
+      </c>
+      <c r="J949" t="inlineStr"/>
+      <c r="K949" t="inlineStr"/>
+      <c r="L949" t="inlineStr"/>
+      <c r="M949" t="inlineStr"/>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D950" t="n">
+        <v>0.1232876712328767</v>
+      </c>
+      <c r="E950" t="n">
+        <v>117982.5583404625</v>
+      </c>
+      <c r="F950" t="n">
+        <v>0.04289536237732518</v>
+      </c>
+      <c r="G950" t="n">
+        <v>0.1620110263450616</v>
+      </c>
+      <c r="H950" t="n">
+        <v>-1.281579453546158</v>
+      </c>
+      <c r="I950" t="n">
+        <v>12.49071084338882</v>
+      </c>
+      <c r="J950" t="inlineStr"/>
+      <c r="K950" t="inlineStr"/>
+      <c r="L950" t="inlineStr"/>
+      <c r="M950" t="inlineStr"/>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D951" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E951" t="n">
+        <v>118655.8683768171</v>
+      </c>
+      <c r="F951" t="n">
+        <v>0.03046812851571434</v>
+      </c>
+      <c r="G951" t="n">
+        <v>0.1735750225277822</v>
+      </c>
+      <c r="H951" t="n">
+        <v>-1.145964116596201</v>
+      </c>
+      <c r="I951" t="n">
+        <v>11.53345595335768</v>
+      </c>
+      <c r="J951" t="inlineStr"/>
+      <c r="K951" t="inlineStr"/>
+      <c r="L951" t="inlineStr"/>
+      <c r="M951" t="inlineStr"/>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D952" t="n">
+        <v>0.2767123287671233</v>
+      </c>
+      <c r="E952" t="n">
+        <v>119366.8164790674</v>
+      </c>
+      <c r="F952" t="n">
+        <v>0.01854850833029607</v>
+      </c>
+      <c r="G952" t="n">
+        <v>0.2076751468508892</v>
+      </c>
+      <c r="H952" t="n">
+        <v>-1.436616527623723</v>
+      </c>
+      <c r="I952" t="n">
+        <v>12.29408422097338</v>
+      </c>
+      <c r="J952" t="inlineStr"/>
+      <c r="K952" t="inlineStr"/>
+      <c r="L952" t="inlineStr"/>
+      <c r="M952" t="inlineStr"/>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D953" t="n">
+        <v>0.3726027397260274</v>
+      </c>
+      <c r="E953" t="n">
+        <v>120244.9566991789</v>
+      </c>
+      <c r="F953" t="n">
+        <v>0.01302175108200674</v>
+      </c>
+      <c r="G953" t="n">
+        <v>0.1986263265919851</v>
+      </c>
+      <c r="H953" t="n">
+        <v>-0.6792479293778165</v>
+      </c>
+      <c r="I953" t="n">
+        <v>6.407332570145709</v>
+      </c>
+      <c r="J953" t="inlineStr"/>
+      <c r="K953" t="inlineStr"/>
+      <c r="L953" t="inlineStr"/>
+      <c r="M953" t="inlineStr"/>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D954" t="n">
+        <v>0.4493150684931507</v>
+      </c>
+      <c r="E954" t="n">
+        <v>121350.214946859</v>
+      </c>
+      <c r="F954" t="n">
+        <v>0.01404187092373234</v>
+      </c>
+      <c r="G954" t="n">
+        <v>0.1996549675989268</v>
+      </c>
+      <c r="H954" t="n">
+        <v>-0.7412946069320099</v>
+      </c>
+      <c r="I954" t="n">
+        <v>7.411305541277764</v>
+      </c>
+      <c r="J954" t="inlineStr"/>
+      <c r="K954" t="inlineStr"/>
+      <c r="L954" t="inlineStr"/>
+      <c r="M954" t="inlineStr"/>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D955" t="n">
+        <v>0.6986301369863014</v>
+      </c>
+      <c r="E955" t="n">
+        <v>121103.6797630952</v>
+      </c>
+      <c r="F955" t="n">
+        <v>-0.008661112359266492</v>
+      </c>
+      <c r="G955" t="n">
+        <v>0.1840769256405153</v>
+      </c>
+      <c r="H955" t="n">
+        <v>-1.332504362440177</v>
+      </c>
+      <c r="I955" t="n">
+        <v>10.16641447187808</v>
+      </c>
+      <c r="J955" t="inlineStr"/>
+      <c r="K955" t="inlineStr"/>
+      <c r="L955" t="inlineStr"/>
+      <c r="M955" t="inlineStr"/>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D956" t="n">
+        <v>0.7753424657534247</v>
+      </c>
+      <c r="E956" t="n">
+        <v>122620.7494221981</v>
+      </c>
+      <c r="F956" t="n">
+        <v>-0.03822307707386723</v>
+      </c>
+      <c r="G956" t="n">
+        <v>0.3019352474335903</v>
+      </c>
+      <c r="H956" t="n">
+        <v>-1.790510669213726</v>
+      </c>
+      <c r="I956" t="n">
+        <v>11.2800260984637</v>
+      </c>
+      <c r="J956" t="inlineStr"/>
+      <c r="K956" t="inlineStr"/>
+      <c r="L956" t="inlineStr"/>
+      <c r="M956" t="inlineStr"/>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D957" t="n">
+        <v>1.024657534246575</v>
+      </c>
+      <c r="E957" t="n">
+        <v>124349.526518944</v>
+      </c>
+      <c r="F957" t="n">
+        <v>-0.0773906024655823</v>
+      </c>
+      <c r="G957" t="n">
+        <v>0.3887584203061669</v>
+      </c>
+      <c r="H957" t="n">
+        <v>-1.832495351531562</v>
+      </c>
+      <c r="I957" t="n">
+        <v>9.855681753719942</v>
+      </c>
+      <c r="J957" t="inlineStr"/>
+      <c r="K957" t="inlineStr"/>
+      <c r="L957" t="inlineStr"/>
+      <c r="M957" t="inlineStr"/>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D958" t="n">
+        <v>1.271232876712329</v>
+      </c>
+      <c r="E958" t="n">
+        <v>126337.6607212174</v>
+      </c>
+      <c r="F958" t="n">
+        <v>-0.1431781587678564</v>
+      </c>
+      <c r="G958" t="n">
+        <v>0.6529245424995945</v>
+      </c>
+      <c r="H958" t="n">
+        <v>-2.540790213097438</v>
+      </c>
+      <c r="I958" t="n">
+        <v>12.42550551413606</v>
+      </c>
+      <c r="J958" t="inlineStr"/>
+      <c r="K958" t="inlineStr"/>
+      <c r="L958" t="inlineStr"/>
+      <c r="M958" t="inlineStr"/>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D959" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E959" t="n">
+        <v>117097.4057955129</v>
+      </c>
+      <c r="F959" t="n">
+        <v>0.1219578724584407</v>
+      </c>
+      <c r="G959" t="n">
+        <v>0.1669123235554588</v>
+      </c>
+      <c r="H959" t="n">
+        <v>-1.53796834261918</v>
+      </c>
+      <c r="I959" t="n">
+        <v>16.1356679850286</v>
+      </c>
+      <c r="J959" t="inlineStr"/>
+      <c r="K959" t="inlineStr"/>
+      <c r="L959" t="inlineStr"/>
+      <c r="M959" t="inlineStr"/>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D960" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E960" t="n">
+        <v>117068.3262566525</v>
+      </c>
+      <c r="F960" t="n">
+        <v>0.1095936343872741</v>
+      </c>
+      <c r="G960" t="n">
+        <v>0.1661896225736003</v>
+      </c>
+      <c r="H960" t="n">
+        <v>-1.146502352187473</v>
+      </c>
+      <c r="I960" t="n">
+        <v>9.094615366209824</v>
+      </c>
+      <c r="J960" t="inlineStr"/>
+      <c r="K960" t="inlineStr"/>
+      <c r="L960" t="inlineStr"/>
+      <c r="M960" t="inlineStr"/>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D961" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E961" t="n">
+        <v>117028.62628845</v>
+      </c>
+      <c r="F961" t="n">
+        <v>0.3094163461483572</v>
+      </c>
+      <c r="G961" t="n">
+        <v>0.164350430078904</v>
+      </c>
+      <c r="H961" t="n">
+        <v>-0.3199883698459225</v>
+      </c>
+      <c r="I961" t="n">
+        <v>4.175997001234516</v>
+      </c>
+      <c r="J961" t="n">
+        <v>0.1197262368520523</v>
+      </c>
+      <c r="K961" t="inlineStr"/>
+      <c r="L961" t="inlineStr"/>
+      <c r="M961" t="inlineStr"/>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>2025-09-24</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D962" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E962" t="n">
+        <v>117125.1781293021</v>
+      </c>
+      <c r="F962" t="n">
+        <v>0.1042567812617171</v>
+      </c>
+      <c r="G962" t="n">
+        <v>0.165468805059278</v>
+      </c>
+      <c r="H962" t="n">
+        <v>-0.7441930805704752</v>
+      </c>
+      <c r="I962" t="n">
+        <v>8.775648177366282</v>
+      </c>
+      <c r="J962" t="inlineStr"/>
+      <c r="K962" t="inlineStr"/>
+      <c r="L962" t="inlineStr"/>
+      <c r="M962" t="inlineStr"/>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D963" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E963" t="n">
+        <v>117133.9122110062</v>
+      </c>
+      <c r="F963" t="n">
+        <v>0.2262942761140729</v>
+      </c>
+      <c r="G963" t="n">
+        <v>0.2080062491388271</v>
+      </c>
+      <c r="H963" t="n">
+        <v>-0.08641494223191094</v>
+      </c>
+      <c r="I963" t="n">
+        <v>5.156825556682436</v>
+      </c>
+      <c r="J963" t="n">
+        <v>0.2750911985713857</v>
+      </c>
+      <c r="K963" t="n">
+        <v>0.02413827133004993</v>
+      </c>
+      <c r="L963" t="n">
+        <v>2.891019533645416e-16</v>
+      </c>
+      <c r="M963" t="n">
+        <v>0.9999999999999998</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D964" t="n">
+        <v>0.00821917808219178</v>
+      </c>
+      <c r="E964" t="n">
+        <v>117034.9730364334</v>
+      </c>
+      <c r="F964" t="n">
+        <v>0.1727672600662484</v>
+      </c>
+      <c r="G964" t="n">
+        <v>0.1980391236303057</v>
+      </c>
+      <c r="H964" t="n">
+        <v>-0.8802046992249465</v>
+      </c>
+      <c r="I964" t="n">
+        <v>7.681348196542678</v>
+      </c>
+      <c r="J964" t="inlineStr"/>
+      <c r="K964" t="inlineStr"/>
+      <c r="L964" t="inlineStr"/>
+      <c r="M964" t="inlineStr"/>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D965" t="n">
+        <v>0.04657534246575343</v>
+      </c>
+      <c r="E965" t="n">
+        <v>117989.7805380193</v>
+      </c>
+      <c r="F965" t="n">
+        <v>0.0978823074051402</v>
+      </c>
+      <c r="G965" t="n">
+        <v>0.1501780347855073</v>
+      </c>
+      <c r="H965" t="n">
+        <v>-1.015365030418042</v>
+      </c>
+      <c r="I965" t="n">
+        <v>9.055620922796669</v>
+      </c>
+      <c r="J965" t="inlineStr"/>
+      <c r="K965" t="inlineStr"/>
+      <c r="L965" t="inlineStr"/>
+      <c r="M965" t="inlineStr"/>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D966" t="n">
+        <v>0.06575342465753424</v>
+      </c>
+      <c r="E966" t="n">
+        <v>118058.7152166847</v>
+      </c>
+      <c r="F966" t="n">
+        <v>0.07817208858304883</v>
+      </c>
+      <c r="G966" t="n">
+        <v>0.1525816019829916</v>
+      </c>
+      <c r="H966" t="n">
+        <v>-0.7255992261860844</v>
+      </c>
+      <c r="I966" t="n">
+        <v>7.099423958564801</v>
+      </c>
+      <c r="J966" t="inlineStr"/>
+      <c r="K966" t="inlineStr"/>
+      <c r="L966" t="inlineStr"/>
+      <c r="M966" t="inlineStr"/>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D967" t="n">
+        <v>0.08493150684931507</v>
+      </c>
+      <c r="E967" t="n">
+        <v>117958.6853243402</v>
+      </c>
+      <c r="F967" t="n">
+        <v>0.06028656912247458</v>
+      </c>
+      <c r="G967" t="n">
+        <v>0.1580789930453955</v>
+      </c>
+      <c r="H967" t="n">
+        <v>-0.6712832499919513</v>
+      </c>
+      <c r="I967" t="n">
+        <v>6.157321997772498</v>
+      </c>
+      <c r="J967" t="inlineStr"/>
+      <c r="K967" t="inlineStr"/>
+      <c r="L967" t="inlineStr"/>
+      <c r="M967" t="inlineStr"/>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D968" t="n">
+        <v>0.02465753424657534</v>
+      </c>
+      <c r="E968" t="n">
+        <v>115822.2496956292</v>
+      </c>
+      <c r="F968" t="n">
+        <v>-0.01218833998739266</v>
+      </c>
+      <c r="G968" t="n">
+        <v>0.1469807926543989</v>
+      </c>
+      <c r="H968" t="n">
+        <v>-1.542105880135277</v>
+      </c>
+      <c r="I968" t="n">
+        <v>15.7809911585817</v>
+      </c>
+      <c r="J968" t="inlineStr"/>
+      <c r="K968" t="inlineStr"/>
+      <c r="L968" t="inlineStr"/>
+      <c r="M968" t="inlineStr"/>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D969" t="n">
+        <v>0.1205479452054795</v>
+      </c>
+      <c r="E969" t="n">
+        <v>116682.416852635</v>
+      </c>
+      <c r="F969" t="n">
+        <v>-0.005252702314999623</v>
+      </c>
+      <c r="G969" t="n">
+        <v>0.1582220041713745</v>
+      </c>
+      <c r="H969" t="n">
+        <v>-1.375405429118615</v>
+      </c>
+      <c r="I969" t="n">
+        <v>12.79148720818062</v>
+      </c>
+      <c r="J969" t="inlineStr"/>
+      <c r="K969" t="inlineStr"/>
+      <c r="L969" t="inlineStr"/>
+      <c r="M969" t="inlineStr"/>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="D970" t="n">
+        <v>0.1972602739726027</v>
+      </c>
+      <c r="E970" t="n">
+        <v>117385.9050352908</v>
+      </c>
+      <c r="F970" t="n">
+        <v>-0.006679512344602833</v>
+      </c>
+      <c r="G970" t="n">
+        <v>0.1714250184705691</v>
+      </c>
+      <c r="H970" t="n">
+        <v>-1.146861493487216</v>
+      </c>
+      <c r="I970" t="n">
+        <v>11.45993870067113</v>
+      </c>
+      <c r="J970" t="inlineStr"/>
+      <c r="K970" t="inlineStr"/>
+      <c r="L970" t="inlineStr"/>
+      <c r="M970" t="inlineStr"/>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>2025-12-26</t>
+        </is>
+      </c>
+      <c r="D971" t="n">
+        <v>0.273972602739726</v>
+      </c>
+      <c r="E971" t="n">
+        <v>118068.3338892571</v>
+      </c>
+      <c r="F971" t="n">
+        <v>-0.0144455146371095</v>
+      </c>
+      <c r="G971" t="n">
+        <v>0.212949946108634</v>
+      </c>
+      <c r="H971" t="n">
+        <v>-1.609561521925613</v>
+      </c>
+      <c r="I971" t="n">
+        <v>13.45205439434847</v>
+      </c>
+      <c r="J971" t="inlineStr"/>
+      <c r="K971" t="inlineStr"/>
+      <c r="L971" t="inlineStr"/>
+      <c r="M971" t="inlineStr"/>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>2026-01-30</t>
+        </is>
+      </c>
+      <c r="D972" t="n">
+        <v>0.3698630136986301</v>
+      </c>
+      <c r="E972" t="n">
+        <v>119208.6428809396</v>
+      </c>
+      <c r="F972" t="n">
+        <v>-0.009800645915073219</v>
+      </c>
+      <c r="G972" t="n">
+        <v>0.1942304192324773</v>
+      </c>
+      <c r="H972" t="n">
+        <v>-0.8094656307714714</v>
+      </c>
+      <c r="I972" t="n">
+        <v>7.995995437878839</v>
+      </c>
+      <c r="J972" t="inlineStr"/>
+      <c r="K972" t="inlineStr"/>
+      <c r="L972" t="inlineStr"/>
+      <c r="M972" t="inlineStr"/>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>2026-02-27</t>
+        </is>
+      </c>
+      <c r="D973" t="n">
+        <v>0.4465753424657534</v>
+      </c>
+      <c r="E973" t="n">
+        <v>119967.6414036005</v>
+      </c>
+      <c r="F973" t="n">
+        <v>-0.0127886104892476</v>
+      </c>
+      <c r="G973" t="n">
+        <v>0.2027490287194912</v>
+      </c>
+      <c r="H973" t="n">
+        <v>-0.8023498443544875</v>
+      </c>
+      <c r="I973" t="n">
+        <v>7.659690874918008</v>
+      </c>
+      <c r="J973" t="inlineStr"/>
+      <c r="K973" t="inlineStr"/>
+      <c r="L973" t="inlineStr"/>
+      <c r="M973" t="inlineStr"/>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>2026-05-29</t>
+        </is>
+      </c>
+      <c r="D974" t="n">
+        <v>0.6958904109589041</v>
+      </c>
+      <c r="E974" t="n">
+        <v>119810.4629630309</v>
+      </c>
+      <c r="F974" t="n">
+        <v>-0.02837587171955037</v>
+      </c>
+      <c r="G974" t="n">
+        <v>0.1819741682566775</v>
+      </c>
+      <c r="H974" t="n">
+        <v>-1.243653847842376</v>
+      </c>
+      <c r="I974" t="n">
+        <v>9.112527876378875</v>
+      </c>
+      <c r="J974" t="inlineStr"/>
+      <c r="K974" t="inlineStr"/>
+      <c r="L974" t="inlineStr"/>
+      <c r="M974" t="inlineStr"/>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>2026-06-26</t>
+        </is>
+      </c>
+      <c r="D975" t="n">
+        <v>0.7726027397260274</v>
+      </c>
+      <c r="E975" t="n">
+        <v>121395.5640692288</v>
+      </c>
+      <c r="F975" t="n">
+        <v>-0.05612613744298988</v>
+      </c>
+      <c r="G975" t="n">
+        <v>0.2987257734517797</v>
+      </c>
+      <c r="H975" t="n">
+        <v>-1.727399913939542</v>
+      </c>
+      <c r="I975" t="n">
+        <v>10.90794079386216</v>
+      </c>
+      <c r="J975" t="inlineStr"/>
+      <c r="K975" t="inlineStr"/>
+      <c r="L975" t="inlineStr"/>
+      <c r="M975" t="inlineStr"/>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>2026-09-25</t>
+        </is>
+      </c>
+      <c r="D976" t="n">
+        <v>1.021917808219178</v>
+      </c>
+      <c r="E976" t="n">
+        <v>123133.9786501865</v>
+      </c>
+      <c r="F976" t="n">
+        <v>-0.09178665824168694</v>
+      </c>
+      <c r="G976" t="n">
+        <v>0.3809134109932317</v>
+      </c>
+      <c r="H976" t="n">
+        <v>-1.746056615987775</v>
+      </c>
+      <c r="I976" t="n">
+        <v>9.384733908644623</v>
+      </c>
+      <c r="J976" t="inlineStr"/>
+      <c r="K976" t="inlineStr"/>
+      <c r="L976" t="inlineStr"/>
+      <c r="M976" t="inlineStr"/>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>2026-12-24</t>
+        </is>
+      </c>
+      <c r="D977" t="n">
+        <v>1.268493150684932</v>
+      </c>
+      <c r="E977" t="n">
+        <v>125089.5405282463</v>
+      </c>
+      <c r="F977" t="n">
+        <v>-0.1582200595696781</v>
+      </c>
+      <c r="G977" t="n">
+        <v>0.6547163992936453</v>
+      </c>
+      <c r="H977" t="n">
+        <v>-2.505896085455013</v>
+      </c>
+      <c r="I977" t="n">
+        <v>12.04364618935917</v>
+      </c>
+      <c r="J977" t="inlineStr"/>
+      <c r="K977" t="inlineStr"/>
+      <c r="L977" t="inlineStr"/>
+      <c r="M977" t="inlineStr"/>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D978" t="n">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="E978" t="n">
+        <v>115833.0382856053</v>
+      </c>
+      <c r="F978" t="n">
+        <v>-0.009099281173086568</v>
+      </c>
+      <c r="G978" t="n">
+        <v>0.1386340166692692</v>
+      </c>
+      <c r="H978" t="n">
+        <v>-0.7987104069201661</v>
+      </c>
+      <c r="I978" t="n">
+        <v>8.201905709305551</v>
+      </c>
+      <c r="J978" t="inlineStr"/>
+      <c r="K978" t="inlineStr"/>
+      <c r="L978" t="inlineStr"/>
+      <c r="M978" t="inlineStr"/>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D979" t="n">
+        <v>0.01643835616438356</v>
+      </c>
+      <c r="E979" t="n">
+        <v>115855.8678336693</v>
+      </c>
+      <c r="F979" t="n">
+        <v>-0.007825505452335813</v>
+      </c>
+      <c r="G979" t="n">
+        <v>0.1318162687006521</v>
+      </c>
+      <c r="H979" t="n">
+        <v>-0.671599126148441</v>
+      </c>
+      <c r="I979" t="n">
+        <v>7.289593061123975</v>
+      </c>
+      <c r="J979" t="inlineStr"/>
+      <c r="K979" t="inlineStr"/>
+      <c r="L979" t="inlineStr"/>
+      <c r="M979" t="inlineStr"/>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>2025-09-24</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D980" t="n">
+        <v>0.01917808219178082</v>
+      </c>
+      <c r="E980" t="n">
+        <v>115864.7057000564</v>
+      </c>
+      <c r="F980" t="n">
+        <v>-0.008344079946989319</v>
+      </c>
+      <c r="G980" t="n">
+        <v>0.1364831324681856</v>
+      </c>
+      <c r="H980" t="n">
+        <v>-0.5403347853237466</v>
+      </c>
+      <c r="I980" t="n">
+        <v>7.583627728075383</v>
+      </c>
+      <c r="J980" t="inlineStr"/>
+      <c r="K980" t="inlineStr"/>
+      <c r="L980" t="inlineStr"/>
+      <c r="M980" t="inlineStr"/>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D981" t="n">
+        <v>0.00273972602739726</v>
+      </c>
+      <c r="E981" t="n">
+        <v>115829.8425709918</v>
+      </c>
+      <c r="F981" t="n">
+        <v>-0.008190596681315524</v>
+      </c>
+      <c r="G981" t="n">
+        <v>0.2111290230085454</v>
+      </c>
+      <c r="H981" t="n">
+        <v>-0.3460508982877387</v>
+      </c>
+      <c r="I981" t="n">
+        <v>5.26643481868777</v>
+      </c>
+      <c r="J981" t="n">
+        <v>0.3107299234386695</v>
+      </c>
+      <c r="K981" t="inlineStr"/>
+      <c r="L981" t="inlineStr"/>
+      <c r="M981" t="inlineStr"/>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D982" t="n">
+        <v>0.02191780821917808</v>
+      </c>
+      <c r="E982" t="n">
+        <v>115838.4318254528</v>
+      </c>
+      <c r="F982" t="n">
+        <v>-0.01120044317874287</v>
+      </c>
+      <c r="G982" t="n">
+        <v>0.1452123325491754</v>
+      </c>
+      <c r="H982" t="n">
+        <v>-0.991770472637882</v>
+      </c>
+      <c r="I982" t="n">
+        <v>9.90375723142076</v>
+      </c>
+      <c r="J982" t="inlineStr"/>
+      <c r="K982" t="inlineStr"/>
+      <c r="L982" t="inlineStr"/>
+      <c r="M982" t="inlineStr"/>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="D983" t="n">
+        <v>0.005479452054794521</v>
+      </c>
+      <c r="E983" t="n">
+        <v>115827.8923048814</v>
+      </c>
+      <c r="F983" t="n">
+        <v>-0.008892053326938029</v>
+      </c>
+      <c r="G983" t="n">
+        <v>0.1815670546072843</v>
+      </c>
+      <c r="H983" t="n">
+        <v>-0.5329559910574448</v>
+      </c>
+      <c r="I983" t="n">
+        <v>6.361196805944346</v>
+      </c>
+      <c r="J983" t="inlineStr"/>
+      <c r="K983" t="inlineStr"/>
+      <c r="L983" t="inlineStr"/>
+      <c r="M983" t="inlineStr"/>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D984" t="n">
+        <v>0.04383561643835616</v>
+      </c>
+      <c r="E984" t="n">
+        <v>116740.1958551062</v>
+      </c>
+      <c r="F984" t="n">
+        <v>0.02196234929121436</v>
+      </c>
+      <c r="G984" t="n">
+        <v>0.1413570128555406</v>
+      </c>
+      <c r="H984" t="n">
+        <v>-1.014185444576263</v>
+      </c>
+      <c r="I984" t="n">
+        <v>9.838753231989887</v>
+      </c>
+      <c r="J984" t="inlineStr"/>
+      <c r="K984" t="inlineStr"/>
+      <c r="L984" t="inlineStr"/>
+      <c r="M984" t="inlineStr"/>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D985" t="n">
+        <v>0.06301369863013699</v>
+      </c>
+      <c r="E985" t="n">
+        <v>116701.4219502936</v>
+      </c>
+      <c r="F985" t="n">
+        <v>0.009963683132610153</v>
+      </c>
+      <c r="G985" t="n">
+        <v>0.1515262040665517</v>
+      </c>
+      <c r="H985" t="n">
+        <v>-0.7902845756117525</v>
+      </c>
+      <c r="I985" t="n">
+        <v>7.021674999138468</v>
+      </c>
+      <c r="J985" t="inlineStr"/>
+      <c r="K985" t="inlineStr"/>
+      <c r="L985" t="inlineStr"/>
+      <c r="M985" t="inlineStr"/>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="D986" t="n">
+        <v>0.0821917808219178</v>
+      </c>
+      <c r="E986" t="n">
+        <v>116822.5852917172</v>
+      </c>
+      <c r="F986" t="n">
+        <v>0.008784818962478283</v>
+      </c>
+      <c r="G986" t="n">
+        <v>0.1405969324560297</v>
+      </c>
+      <c r="H986" t="n">
+        <v>-0.4843056150985673</v>
+      </c>
+      <c r="I986" t="n">
+        <v>5.908878308659542</v>
+      </c>
+      <c r="J986" t="inlineStr"/>
+      <c r="K986" t="inlineStr"/>
+      <c r="L986" t="inlineStr"/>
+      <c r="M986" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
processed and analyzed new data
</commit_message>
<xml_diff>
--- a/data_analyzed/moment.xlsx
+++ b/data_analyzed/moment.xlsx
@@ -28590,10 +28590,18 @@
       <c r="I646" t="n">
         <v>6.186288621977192</v>
       </c>
-      <c r="J646" t="inlineStr"/>
-      <c r="K646" t="inlineStr"/>
-      <c r="L646" t="inlineStr"/>
-      <c r="M646" t="inlineStr"/>
+      <c r="J646" t="n">
+        <v>-0.05808045239458798</v>
+      </c>
+      <c r="K646" t="n">
+        <v>0.2399996375480334</v>
+      </c>
+      <c r="L646" t="n">
+        <v>0.237099825084014</v>
+      </c>
+      <c r="M646" t="n">
+        <v>2.554812062321973</v>
+      </c>
     </row>
     <row r="647">
       <c r="A647" t="inlineStr">
@@ -29411,10 +29419,18 @@
       <c r="I665" t="n">
         <v>5.8085666925921</v>
       </c>
-      <c r="J665" t="inlineStr"/>
-      <c r="K665" t="inlineStr"/>
-      <c r="L665" t="inlineStr"/>
-      <c r="M665" t="inlineStr"/>
+      <c r="J665" t="n">
+        <v>-0.3647414710054033</v>
+      </c>
+      <c r="K665" t="n">
+        <v>0.2426200462448084</v>
+      </c>
+      <c r="L665" t="n">
+        <v>0.2814819410217358</v>
+      </c>
+      <c r="M665" t="n">
+        <v>2.570540023702133</v>
+      </c>
     </row>
     <row r="666">
       <c r="A666" t="inlineStr">
@@ -30226,10 +30242,18 @@
       <c r="I684" t="n">
         <v>5.831970636100692</v>
       </c>
-      <c r="J684" t="inlineStr"/>
-      <c r="K684" t="inlineStr"/>
-      <c r="L684" t="inlineStr"/>
-      <c r="M684" t="inlineStr"/>
+      <c r="J684" t="n">
+        <v>0.1812112505621168</v>
+      </c>
+      <c r="K684" t="n">
+        <v>0.2568683653986759</v>
+      </c>
+      <c r="L684" t="n">
+        <v>0.3217421160765271</v>
+      </c>
+      <c r="M684" t="n">
+        <v>2.484956439386924</v>
+      </c>
     </row>
     <row r="685">
       <c r="A685" t="inlineStr">
@@ -31041,10 +31065,18 @@
       <c r="I703" t="n">
         <v>5.465895759083472</v>
       </c>
-      <c r="J703" t="inlineStr"/>
-      <c r="K703" t="inlineStr"/>
-      <c r="L703" t="inlineStr"/>
-      <c r="M703" t="inlineStr"/>
+      <c r="J703" t="n">
+        <v>0.4954102784692063</v>
+      </c>
+      <c r="K703" t="n">
+        <v>0.2573349478400102</v>
+      </c>
+      <c r="L703" t="n">
+        <v>0.276846350178154</v>
+      </c>
+      <c r="M703" t="n">
+        <v>2.488042276717461</v>
+      </c>
     </row>
     <row r="704">
       <c r="A704" t="inlineStr">
@@ -31856,10 +31888,18 @@
       <c r="I722" t="n">
         <v>42.48128837360665</v>
       </c>
-      <c r="J722" t="inlineStr"/>
-      <c r="K722" t="inlineStr"/>
-      <c r="L722" t="inlineStr"/>
-      <c r="M722" t="inlineStr"/>
+      <c r="J722" t="n">
+        <v>0.2049479017366116</v>
+      </c>
+      <c r="K722" t="n">
+        <v>0.263184587419064</v>
+      </c>
+      <c r="L722" t="n">
+        <v>0.2449524956484287</v>
+      </c>
+      <c r="M722" t="n">
+        <v>2.431376744545068</v>
+      </c>
     </row>
     <row r="723">
       <c r="A723" t="inlineStr">
@@ -32624,10 +32664,18 @@
       <c r="I740" t="n">
         <v>41.96604126698929</v>
       </c>
-      <c r="J740" t="inlineStr"/>
-      <c r="K740" t="inlineStr"/>
-      <c r="L740" t="inlineStr"/>
-      <c r="M740" t="inlineStr"/>
+      <c r="J740" t="n">
+        <v>0.03477683984818711</v>
+      </c>
+      <c r="K740" t="n">
+        <v>0.2704625831437422</v>
+      </c>
+      <c r="L740" t="n">
+        <v>0.2362491449239708</v>
+      </c>
+      <c r="M740" t="n">
+        <v>2.364507701123102</v>
+      </c>
     </row>
     <row r="741">
       <c r="A741" t="inlineStr">
@@ -33398,10 +33446,18 @@
       <c r="I758" t="n">
         <v>14.33606068843104</v>
       </c>
-      <c r="J758" t="inlineStr"/>
-      <c r="K758" t="inlineStr"/>
-      <c r="L758" t="inlineStr"/>
-      <c r="M758" t="inlineStr"/>
+      <c r="J758" t="n">
+        <v>0.8021519022689512</v>
+      </c>
+      <c r="K758" t="n">
+        <v>0.260316539010564</v>
+      </c>
+      <c r="L758" t="n">
+        <v>0.2282781566817243</v>
+      </c>
+      <c r="M758" t="n">
+        <v>2.418057025656014</v>
+      </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
@@ -34205,10 +34261,18 @@
       <c r="I777" t="n">
         <v>43.53086165472727</v>
       </c>
-      <c r="J777" t="inlineStr"/>
-      <c r="K777" t="inlineStr"/>
-      <c r="L777" t="inlineStr"/>
-      <c r="M777" t="inlineStr"/>
+      <c r="J777" t="n">
+        <v>0.4238415822648009</v>
+      </c>
+      <c r="K777" t="n">
+        <v>0.2208003802520098</v>
+      </c>
+      <c r="L777" t="n">
+        <v>0.2516512283222432</v>
+      </c>
+      <c r="M777" t="n">
+        <v>2.565679521489</v>
+      </c>
     </row>
     <row r="778">
       <c r="A778" t="inlineStr">
@@ -35012,10 +35076,18 @@
       <c r="I796" t="n">
         <v>42.70468449013802</v>
       </c>
-      <c r="J796" t="inlineStr"/>
-      <c r="K796" t="inlineStr"/>
-      <c r="L796" t="inlineStr"/>
-      <c r="M796" t="inlineStr"/>
+      <c r="J796" t="n">
+        <v>0.349748557851123</v>
+      </c>
+      <c r="K796" t="n">
+        <v>0.2242144557103363</v>
+      </c>
+      <c r="L796" t="n">
+        <v>0.1948034178860719</v>
+      </c>
+      <c r="M796" t="n">
+        <v>2.540403574172122</v>
+      </c>
     </row>
     <row r="797">
       <c r="A797" t="inlineStr">
@@ -35772,10 +35844,18 @@
       <c r="I814" t="n">
         <v>45.83537110914045</v>
       </c>
-      <c r="J814" t="inlineStr"/>
-      <c r="K814" t="inlineStr"/>
-      <c r="L814" t="inlineStr"/>
-      <c r="M814" t="inlineStr"/>
+      <c r="J814" t="n">
+        <v>0.6842399319549618</v>
+      </c>
+      <c r="K814" t="n">
+        <v>0.2163398458498075</v>
+      </c>
+      <c r="L814" t="n">
+        <v>0.1645595860744188</v>
+      </c>
+      <c r="M814" t="n">
+        <v>2.635073052411303</v>
+      </c>
     </row>
     <row r="815">
       <c r="A815" t="inlineStr">
@@ -35811,10 +35891,18 @@
       <c r="I815" t="n">
         <v>5.310094348048753</v>
       </c>
-      <c r="J815" t="inlineStr"/>
-      <c r="K815" t="inlineStr"/>
-      <c r="L815" t="inlineStr"/>
-      <c r="M815" t="inlineStr"/>
+      <c r="J815" t="n">
+        <v>0.9585908516801056</v>
+      </c>
+      <c r="K815" t="n">
+        <v>0.4914461501244363</v>
+      </c>
+      <c r="L815" t="n">
+        <v>0.4577586258096178</v>
+      </c>
+      <c r="M815" t="n">
+        <v>2.225721949624816</v>
+      </c>
     </row>
     <row r="816">
       <c r="A816" t="inlineStr">
@@ -36577,10 +36665,18 @@
       <c r="I833" t="n">
         <v>5.571798574880623</v>
       </c>
-      <c r="J833" t="inlineStr"/>
-      <c r="K833" t="inlineStr"/>
-      <c r="L833" t="inlineStr"/>
-      <c r="M833" t="inlineStr"/>
+      <c r="J833" t="n">
+        <v>0.4643152847966753</v>
+      </c>
+      <c r="K833" t="n">
+        <v>0.2166321763746371</v>
+      </c>
+      <c r="L833" t="n">
+        <v>0.09876596577347316</v>
+      </c>
+      <c r="M833" t="n">
+        <v>2.670391752303761</v>
+      </c>
     </row>
     <row r="834">
       <c r="A834" t="inlineStr">
@@ -36616,10 +36712,18 @@
       <c r="I834" t="n">
         <v>5.371320605976026</v>
       </c>
-      <c r="J834" t="inlineStr"/>
-      <c r="K834" t="inlineStr"/>
-      <c r="L834" t="inlineStr"/>
-      <c r="M834" t="inlineStr"/>
+      <c r="J834" t="n">
+        <v>0.7433026278503435</v>
+      </c>
+      <c r="K834" t="n">
+        <v>0.490140279905831</v>
+      </c>
+      <c r="L834" t="n">
+        <v>0.4156417725326108</v>
+      </c>
+      <c r="M834" t="n">
+        <v>2.21484215664195</v>
+      </c>
     </row>
     <row r="835">
       <c r="A835" t="inlineStr">
@@ -37376,10 +37480,18 @@
       <c r="I852" t="n">
         <v>5.976765079822982</v>
       </c>
-      <c r="J852" t="inlineStr"/>
-      <c r="K852" t="inlineStr"/>
-      <c r="L852" t="inlineStr"/>
-      <c r="M852" t="inlineStr"/>
+      <c r="J852" t="n">
+        <v>0.3532612570755742</v>
+      </c>
+      <c r="K852" t="n">
+        <v>0.2141232790717038</v>
+      </c>
+      <c r="L852" t="n">
+        <v>-0.1106676956798791</v>
+      </c>
+      <c r="M852" t="n">
+        <v>2.89103650729813</v>
+      </c>
     </row>
     <row r="853">
       <c r="A853" t="inlineStr">
@@ -37415,10 +37527,18 @@
       <c r="I853" t="n">
         <v>5.362469780063074</v>
       </c>
-      <c r="J853" t="inlineStr"/>
-      <c r="K853" t="inlineStr"/>
-      <c r="L853" t="inlineStr"/>
-      <c r="M853" t="inlineStr"/>
+      <c r="J853" t="n">
+        <v>0.6466138601298965</v>
+      </c>
+      <c r="K853" t="n">
+        <v>0.4806400749445675</v>
+      </c>
+      <c r="L853" t="n">
+        <v>0.2873446956070686</v>
+      </c>
+      <c r="M853" t="n">
+        <v>2.21951688451959</v>
+      </c>
     </row>
     <row r="854">
       <c r="A854" t="inlineStr">
@@ -38175,10 +38295,18 @@
       <c r="I871" t="n">
         <v>6.152338567716306</v>
       </c>
-      <c r="J871" t="inlineStr"/>
-      <c r="K871" t="inlineStr"/>
-      <c r="L871" t="inlineStr"/>
-      <c r="M871" t="inlineStr"/>
+      <c r="J871" t="n">
+        <v>0.4270390154741289</v>
+      </c>
+      <c r="K871" t="n">
+        <v>0.2157505895368739</v>
+      </c>
+      <c r="L871" t="n">
+        <v>-0.1957046463614244</v>
+      </c>
+      <c r="M871" t="n">
+        <v>2.961627167294484</v>
+      </c>
     </row>
     <row r="872">
       <c r="A872" t="inlineStr">
@@ -38214,10 +38342,18 @@
       <c r="I872" t="n">
         <v>5.49745497074329</v>
       </c>
-      <c r="J872" t="inlineStr"/>
-      <c r="K872" t="inlineStr"/>
-      <c r="L872" t="inlineStr"/>
-      <c r="M872" t="inlineStr"/>
+      <c r="J872" t="n">
+        <v>0.7259974791323728</v>
+      </c>
+      <c r="K872" t="n">
+        <v>0.4796735828753367</v>
+      </c>
+      <c r="L872" t="n">
+        <v>0.2329828474207306</v>
+      </c>
+      <c r="M872" t="n">
+        <v>2.229085699281371</v>
+      </c>
     </row>
     <row r="873">
       <c r="A873" t="inlineStr">
@@ -38974,10 +39110,18 @@
       <c r="I890" t="n">
         <v>6.664206672859858</v>
       </c>
-      <c r="J890" t="inlineStr"/>
-      <c r="K890" t="inlineStr"/>
-      <c r="L890" t="inlineStr"/>
-      <c r="M890" t="inlineStr"/>
+      <c r="J890" t="n">
+        <v>0.07946202988409848</v>
+      </c>
+      <c r="K890" t="n">
+        <v>0.2248679576934663</v>
+      </c>
+      <c r="L890" t="n">
+        <v>-0.2126869254608079</v>
+      </c>
+      <c r="M890" t="n">
+        <v>2.850489859459953</v>
+      </c>
     </row>
     <row r="891">
       <c r="A891" t="inlineStr">
@@ -39013,10 +39157,18 @@
       <c r="I891" t="n">
         <v>5.557220421447647</v>
       </c>
-      <c r="J891" t="inlineStr"/>
-      <c r="K891" t="inlineStr"/>
-      <c r="L891" t="inlineStr"/>
-      <c r="M891" t="inlineStr"/>
+      <c r="J891" t="n">
+        <v>0.3876132281515216</v>
+      </c>
+      <c r="K891" t="n">
+        <v>0.4908161211871584</v>
+      </c>
+      <c r="L891" t="n">
+        <v>0.1841657294355093</v>
+      </c>
+      <c r="M891" t="n">
+        <v>2.182193930958745</v>
+      </c>
     </row>
     <row r="892">
       <c r="A892" t="inlineStr">
@@ -39726,10 +39878,18 @@
       <c r="I908" t="n">
         <v>6.961375465380724</v>
       </c>
-      <c r="J908" t="inlineStr"/>
-      <c r="K908" t="inlineStr"/>
-      <c r="L908" t="inlineStr"/>
-      <c r="M908" t="inlineStr"/>
+      <c r="J908" t="n">
+        <v>0.03858115821364612</v>
+      </c>
+      <c r="K908" t="n">
+        <v>0.23502451085558</v>
+      </c>
+      <c r="L908" t="n">
+        <v>-0.2184581852699795</v>
+      </c>
+      <c r="M908" t="n">
+        <v>2.731007526202857</v>
+      </c>
     </row>
     <row r="909">
       <c r="A909" t="inlineStr">
@@ -39765,10 +39925,18 @@
       <c r="I909" t="n">
         <v>5.479943412847926</v>
       </c>
-      <c r="J909" t="inlineStr"/>
-      <c r="K909" t="inlineStr"/>
-      <c r="L909" t="inlineStr"/>
-      <c r="M909" t="inlineStr"/>
+      <c r="J909" t="n">
+        <v>0.3569533601582136</v>
+      </c>
+      <c r="K909" t="n">
+        <v>0.503493624976924</v>
+      </c>
+      <c r="L909" t="n">
+        <v>0.1370214183447129</v>
+      </c>
+      <c r="M909" t="n">
+        <v>2.132386593961161</v>
+      </c>
     </row>
     <row r="910">
       <c r="A910" t="inlineStr">
@@ -40523,10 +40691,18 @@
       <c r="I927" t="n">
         <v>7.777405239588595</v>
       </c>
-      <c r="J927" t="inlineStr"/>
-      <c r="K927" t="inlineStr"/>
-      <c r="L927" t="inlineStr"/>
-      <c r="M927" t="inlineStr"/>
+      <c r="J927" t="n">
+        <v>-0.1119300937248394</v>
+      </c>
+      <c r="K927" t="n">
+        <v>0.2456466839623254</v>
+      </c>
+      <c r="L927" t="n">
+        <v>-0.1838583654545527</v>
+      </c>
+      <c r="M927" t="n">
+        <v>2.610687095238301</v>
+      </c>
     </row>
     <row r="928">
       <c r="A928" t="inlineStr">
@@ -40562,10 +40738,18 @@
       <c r="I928" t="n">
         <v>6.477308024687465</v>
       </c>
-      <c r="J928" t="inlineStr"/>
-      <c r="K928" t="inlineStr"/>
-      <c r="L928" t="inlineStr"/>
-      <c r="M928" t="inlineStr"/>
+      <c r="J928" t="n">
+        <v>0.2190844768866997</v>
+      </c>
+      <c r="K928" t="n">
+        <v>0.5198204364300951</v>
+      </c>
+      <c r="L928" t="n">
+        <v>0.1047479672860789</v>
+      </c>
+      <c r="M928" t="n">
+        <v>2.06667398167574</v>
+      </c>
     </row>
     <row r="929">
       <c r="A929" t="inlineStr">
@@ -41314,10 +41498,18 @@
       <c r="I946" t="n">
         <v>8.958770030864056</v>
       </c>
-      <c r="J946" t="inlineStr"/>
-      <c r="K946" t="inlineStr"/>
-      <c r="L946" t="inlineStr"/>
-      <c r="M946" t="inlineStr"/>
+      <c r="J946" t="n">
+        <v>-0.06439574632716669</v>
+      </c>
+      <c r="K946" t="n">
+        <v>0.2820221037857273</v>
+      </c>
+      <c r="L946" t="n">
+        <v>-0.05024023413823025</v>
+      </c>
+      <c r="M946" t="n">
+        <v>2.288968724969885</v>
+      </c>
     </row>
     <row r="947">
       <c r="A947" t="inlineStr">
@@ -41353,10 +41545,18 @@
       <c r="I947" t="n">
         <v>6.678315202598641</v>
       </c>
-      <c r="J947" t="inlineStr"/>
-      <c r="K947" t="inlineStr"/>
-      <c r="L947" t="inlineStr"/>
-      <c r="M947" t="inlineStr"/>
+      <c r="J947" t="n">
+        <v>0.3127488043338543</v>
+      </c>
+      <c r="K947" t="n">
+        <v>0.5765091068230044</v>
+      </c>
+      <c r="L947" t="n">
+        <v>0.01146066641156172</v>
+      </c>
+      <c r="M947" t="n">
+        <v>1.873828640831355</v>
+      </c>
     </row>
     <row r="948">
       <c r="A948" t="inlineStr">
@@ -42105,10 +42305,18 @@
       <c r="I965" t="n">
         <v>9.055620922796669</v>
       </c>
-      <c r="J965" t="inlineStr"/>
-      <c r="K965" t="inlineStr"/>
-      <c r="L965" t="inlineStr"/>
-      <c r="M965" t="inlineStr"/>
+      <c r="J965" t="n">
+        <v>-0.1227366928773208</v>
+      </c>
+      <c r="K965" t="n">
+        <v>0.2977747339815092</v>
+      </c>
+      <c r="L965" t="n">
+        <v>-0.0121057452347735</v>
+      </c>
+      <c r="M965" t="n">
+        <v>2.172310786008958</v>
+      </c>
     </row>
     <row r="966">
       <c r="A966" t="inlineStr">
@@ -42144,10 +42352,18 @@
       <c r="I966" t="n">
         <v>7.099423958564801</v>
       </c>
-      <c r="J966" t="inlineStr"/>
-      <c r="K966" t="inlineStr"/>
-      <c r="L966" t="inlineStr"/>
-      <c r="M966" t="inlineStr"/>
+      <c r="J966" t="n">
+        <v>0.2721110030661992</v>
+      </c>
+      <c r="K966" t="n">
+        <v>0.5975685436877082</v>
+      </c>
+      <c r="L966" t="n">
+        <v>-0.02932312144336056</v>
+      </c>
+      <c r="M966" t="n">
+        <v>1.816670092425335</v>
+      </c>
     </row>
     <row r="967">
       <c r="A967" t="inlineStr">
@@ -42896,10 +43112,18 @@
       <c r="I984" t="n">
         <v>9.838753231989887</v>
       </c>
-      <c r="J984" t="inlineStr"/>
-      <c r="K984" t="inlineStr"/>
-      <c r="L984" t="inlineStr"/>
-      <c r="M984" t="inlineStr"/>
+      <c r="J984" t="n">
+        <v>-0.2576168628374579</v>
+      </c>
+      <c r="K984" t="n">
+        <v>0.3124817461483998</v>
+      </c>
+      <c r="L984" t="n">
+        <v>0.06428166151588985</v>
+      </c>
+      <c r="M984" t="n">
+        <v>2.096280837135003</v>
+      </c>
     </row>
     <row r="985">
       <c r="A985" t="inlineStr">
@@ -42935,10 +43159,18 @@
       <c r="I985" t="n">
         <v>7.021674999138468</v>
       </c>
-      <c r="J985" t="inlineStr"/>
-      <c r="K985" t="inlineStr"/>
-      <c r="L985" t="inlineStr"/>
-      <c r="M985" t="inlineStr"/>
+      <c r="J985" t="n">
+        <v>0.1590101908321545</v>
+      </c>
+      <c r="K985" t="n">
+        <v>0.6224962746847555</v>
+      </c>
+      <c r="L985" t="n">
+        <v>-0.05365819701479892</v>
+      </c>
+      <c r="M985" t="n">
+        <v>1.748192084962298</v>
+      </c>
     </row>
     <row r="986">
       <c r="A986" t="inlineStr">

</xml_diff>

<commit_message>
update processed and analysed data
</commit_message>
<xml_diff>
--- a/data_analyzed/moment.xlsx
+++ b/data_analyzed/moment.xlsx
@@ -722,10 +722,18 @@
       <c r="I6" t="n">
         <v>12.22864035222789</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>1.477282346912468</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.6430008601316372</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.2172062532435262</v>
+      </c>
+      <c r="M6" t="n">
+        <v>2.742617893978283</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1559,10 +1567,18 @@
       <c r="I25" t="n">
         <v>12.0913129524412</v>
       </c>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>1.289671547221794</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.5206953613327997</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.07372489015042043</v>
+      </c>
+      <c r="M25" t="n">
+        <v>2.19796163554654</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2396,10 +2412,18 @@
       <c r="I44" t="n">
         <v>12.97648910173117</v>
       </c>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
+      <c r="J44" t="n">
+        <v>0.7525028612459097</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0.4834040075754473</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0.05804491740751398</v>
+      </c>
+      <c r="M44" t="n">
+        <v>2.279527057949995</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3227,10 +3251,18 @@
       <c r="I63" t="n">
         <v>12.5086040286615</v>
       </c>
-      <c r="J63" t="inlineStr"/>
-      <c r="K63" t="inlineStr"/>
-      <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr"/>
+      <c r="J63" t="n">
+        <v>0.6295521131073972</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.4508479156658732</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-0.001005534651262963</v>
+      </c>
+      <c r="M63" t="n">
+        <v>2.434995522272491</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4058,10 +4090,18 @@
       <c r="I82" t="n">
         <v>10.502493632555</v>
       </c>
-      <c r="J82" t="inlineStr"/>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
+      <c r="J82" t="n">
+        <v>-0.516135260677097</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.4525158602337503</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0.01543451336434984</v>
+      </c>
+      <c r="M82" t="n">
+        <v>2.435815503854494</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4895,10 +4935,18 @@
       <c r="I101" t="n">
         <v>13.41794205435837</v>
       </c>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
+      <c r="J101" t="n">
+        <v>-1.076622977925301</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.448376582304099</v>
+      </c>
+      <c r="L101" t="n">
+        <v>0.05765380539135707</v>
+      </c>
+      <c r="M101" t="n">
+        <v>2.483069796822584</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5726,10 +5774,18 @@
       <c r="I120" t="n">
         <v>12.32410070557436</v>
       </c>
-      <c r="J120" t="inlineStr"/>
-      <c r="K120" t="inlineStr"/>
-      <c r="L120" t="inlineStr"/>
-      <c r="M120" t="inlineStr"/>
+      <c r="J120" t="n">
+        <v>-0.4541269873383775</v>
+      </c>
+      <c r="K120" t="n">
+        <v>0.4506361868609465</v>
+      </c>
+      <c r="L120" t="n">
+        <v>0.07358145160110161</v>
+      </c>
+      <c r="M120" t="n">
+        <v>2.480718658867192</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6557,10 +6613,18 @@
       <c r="I139" t="n">
         <v>11.60767055117902</v>
       </c>
-      <c r="J139" t="inlineStr"/>
-      <c r="K139" t="inlineStr"/>
-      <c r="L139" t="inlineStr"/>
-      <c r="M139" t="inlineStr"/>
+      <c r="J139" t="n">
+        <v>-0.6575302404215204</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.4508445361474317</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.09288533878809677</v>
+      </c>
+      <c r="M139" t="n">
+        <v>2.496184122438338</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -7388,10 +7452,18 @@
       <c r="I158" t="n">
         <v>10.96888143120432</v>
       </c>
-      <c r="J158" t="inlineStr"/>
-      <c r="K158" t="inlineStr"/>
-      <c r="L158" t="inlineStr"/>
-      <c r="M158" t="inlineStr"/>
+      <c r="J158" t="n">
+        <v>-0.6647498008515189</v>
+      </c>
+      <c r="K158" t="n">
+        <v>0.450967951930201</v>
+      </c>
+      <c r="L158" t="n">
+        <v>0.1125813004828595</v>
+      </c>
+      <c r="M158" t="n">
+        <v>2.513282465284228</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -8219,10 +8291,18 @@
       <c r="I177" t="n">
         <v>10.73435915106776</v>
       </c>
-      <c r="J177" t="inlineStr"/>
-      <c r="K177" t="inlineStr"/>
-      <c r="L177" t="inlineStr"/>
-      <c r="M177" t="inlineStr"/>
+      <c r="J177" t="n">
+        <v>-0.6141830484198026</v>
+      </c>
+      <c r="K177" t="n">
+        <v>0.451704197853215</v>
+      </c>
+      <c r="L177" t="n">
+        <v>0.1321754508754534</v>
+      </c>
+      <c r="M177" t="n">
+        <v>2.526671512074564</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -9056,10 +9136,18 @@
       <c r="I196" t="n">
         <v>12.45594312940294</v>
       </c>
-      <c r="J196" t="inlineStr"/>
-      <c r="K196" t="inlineStr"/>
-      <c r="L196" t="inlineStr"/>
-      <c r="M196" t="inlineStr"/>
+      <c r="J196" t="n">
+        <v>-0.7382099015725235</v>
+      </c>
+      <c r="K196" t="n">
+        <v>0.4519257258104675</v>
+      </c>
+      <c r="L196" t="n">
+        <v>0.1940638174351965</v>
+      </c>
+      <c r="M196" t="n">
+        <v>2.588047259604172</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9887,10 +9975,18 @@
       <c r="I215" t="n">
         <v>12.18325821204666</v>
       </c>
-      <c r="J215" t="inlineStr"/>
-      <c r="K215" t="inlineStr"/>
-      <c r="L215" t="inlineStr"/>
-      <c r="M215" t="inlineStr"/>
+      <c r="J215" t="n">
+        <v>-0.6762232433871019</v>
+      </c>
+      <c r="K215" t="n">
+        <v>0.451917121526646</v>
+      </c>
+      <c r="L215" t="n">
+        <v>0.2157933155075947</v>
+      </c>
+      <c r="M215" t="n">
+        <v>2.611954445245234</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -10718,10 +10814,18 @@
       <c r="I234" t="n">
         <v>13.7504751161537</v>
       </c>
-      <c r="J234" t="inlineStr"/>
-      <c r="K234" t="inlineStr"/>
-      <c r="L234" t="inlineStr"/>
-      <c r="M234" t="inlineStr"/>
+      <c r="J234" t="n">
+        <v>-0.5934017483515905</v>
+      </c>
+      <c r="K234" t="n">
+        <v>0.4529499003166974</v>
+      </c>
+      <c r="L234" t="n">
+        <v>0.2367433508890373</v>
+      </c>
+      <c r="M234" t="n">
+        <v>2.628059292783453</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -11543,10 +11647,18 @@
       <c r="I253" t="n">
         <v>14.61334348651454</v>
       </c>
-      <c r="J253" t="inlineStr"/>
-      <c r="K253" t="inlineStr"/>
-      <c r="L253" t="inlineStr"/>
-      <c r="M253" t="inlineStr"/>
+      <c r="J253" t="n">
+        <v>-0.6830381338146789</v>
+      </c>
+      <c r="K253" t="n">
+        <v>0.4528597409125978</v>
+      </c>
+      <c r="L253" t="n">
+        <v>0.2594084689748836</v>
+      </c>
+      <c r="M253" t="n">
+        <v>2.655278111889562</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -12286,10 +12398,18 @@
       <c r="I270" t="n">
         <v>14.6061876952162</v>
       </c>
-      <c r="J270" t="inlineStr"/>
-      <c r="K270" t="inlineStr"/>
-      <c r="L270" t="inlineStr"/>
-      <c r="M270" t="inlineStr"/>
+      <c r="J270" t="n">
+        <v>-0.1981799344354955</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0.4570840386122355</v>
+      </c>
+      <c r="L270" t="n">
+        <v>0.267064564299616</v>
+      </c>
+      <c r="M270" t="n">
+        <v>2.636059852754527</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -13076,10 +13196,18 @@
       <c r="I288" t="n">
         <v>14.16771763371706</v>
       </c>
-      <c r="J288" t="inlineStr"/>
-      <c r="K288" t="inlineStr"/>
-      <c r="L288" t="inlineStr"/>
-      <c r="M288" t="inlineStr"/>
+      <c r="J288" t="n">
+        <v>-0.6627369299571171</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0.457686881153907</v>
+      </c>
+      <c r="L288" t="n">
+        <v>0.3379598144967776</v>
+      </c>
+      <c r="M288" t="n">
+        <v>2.720457785699356</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -13899,10 +14027,18 @@
       <c r="I307" t="n">
         <v>13.02946973096475</v>
       </c>
-      <c r="J307" t="inlineStr"/>
-      <c r="K307" t="inlineStr"/>
-      <c r="L307" t="inlineStr"/>
-      <c r="M307" t="inlineStr"/>
+      <c r="J307" t="n">
+        <v>-0.6640704137585214</v>
+      </c>
+      <c r="K307" t="n">
+        <v>0.457913895639154</v>
+      </c>
+      <c r="L307" t="n">
+        <v>0.3625523166945925</v>
+      </c>
+      <c r="M307" t="n">
+        <v>2.7515562354048</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -14722,10 +14858,18 @@
       <c r="I326" t="n">
         <v>14.18296960958322</v>
       </c>
-      <c r="J326" t="inlineStr"/>
-      <c r="K326" t="inlineStr"/>
-      <c r="L326" t="inlineStr"/>
-      <c r="M326" t="inlineStr"/>
+      <c r="J326" t="n">
+        <v>-0.649233777652959</v>
+      </c>
+      <c r="K326" t="n">
+        <v>0.4583536105638675</v>
+      </c>
+      <c r="L326" t="n">
+        <v>0.3873467178024197</v>
+      </c>
+      <c r="M326" t="n">
+        <v>2.782278801375452</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -15545,10 +15689,18 @@
       <c r="I345" t="n">
         <v>13.29899062754492</v>
       </c>
-      <c r="J345" t="inlineStr"/>
-      <c r="K345" t="inlineStr"/>
-      <c r="L345" t="inlineStr"/>
-      <c r="M345" t="inlineStr"/>
+      <c r="J345" t="n">
+        <v>-0.6759486140615097</v>
+      </c>
+      <c r="K345" t="n">
+        <v>0.4584227415980057</v>
+      </c>
+      <c r="L345" t="n">
+        <v>0.4132038225786378</v>
+      </c>
+      <c r="M345" t="n">
+        <v>2.818383311834202</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -16368,10 +16520,18 @@
       <c r="I364" t="n">
         <v>11.61592393302996</v>
       </c>
-      <c r="J364" t="inlineStr"/>
-      <c r="K364" t="inlineStr"/>
-      <c r="L364" t="inlineStr"/>
-      <c r="M364" t="inlineStr"/>
+      <c r="J364" t="n">
+        <v>-0.213011757062836</v>
+      </c>
+      <c r="K364" t="n">
+        <v>0.4629671583968761</v>
+      </c>
+      <c r="L364" t="n">
+        <v>0.4214911133908249</v>
+      </c>
+      <c r="M364" t="n">
+        <v>2.799257955029619</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -17197,10 +17357,18 @@
       <c r="I383" t="n">
         <v>13.05208136015519</v>
       </c>
-      <c r="J383" t="inlineStr"/>
-      <c r="K383" t="inlineStr"/>
-      <c r="L383" t="inlineStr"/>
-      <c r="M383" t="inlineStr"/>
+      <c r="J383" t="n">
+        <v>-0.1931047144327512</v>
+      </c>
+      <c r="K383" t="n">
+        <v>0.4780943459631815</v>
+      </c>
+      <c r="L383" t="n">
+        <v>0.4160877221743743</v>
+      </c>
+      <c r="M383" t="n">
+        <v>2.714819154945082</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -18020,10 +18188,18 @@
       <c r="I402" t="n">
         <v>13.28835826560207</v>
       </c>
-      <c r="J402" t="inlineStr"/>
-      <c r="K402" t="inlineStr"/>
-      <c r="L402" t="inlineStr"/>
-      <c r="M402" t="inlineStr"/>
+      <c r="J402" t="n">
+        <v>0.12315217332237</v>
+      </c>
+      <c r="K402" t="n">
+        <v>0.4834173371618073</v>
+      </c>
+      <c r="L402" t="n">
+        <v>0.4079614427643469</v>
+      </c>
+      <c r="M402" t="n">
+        <v>2.682563357569987</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -18843,10 +19019,18 @@
       <c r="I421" t="n">
         <v>13.19126585584797</v>
       </c>
-      <c r="J421" t="inlineStr"/>
-      <c r="K421" t="inlineStr"/>
-      <c r="L421" t="inlineStr"/>
-      <c r="M421" t="inlineStr"/>
+      <c r="J421" t="n">
+        <v>-0.04229948730612585</v>
+      </c>
+      <c r="K421" t="n">
+        <v>0.4890179029360937</v>
+      </c>
+      <c r="L421" t="n">
+        <v>0.40771897256185</v>
+      </c>
+      <c r="M421" t="n">
+        <v>2.653083192022226</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
@@ -19666,10 +19850,18 @@
       <c r="I440" t="n">
         <v>10.02007597727468</v>
       </c>
-      <c r="J440" t="inlineStr"/>
-      <c r="K440" t="inlineStr"/>
-      <c r="L440" t="inlineStr"/>
-      <c r="M440" t="inlineStr"/>
+      <c r="J440" t="n">
+        <v>-0.4050618212753369</v>
+      </c>
+      <c r="K440" t="n">
+        <v>0.4928632049788898</v>
+      </c>
+      <c r="L440" t="n">
+        <v>0.4256430241151026</v>
+      </c>
+      <c r="M440" t="n">
+        <v>2.652482080263422</v>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
@@ -20489,10 +20681,18 @@
       <c r="I459" t="n">
         <v>9.509317549000551</v>
       </c>
-      <c r="J459" t="inlineStr"/>
-      <c r="K459" t="inlineStr"/>
-      <c r="L459" t="inlineStr"/>
-      <c r="M459" t="inlineStr"/>
+      <c r="J459" t="n">
+        <v>-0.4551375938158524</v>
+      </c>
+      <c r="K459" t="n">
+        <v>0.4962935625645516</v>
+      </c>
+      <c r="L459" t="n">
+        <v>0.4459566511720581</v>
+      </c>
+      <c r="M459" t="n">
+        <v>2.658316893901198</v>
+      </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
@@ -21318,10 +21518,18 @@
       <c r="I478" t="n">
         <v>12.92348149368938</v>
       </c>
-      <c r="J478" t="inlineStr"/>
-      <c r="K478" t="inlineStr"/>
-      <c r="L478" t="inlineStr"/>
-      <c r="M478" t="inlineStr"/>
+      <c r="J478" t="n">
+        <v>-1.026102418389584</v>
+      </c>
+      <c r="K478" t="n">
+        <v>0.4913086182698061</v>
+      </c>
+      <c r="L478" t="n">
+        <v>0.5325361988068151</v>
+      </c>
+      <c r="M478" t="n">
+        <v>2.816322965910428</v>
+      </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
@@ -22141,10 +22349,18 @@
       <c r="I497" t="n">
         <v>10.99633228977906</v>
       </c>
-      <c r="J497" t="inlineStr"/>
-      <c r="K497" t="inlineStr"/>
-      <c r="L497" t="inlineStr"/>
-      <c r="M497" t="inlineStr"/>
+      <c r="J497" t="n">
+        <v>-0.8873889631228897</v>
+      </c>
+      <c r="K497" t="n">
+        <v>0.4877282578269154</v>
+      </c>
+      <c r="L497" t="n">
+        <v>0.5675000282201691</v>
+      </c>
+      <c r="M497" t="n">
+        <v>2.89667423575272</v>
+      </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
@@ -22964,10 +23180,18 @@
       <c r="I516" t="n">
         <v>9.809290619843214</v>
       </c>
-      <c r="J516" t="inlineStr"/>
-      <c r="K516" t="inlineStr"/>
-      <c r="L516" t="inlineStr"/>
-      <c r="M516" t="inlineStr"/>
+      <c r="J516" t="n">
+        <v>-1.304125163509162</v>
+      </c>
+      <c r="K516" t="n">
+        <v>0.4726427527162234</v>
+      </c>
+      <c r="L516" t="n">
+        <v>0.590360291702797</v>
+      </c>
+      <c r="M516" t="n">
+        <v>3.020339017269187</v>
+      </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
@@ -23787,10 +24011,18 @@
       <c r="I535" t="n">
         <v>10.97878240271202</v>
       </c>
-      <c r="J535" t="inlineStr"/>
-      <c r="K535" t="inlineStr"/>
-      <c r="L535" t="inlineStr"/>
-      <c r="M535" t="inlineStr"/>
+      <c r="J535" t="n">
+        <v>-0.8499757026326253</v>
+      </c>
+      <c r="K535" t="n">
+        <v>0.4695572284139592</v>
+      </c>
+      <c r="L535" t="n">
+        <v>0.6273898113437535</v>
+      </c>
+      <c r="M535" t="n">
+        <v>3.108478537897936</v>
+      </c>
     </row>
     <row r="536">
       <c r="A536" t="inlineStr">
@@ -24610,10 +24842,18 @@
       <c r="I554" t="n">
         <v>11.30089800010525</v>
       </c>
-      <c r="J554" t="inlineStr"/>
-      <c r="K554" t="inlineStr"/>
-      <c r="L554" t="inlineStr"/>
-      <c r="M554" t="inlineStr"/>
+      <c r="J554" t="n">
+        <v>-0.7175322941186084</v>
+      </c>
+      <c r="K554" t="n">
+        <v>0.4690546999669646</v>
+      </c>
+      <c r="L554" t="n">
+        <v>0.6624895649182415</v>
+      </c>
+      <c r="M554" t="n">
+        <v>3.175250609064786</v>
+      </c>
     </row>
     <row r="555">
       <c r="A555" t="inlineStr">
@@ -25439,10 +25679,18 @@
       <c r="I573" t="n">
         <v>12.74818063125277</v>
       </c>
-      <c r="J573" t="inlineStr"/>
-      <c r="K573" t="inlineStr"/>
-      <c r="L573" t="inlineStr"/>
-      <c r="M573" t="inlineStr"/>
+      <c r="J573" t="n">
+        <v>-0.3125041300915371</v>
+      </c>
+      <c r="K573" t="n">
+        <v>0.4712093240364904</v>
+      </c>
+      <c r="L573" t="n">
+        <v>0.7536979182829137</v>
+      </c>
+      <c r="M573" t="n">
+        <v>3.332998588019548</v>
+      </c>
     </row>
     <row r="574">
       <c r="A574" t="inlineStr">
@@ -26262,10 +26510,18 @@
       <c r="I592" t="n">
         <v>10.55689381395363</v>
       </c>
-      <c r="J592" t="inlineStr"/>
-      <c r="K592" t="inlineStr"/>
-      <c r="L592" t="inlineStr"/>
-      <c r="M592" t="inlineStr"/>
+      <c r="J592" t="n">
+        <v>-0.1772000188674474</v>
+      </c>
+      <c r="K592" t="n">
+        <v>0.4772399240310436</v>
+      </c>
+      <c r="L592" t="n">
+        <v>0.7597635802022941</v>
+      </c>
+      <c r="M592" t="n">
+        <v>3.304213389742004</v>
+      </c>
     </row>
     <row r="593">
       <c r="A593" t="inlineStr">
@@ -27085,10 +27341,18 @@
       <c r="I611" t="n">
         <v>11.53110329535999</v>
       </c>
-      <c r="J611" t="inlineStr"/>
-      <c r="K611" t="inlineStr"/>
-      <c r="L611" t="inlineStr"/>
-      <c r="M611" t="inlineStr"/>
+      <c r="J611" t="n">
+        <v>0.03765113525854395</v>
+      </c>
+      <c r="K611" t="n">
+        <v>0.4838488370217698</v>
+      </c>
+      <c r="L611" t="n">
+        <v>0.752364869482401</v>
+      </c>
+      <c r="M611" t="n">
+        <v>3.256976923646162</v>
+      </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
@@ -27908,10 +28172,18 @@
       <c r="I630" t="n">
         <v>11.47201725257162</v>
       </c>
-      <c r="J630" t="inlineStr"/>
-      <c r="K630" t="inlineStr"/>
-      <c r="L630" t="inlineStr"/>
-      <c r="M630" t="inlineStr"/>
+      <c r="J630" t="n">
+        <v>-0.02340473408778189</v>
+      </c>
+      <c r="K630" t="n">
+        <v>0.4906560012967206</v>
+      </c>
+      <c r="L630" t="n">
+        <v>0.748530925748327</v>
+      </c>
+      <c r="M630" t="n">
+        <v>3.213228907425157</v>
+      </c>
     </row>
     <row r="631">
       <c r="A631" t="inlineStr">
@@ -28731,10 +29003,18 @@
       <c r="I649" t="n">
         <v>14.41872135162159</v>
       </c>
-      <c r="J649" t="inlineStr"/>
-      <c r="K649" t="inlineStr"/>
-      <c r="L649" t="inlineStr"/>
-      <c r="M649" t="inlineStr"/>
+      <c r="J649" t="n">
+        <v>-0.3261774413778852</v>
+      </c>
+      <c r="K649" t="n">
+        <v>0.4961668977682696</v>
+      </c>
+      <c r="L649" t="n">
+        <v>0.7648173613827539</v>
+      </c>
+      <c r="M649" t="n">
+        <v>3.206213021077398</v>
+      </c>
     </row>
     <row r="650">
       <c r="A650" t="inlineStr">
@@ -29560,10 +29840,18 @@
       <c r="I668" t="n">
         <v>13.94330982624902</v>
       </c>
-      <c r="J668" t="inlineStr"/>
-      <c r="K668" t="inlineStr"/>
-      <c r="L668" t="inlineStr"/>
-      <c r="M668" t="inlineStr"/>
+      <c r="J668" t="n">
+        <v>0.2249675675517139</v>
+      </c>
+      <c r="K668" t="n">
+        <v>0.5161496630566509</v>
+      </c>
+      <c r="L668" t="n">
+        <v>0.765648256423696</v>
+      </c>
+      <c r="M668" t="n">
+        <v>3.108089542562038</v>
+      </c>
     </row>
     <row r="669">
       <c r="A669" t="inlineStr">
@@ -30383,10 +30671,18 @@
       <c r="I687" t="n">
         <v>13.35867396994571</v>
       </c>
-      <c r="J687" t="inlineStr"/>
-      <c r="K687" t="inlineStr"/>
-      <c r="L687" t="inlineStr"/>
-      <c r="M687" t="inlineStr"/>
+      <c r="J687" t="n">
+        <v>0.5344404915603791</v>
+      </c>
+      <c r="K687" t="n">
+        <v>0.5197070283324361</v>
+      </c>
+      <c r="L687" t="n">
+        <v>0.7419874107148443</v>
+      </c>
+      <c r="M687" t="n">
+        <v>3.074251699119845</v>
+      </c>
     </row>
     <row r="688">
       <c r="A688" t="inlineStr">
@@ -31206,10 +31502,18 @@
       <c r="I706" t="n">
         <v>12.59163667277719</v>
       </c>
-      <c r="J706" t="inlineStr"/>
-      <c r="K706" t="inlineStr"/>
-      <c r="L706" t="inlineStr"/>
-      <c r="M706" t="inlineStr"/>
+      <c r="J706" t="n">
+        <v>0.2422552835924969</v>
+      </c>
+      <c r="K706" t="n">
+        <v>0.5268133146755812</v>
+      </c>
+      <c r="L706" t="n">
+        <v>0.7235849514517669</v>
+      </c>
+      <c r="M706" t="n">
+        <v>3.022931541449702</v>
+      </c>
     </row>
     <row r="707">
       <c r="A707" t="inlineStr">
@@ -32023,10 +32327,18 @@
       <c r="I725" t="n">
         <v>12.30725302030576</v>
       </c>
-      <c r="J725" t="inlineStr"/>
-      <c r="K725" t="inlineStr"/>
-      <c r="L725" t="inlineStr"/>
-      <c r="M725" t="inlineStr"/>
+      <c r="J725" t="n">
+        <v>0.07225593691223042</v>
+      </c>
+      <c r="K725" t="n">
+        <v>0.5349644508647857</v>
+      </c>
+      <c r="L725" t="n">
+        <v>0.7136139080027292</v>
+      </c>
+      <c r="M725" t="n">
+        <v>2.972965183273405</v>
+      </c>
     </row>
     <row r="726">
       <c r="A726" t="inlineStr">
@@ -32758,10 +33070,18 @@
       <c r="I742" t="n">
         <v>12.50129700330394</v>
       </c>
-      <c r="J742" t="inlineStr"/>
-      <c r="K742" t="inlineStr"/>
-      <c r="L742" t="inlineStr"/>
-      <c r="M742" t="inlineStr"/>
+      <c r="J742" t="n">
+        <v>0.8303227957310438</v>
+      </c>
+      <c r="K742" t="n">
+        <v>0.5326835134425084</v>
+      </c>
+      <c r="L742" t="n">
+        <v>0.6985624488779159</v>
+      </c>
+      <c r="M742" t="n">
+        <v>2.96954242281555</v>
+      </c>
     </row>
     <row r="743">
       <c r="A743" t="inlineStr">
@@ -33540,10 +33860,18 @@
       <c r="I760" t="n">
         <v>8.492973349451711</v>
       </c>
-      <c r="J760" t="inlineStr"/>
-      <c r="K760" t="inlineStr"/>
-      <c r="L760" t="inlineStr"/>
-      <c r="M760" t="inlineStr"/>
+      <c r="J760" t="n">
+        <v>0.4121774926820508</v>
+      </c>
+      <c r="K760" t="n">
+        <v>0.52947771820412</v>
+      </c>
+      <c r="L760" t="n">
+        <v>0.6311327964926509</v>
+      </c>
+      <c r="M760" t="n">
+        <v>2.929050836434688</v>
+      </c>
     </row>
     <row r="761">
       <c r="A761" t="inlineStr">
@@ -34355,10 +34683,18 @@
       <c r="I779" t="n">
         <v>8.751427601134663</v>
       </c>
-      <c r="J779" t="inlineStr"/>
-      <c r="K779" t="inlineStr"/>
-      <c r="L779" t="inlineStr"/>
-      <c r="M779" t="inlineStr"/>
+      <c r="J779" t="n">
+        <v>0.332436778392457</v>
+      </c>
+      <c r="K779" t="n">
+        <v>0.5367335221490712</v>
+      </c>
+      <c r="L779" t="n">
+        <v>0.6074970978651285</v>
+      </c>
+      <c r="M779" t="n">
+        <v>2.87981202521023</v>
+      </c>
     </row>
     <row r="780">
       <c r="A780" t="inlineStr">
@@ -35170,10 +35506,18 @@
       <c r="I798" t="n">
         <v>10.5472320775076</v>
       </c>
-      <c r="J798" t="inlineStr"/>
-      <c r="K798" t="inlineStr"/>
-      <c r="L798" t="inlineStr"/>
-      <c r="M798" t="inlineStr"/>
+      <c r="J798" t="n">
+        <v>0.655420508356823</v>
+      </c>
+      <c r="K798" t="n">
+        <v>0.5387434162345179</v>
+      </c>
+      <c r="L798" t="n">
+        <v>0.580364417305138</v>
+      </c>
+      <c r="M798" t="n">
+        <v>2.860943871911835</v>
+      </c>
     </row>
     <row r="799">
       <c r="A799" t="inlineStr">
@@ -35985,10 +36329,18 @@
       <c r="I817" t="n">
         <v>10.43423696254672</v>
       </c>
-      <c r="J817" t="inlineStr"/>
-      <c r="K817" t="inlineStr"/>
-      <c r="L817" t="inlineStr"/>
-      <c r="M817" t="inlineStr"/>
+      <c r="J817" t="n">
+        <v>0.4269757926895136</v>
+      </c>
+      <c r="K817" t="n">
+        <v>0.5451654426702852</v>
+      </c>
+      <c r="L817" t="n">
+        <v>0.5531585209632127</v>
+      </c>
+      <c r="M817" t="n">
+        <v>2.81890317602702</v>
+      </c>
     </row>
     <row r="818">
       <c r="A818" t="inlineStr">
@@ -36806,10 +37158,18 @@
       <c r="I836" t="n">
         <v>11.75268514010502</v>
       </c>
-      <c r="J836" t="inlineStr"/>
-      <c r="K836" t="inlineStr"/>
-      <c r="L836" t="inlineStr"/>
-      <c r="M836" t="inlineStr"/>
+      <c r="J836" t="n">
+        <v>0.2853347213291343</v>
+      </c>
+      <c r="K836" t="n">
+        <v>0.5652247219704619</v>
+      </c>
+      <c r="L836" t="n">
+        <v>0.47170424782565</v>
+      </c>
+      <c r="M836" t="n">
+        <v>2.699537866382877</v>
+      </c>
     </row>
     <row r="837">
       <c r="A837" t="inlineStr">
@@ -37621,10 +37981,18 @@
       <c r="I855" t="n">
         <v>8.814173138256782</v>
       </c>
-      <c r="J855" t="inlineStr"/>
-      <c r="K855" t="inlineStr"/>
-      <c r="L855" t="inlineStr"/>
-      <c r="M855" t="inlineStr"/>
+      <c r="J855" t="n">
+        <v>0.3486084367838913</v>
+      </c>
+      <c r="K855" t="n">
+        <v>0.5738014500075432</v>
+      </c>
+      <c r="L855" t="n">
+        <v>0.4457564652853099</v>
+      </c>
+      <c r="M855" t="n">
+        <v>2.653079583015679</v>
+      </c>
     </row>
     <row r="856">
       <c r="A856" t="inlineStr">
@@ -38436,10 +38804,18 @@
       <c r="I874" t="n">
         <v>8.774752746187053</v>
       </c>
-      <c r="J874" t="inlineStr"/>
-      <c r="K874" t="inlineStr"/>
-      <c r="L874" t="inlineStr"/>
-      <c r="M874" t="inlineStr"/>
+      <c r="J874" t="n">
+        <v>-0.002324162143818885</v>
+      </c>
+      <c r="K874" t="n">
+        <v>0.5850523549518037</v>
+      </c>
+      <c r="L874" t="n">
+        <v>0.4416249576227806</v>
+      </c>
+      <c r="M874" t="n">
+        <v>2.602162949010471</v>
+      </c>
     </row>
     <row r="875">
       <c r="A875" t="inlineStr">
@@ -39251,10 +39627,18 @@
       <c r="I893" t="n">
         <v>9.359814936911434</v>
       </c>
-      <c r="J893" t="inlineStr"/>
-      <c r="K893" t="inlineStr"/>
-      <c r="L893" t="inlineStr"/>
-      <c r="M893" t="inlineStr"/>
+      <c r="J893" t="n">
+        <v>-0.04578012498524904</v>
+      </c>
+      <c r="K893" t="n">
+        <v>0.5967123075441018</v>
+      </c>
+      <c r="L893" t="n">
+        <v>0.4408012633709308</v>
+      </c>
+      <c r="M893" t="n">
+        <v>2.553532143010382</v>
+      </c>
     </row>
     <row r="894">
       <c r="A894" t="inlineStr">
@@ -39972,10 +40356,18 @@
       <c r="I910" t="n">
         <v>5.834648396060894</v>
       </c>
-      <c r="J910" t="inlineStr"/>
-      <c r="K910" t="inlineStr"/>
-      <c r="L910" t="inlineStr"/>
-      <c r="M910" t="inlineStr"/>
+      <c r="J910" t="n">
+        <v>0.1801380462221302</v>
+      </c>
+      <c r="K910" t="n">
+        <v>0.5767138759588911</v>
+      </c>
+      <c r="L910" t="n">
+        <v>0.1547621596160096</v>
+      </c>
+      <c r="M910" t="n">
+        <v>2.505388901929666</v>
+      </c>
     </row>
     <row r="911">
       <c r="A911" t="inlineStr">
@@ -40058,10 +40450,18 @@
       <c r="I912" t="n">
         <v>10.52864733864939</v>
       </c>
-      <c r="J912" t="inlineStr"/>
-      <c r="K912" t="inlineStr"/>
-      <c r="L912" t="inlineStr"/>
-      <c r="M912" t="inlineStr"/>
+      <c r="J912" t="n">
+        <v>-0.195105760602844</v>
+      </c>
+      <c r="K912" t="n">
+        <v>0.6081287845824713</v>
+      </c>
+      <c r="L912" t="n">
+        <v>0.451901484868166</v>
+      </c>
+      <c r="M912" t="n">
+        <v>2.517552118679247</v>
+      </c>
     </row>
     <row r="913">
       <c r="A913" t="inlineStr">
@@ -40785,10 +41185,18 @@
       <c r="I929" t="n">
         <v>5.484758287719742</v>
       </c>
-      <c r="J929" t="inlineStr"/>
-      <c r="K929" t="inlineStr"/>
-      <c r="L929" t="inlineStr"/>
-      <c r="M929" t="inlineStr"/>
+      <c r="J929" t="n">
+        <v>0.035706369411352</v>
+      </c>
+      <c r="K929" t="n">
+        <v>0.5931560001382098</v>
+      </c>
+      <c r="L929" t="n">
+        <v>0.1487503366435251</v>
+      </c>
+      <c r="M929" t="n">
+        <v>2.435309308996479</v>
+      </c>
     </row>
     <row r="930">
       <c r="A930" t="inlineStr">
@@ -40871,10 +41279,18 @@
       <c r="I931" t="n">
         <v>11.57436934395236</v>
       </c>
-      <c r="J931" t="inlineStr"/>
-      <c r="K931" t="inlineStr"/>
-      <c r="L931" t="inlineStr"/>
-      <c r="M931" t="inlineStr"/>
+      <c r="J931" t="n">
+        <v>-0.1390649750100463</v>
+      </c>
+      <c r="K931" t="n">
+        <v>0.6440599939930639</v>
+      </c>
+      <c r="L931" t="n">
+        <v>0.4936289468824919</v>
+      </c>
+      <c r="M931" t="n">
+        <v>2.423707911152657</v>
+      </c>
     </row>
     <row r="932">
       <c r="A932" t="inlineStr">
@@ -41592,10 +42008,18 @@
       <c r="I948" t="n">
         <v>6.499995497826918</v>
       </c>
-      <c r="J948" t="inlineStr"/>
-      <c r="K948" t="inlineStr"/>
-      <c r="L948" t="inlineStr"/>
-      <c r="M948" t="inlineStr"/>
+      <c r="J948" t="n">
+        <v>0.1070944970656949</v>
+      </c>
+      <c r="K948" t="n">
+        <v>0.6482476954050463</v>
+      </c>
+      <c r="L948" t="n">
+        <v>0.1388475111057705</v>
+      </c>
+      <c r="M948" t="n">
+        <v>2.229431919465588</v>
+      </c>
     </row>
     <row r="949">
       <c r="A949" t="inlineStr">
@@ -41678,10 +42102,18 @@
       <c r="I950" t="n">
         <v>12.49071084338882</v>
       </c>
-      <c r="J950" t="inlineStr"/>
-      <c r="K950" t="inlineStr"/>
-      <c r="L950" t="inlineStr"/>
-      <c r="M950" t="inlineStr"/>
+      <c r="J950" t="n">
+        <v>-0.194822487875913</v>
+      </c>
+      <c r="K950" t="n">
+        <v>0.657547312178322</v>
+      </c>
+      <c r="L950" t="n">
+        <v>0.5045337537922706</v>
+      </c>
+      <c r="M950" t="n">
+        <v>2.387282082693997</v>
+      </c>
     </row>
     <row r="951">
       <c r="A951" t="inlineStr">
@@ -42399,10 +42831,18 @@
       <c r="I967" t="n">
         <v>6.157321997772498</v>
       </c>
-      <c r="J967" t="inlineStr"/>
-      <c r="K967" t="inlineStr"/>
-      <c r="L967" t="inlineStr"/>
-      <c r="M967" t="inlineStr"/>
+      <c r="J967" t="n">
+        <v>0.05736490908427533</v>
+      </c>
+      <c r="K967" t="n">
+        <v>0.669056075986034</v>
+      </c>
+      <c r="L967" t="n">
+        <v>0.1301275567536507</v>
+      </c>
+      <c r="M967" t="n">
+        <v>2.159255876829187</v>
+      </c>
     </row>
     <row r="968">
       <c r="A968" t="inlineStr">
@@ -42485,10 +42925,18 @@
       <c r="I969" t="n">
         <v>12.79148720818062</v>
       </c>
-      <c r="J969" t="inlineStr"/>
-      <c r="K969" t="inlineStr"/>
-      <c r="L969" t="inlineStr"/>
-      <c r="M969" t="inlineStr"/>
+      <c r="J969" t="n">
+        <v>-0.3216975593808727</v>
+      </c>
+      <c r="K969" t="n">
+        <v>0.6701918066130262</v>
+      </c>
+      <c r="L969" t="n">
+        <v>0.5263752878107336</v>
+      </c>
+      <c r="M969" t="n">
+        <v>2.367711971973246</v>
+      </c>
     </row>
     <row r="970">
       <c r="A970" t="inlineStr">
@@ -43206,10 +43654,18 @@
       <c r="I986" t="n">
         <v>5.908878308659542</v>
       </c>
-      <c r="J986" t="inlineStr"/>
-      <c r="K986" t="inlineStr"/>
-      <c r="L986" t="inlineStr"/>
-      <c r="M986" t="inlineStr"/>
+      <c r="J986" t="n">
+        <v>-0.06444003869336853</v>
+      </c>
+      <c r="K986" t="n">
+        <v>0.6912239929730917</v>
+      </c>
+      <c r="L986" t="n">
+        <v>0.1355354538661993</v>
+      </c>
+      <c r="M986" t="n">
+        <v>2.091729358658431</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>